<commit_message>
Added a dialog that will show up the first time someone opens the app to tell them about the obvious features and point them towards the settings.
Added a new feature that allows the user to display the average roll result next to the actual roll result.
</commit_message>
<xml_diff>
--- a/InstallTracker.xlsx
+++ b/InstallTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A3B24F-D3C3-4FAD-BA0C-CAAEDF7B05EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A896AB-D22A-40A8-9D8E-92034CB2B45E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,6 +425,9 @@
                 <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -511,6 +514,15 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1137,6 +1149,9 @@
                 <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1223,6 +1238,15 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1849,6 +1873,9 @@
                 <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -1935,6 +1962,15 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2560,6 +2596,9 @@
                 <c:pt idx="49">
                   <c:v>49</c:v>
                 </c:pt>
+                <c:pt idx="50">
+                  <c:v>50</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2646,6 +2685,15 @@
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>72</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5593,10 +5641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5647,23 +5695,23 @@
         <v>3</v>
       </c>
       <c r="D2" s="2">
-        <f>1.5638*B2+3</f>
+        <f>1.7932*B2+3</f>
         <v>3</v>
       </c>
       <c r="E2" s="2">
-        <f>0.0837*B2^2-0.0362*B2+3</f>
+        <f>0.0913*B2^2-0.1586*B2+3</f>
         <v>3</v>
       </c>
       <c r="F2" s="2">
-        <f>0.0014*B2^3 + 0.0367*B2^2 + 0.3231*B2 + 3</f>
+        <f>0.0016*B2^3 + 0.0305*B2^2 + 0.3612*B2 + 3</f>
         <v>3</v>
       </c>
       <c r="G2" s="2">
-        <f>3*EXP(0.1234*B2)</f>
+        <f>3*EXP(0.121*B2)</f>
         <v>3</v>
       </c>
       <c r="H2" s="1">
-        <v>43654</v>
+        <v>43655</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5671,27 +5719,27 @@
         <v>43626</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B51" si="0">B2+1</f>
+        <f t="shared" ref="B3:B58" si="0">B2+1</f>
         <v>1</v>
       </c>
       <c r="C3" s="2">
         <v>4</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D51" si="1">1.5638*B3+3</f>
-        <v>4.5638000000000005</v>
+        <f t="shared" ref="D3:D58" si="1">1.7932*B3+3</f>
+        <v>4.7931999999999997</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E51" si="2">0.0837*B3^2-0.0362*B3+3</f>
-        <v>3.0474999999999999</v>
+        <f t="shared" ref="E3:E58" si="2">0.0913*B3^2-0.1586*B3+3</f>
+        <v>2.9327000000000001</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F51" si="3">0.0014*B3^3 + 0.0367*B3^2 + 0.3231*B3 + 3</f>
-        <v>3.3612000000000002</v>
+        <f t="shared" ref="F3:F58" si="3">0.0016*B3^3 + 0.0305*B3^2 + 0.3612*B3 + 3</f>
+        <v>3.3933</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G51" si="4">3*EXP(0.1234*B3)</f>
-        <v>3.3940105955960576</v>
+        <f t="shared" ref="G3:G58" si="4">3*EXP(0.121*B3)</f>
+        <v>3.3858747371020321</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5707,19 +5755,19 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>6.1276000000000002</v>
+        <v>6.5863999999999994</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="2"/>
-        <v>3.2624</v>
+        <v>3.048</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="3"/>
-        <v>3.8041999999999998</v>
+        <v>3.8572000000000002</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="4"/>
-        <v>3.839769307672769</v>
+        <v>3.8213825784485849</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5735,19 +5783,19 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>7.6913999999999998</v>
+        <v>8.3795999999999999</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>3.6446999999999998</v>
+        <v>3.3459000000000003</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="3"/>
-        <v>4.3374000000000006</v>
+        <v>4.4013</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="4"/>
-        <v>4.3440725716286401</v>
+        <v>4.3129075777236281</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5763,19 +5811,19 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>9.2552000000000003</v>
+        <v>10.172799999999999</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="2"/>
-        <v>4.1943999999999999</v>
+        <v>3.8264</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="3"/>
-        <v>4.9691999999999998</v>
+        <v>5.0351999999999997</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="4"/>
-        <v>4.9146094453819389</v>
+        <v>4.8676549369567841</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5791,19 +5839,19 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>10.819000000000001</v>
+        <v>11.965999999999999</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>4.9115000000000002</v>
+        <v>4.4895000000000005</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="3"/>
-        <v>5.7080000000000002</v>
+        <v>5.7684999999999995</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="4"/>
-        <v>5.5600788436142556</v>
+        <v>5.4937566266573192</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5819,19 +5867,19 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>12.3828</v>
+        <v>13.7592</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="2"/>
-        <v>5.7959999999999994</v>
+        <v>5.3352000000000004</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="3"/>
-        <v>6.5622000000000007</v>
+        <v>6.6108000000000002</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="4"/>
-        <v>6.2903221691920868</v>
+        <v>6.2003905913286319</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5847,19 +5895,19 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>13.9466</v>
+        <v>15.552399999999999</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="2"/>
-        <v>6.8479000000000001</v>
+        <v>6.3635000000000002</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="3"/>
-        <v>7.5402000000000005</v>
+        <v>7.5716999999999999</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="4"/>
-        <v>7.1164733639835749</v>
+        <v>6.9979152877815824</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5875,19 +5923,19 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>15.510400000000001</v>
+        <v>17.345599999999997</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>8.0671999999999997</v>
+        <v>7.5744000000000007</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="3"/>
-        <v>8.6504000000000012</v>
+        <v>8.6608000000000001</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="4"/>
-        <v>8.0511286668791229</v>
+        <v>7.8980215284265842</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5903,19 +5951,19 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>17.074200000000001</v>
+        <v>19.1388</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="2"/>
-        <v>9.4539000000000009</v>
+        <v>8.9679000000000002</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="3"/>
-        <v>9.9011999999999993</v>
+        <v>9.8877000000000006</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="4"/>
-        <v>9.1085386672983049</v>
+        <v>8.9139038553958496</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5931,19 +5979,19 @@
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>18.638000000000002</v>
+        <v>20.931999999999999</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="2"/>
-        <v>11.007999999999999</v>
+        <v>10.544</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="3"/>
-        <v>11.301</v>
+        <v>11.262</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="4"/>
-        <v>10.30482558240228</v>
+        <v>10.06045395764707</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -5959,19 +6007,19 @@
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>20.201800000000002</v>
+        <v>22.725199999999997</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="2"/>
-        <v>12.7295</v>
+        <v>12.3027</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="3"/>
-        <v>12.8582</v>
+        <v>12.7933</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="4"/>
-        <v>11.658229070814217</v>
+        <v>11.354478966325123</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -5987,19 +6035,19 @@
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>21.765599999999999</v>
+        <v>24.5184</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>14.618399999999999</v>
+        <v>14.244000000000002</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="3"/>
-        <v>14.581200000000001</v>
+        <v>14.491199999999999</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="4"/>
-        <v>13.189384330743145</v>
+        <v>12.814947828345545</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6015,19 +6063,19 @@
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>23.3294</v>
+        <v>26.311599999999999</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="2"/>
-        <v>16.674700000000001</v>
+        <v>16.367899999999999</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="3"/>
-        <v>16.478400000000001</v>
+        <v>16.365299999999998</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="4"/>
-        <v>14.921636722643619</v>
+        <v>14.463269369758573</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6043,19 +6091,19 @@
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>24.8932</v>
+        <v>28.104799999999997</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>18.898400000000002</v>
+        <v>18.674399999999999</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="3"/>
-        <v>18.558199999999999</v>
+        <v>18.4252</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="4"/>
-        <v>16.88139771342923</v>
+        <v>16.323606124989062</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6071,19 +6119,19 @@
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>26.457000000000001</v>
+        <v>29.898</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>21.2895</v>
+        <v>21.163499999999999</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="3"/>
-        <v>20.829000000000001</v>
+        <v>20.680499999999999</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="4"/>
-        <v>19.098547569283287</v>
+        <v>18.423228532334818</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6099,19 +6147,19 @@
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>28.020800000000001</v>
+        <v>31.691199999999998</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="2"/>
-        <v>23.847999999999999</v>
+        <v>23.8352</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="3"/>
-        <v>23.299199999999999</v>
+        <v>23.140799999999999</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="4"/>
-        <v>21.606890936880941</v>
+        <v>20.792914687829935</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6127,19 +6175,19 @@
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>29.584600000000002</v>
+        <v>33.484399999999994</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="2"/>
-        <v>26.573899999999998</v>
+        <v>26.689500000000002</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="3"/>
-        <v>25.9772</v>
+        <v>25.8157</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="4"/>
-        <v>24.444672259220781</v>
+        <v>23.46740151741372</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6155,19 +6203,19 @@
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>31.148400000000002</v>
+        <v>35.2776</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="2"/>
-        <v>29.467200000000002</v>
+        <v>29.726400000000002</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="3"/>
-        <v>28.871399999999998</v>
+        <v>28.7148</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="4"/>
-        <v>27.655158884556123</v>
+        <v>26.485893981080331</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6183,19 +6231,19 @@
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>32.712200000000003</v>
+        <v>37.070799999999998</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="2"/>
-        <v>32.527900000000002</v>
+        <v>32.945899999999995</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="3"/>
-        <v>31.990200000000002</v>
+        <v>31.847700000000003</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="4"/>
-        <v>31.2873007590253</v>
+        <v>29.892639773367556</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6211,19 +6259,19 @@
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>34.276000000000003</v>
+        <v>38.863999999999997</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="2"/>
-        <v>35.756</v>
+        <v>36.348000000000006</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="3"/>
-        <v>35.341999999999999</v>
+        <v>35.224000000000004</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="4"/>
-        <v>35.396476761244159</v>
+        <v>33.737577944645537</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6239,19 +6287,19 @@
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>35.839800000000004</v>
+        <v>40.657199999999996</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="2"/>
-        <v>39.151499999999999</v>
+        <v>39.932700000000004</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="3"/>
-        <v>38.935200000000002</v>
+        <v>38.853300000000004</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="4"/>
-        <v>40.045339058144094</v>
+        <v>38.077070951262002</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6267,19 +6315,19 @@
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>37.403600000000004</v>
+        <v>42.450399999999995</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
-        <v>42.714399999999998</v>
+        <v>43.7</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="3"/>
-        <v>42.778199999999998</v>
+        <v>42.745199999999997</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="4"/>
-        <v>45.304768355859252</v>
+        <v>42.974730865573214</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6295,19 +6343,19 @@
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>38.967400000000005</v>
+        <v>44.243600000000001</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>46.444699999999997</v>
+        <v>47.649900000000009</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="3"/>
-        <v>46.879399999999997</v>
+        <v>46.909300000000002</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" si="4"/>
-        <v>51.254954610270438</v>
+        <v>48.50235185716776</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6323,19 +6371,19 @@
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
-        <v>40.531199999999998</v>
+        <v>46.036799999999999</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="2"/>
-        <v>50.342399999999998</v>
+        <v>51.78240000000001</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="3"/>
-        <v>51.247200000000007</v>
+        <v>51.355199999999996</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="4"/>
-        <v>57.986619674684277</v>
+        <v>54.740962614406051</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6351,19 +6399,19 @@
       </c>
       <c r="D27" s="2">
         <f t="shared" si="1"/>
-        <v>42.094999999999999</v>
+        <v>47.83</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="2"/>
-        <v>54.407499999999999</v>
+        <v>56.097500000000011</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="3"/>
-        <v>55.89</v>
+        <v>56.092500000000001</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="4"/>
-        <v>65.602400526225765</v>
+        <v>61.782014133588085</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6374,22 +6422,24 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28">
+        <v>63</v>
+      </c>
       <c r="D28" s="2">
         <f t="shared" si="1"/>
-        <v>43.658799999999999</v>
+        <v>49.623199999999997</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="2"/>
-        <v>58.639999999999993</v>
+        <v>60.595200000000006</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="3"/>
-        <v>60.816199999999995</v>
+        <v>61.130799999999994</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="4"/>
-        <v>74.21841416084888</v>
+        <v>69.728720287398858</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6400,22 +6450,24 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29">
+        <v>66</v>
+      </c>
       <c r="D29" s="2">
         <f t="shared" si="1"/>
-        <v>45.2226</v>
+        <v>51.416399999999996</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="2"/>
-        <v>63.039899999999996</v>
+        <v>65.275500000000008</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="3"/>
-        <v>66.034199999999998</v>
+        <v>66.479700000000008</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" si="4"/>
-        <v>83.966028016752531</v>
+        <v>78.697570823852573</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6426,22 +6478,24 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30">
+        <v>72</v>
+      </c>
       <c r="D30" s="2">
         <f t="shared" si="1"/>
-        <v>46.7864</v>
+        <v>53.209599999999995</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="2"/>
-        <v>67.607200000000006</v>
+        <v>70.138400000000004</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="3"/>
-        <v>71.552400000000006</v>
+        <v>72.148800000000008</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="4"/>
-        <v>94.993862919657886</v>
+        <v>88.820038974593459</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6455,19 +6509,19 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2">
         <f t="shared" si="1"/>
-        <v>48.350200000000001</v>
+        <v>55.002800000000001</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="2"/>
-        <v>72.341899999999995</v>
+        <v>75.183900000000008</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="3"/>
-        <v>77.379199999999997</v>
+        <v>78.1477</v>
       </c>
       <c r="G31" s="2">
         <f t="shared" si="4"/>
-        <v>107.4700590886394</v>
+        <v>100.24450870416462</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6481,19 +6535,19 @@
       <c r="C32" s="2"/>
       <c r="D32" s="2">
         <f t="shared" si="1"/>
-        <v>49.914000000000001</v>
+        <v>56.795999999999999</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="2"/>
-        <v>77.244</v>
+        <v>80.412000000000006</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="3"/>
-        <v>83.522999999999996</v>
+        <v>84.486000000000004</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" si="4"/>
-        <v>121.58483975205888</v>
+        <v>113.13844985154523</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -6507,19 +6561,19 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2">
         <f t="shared" si="1"/>
-        <v>51.477800000000002</v>
+        <v>58.589199999999998</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="2"/>
-        <v>82.313499999999991</v>
+        <v>85.822699999999998</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="3"/>
-        <v>89.992199999999997</v>
+        <v>91.173299999999998</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" si="4"/>
-        <v>137.55341146077882</v>
+        <v>127.69087304907738</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -6533,19 +6587,19 @@
       <c r="C34" s="2"/>
       <c r="D34" s="2">
         <f t="shared" si="1"/>
-        <v>53.041600000000003</v>
+        <v>60.382399999999997</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="2"/>
-        <v>87.550399999999996</v>
+        <v>91.416000000000011</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="3"/>
-        <v>96.795200000000008</v>
+        <v>98.219200000000001</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="4"/>
-        <v>155.61924531942256</v>
+        <v>144.11510040512459</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -6559,19 +6613,19 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2">
         <f t="shared" si="1"/>
-        <v>54.605400000000003</v>
+        <v>62.175599999999996</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="2"/>
-        <v>92.954700000000003</v>
+        <v>97.191900000000004</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="3"/>
-        <v>103.9404</v>
+        <v>105.63330000000001</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="4"/>
-        <v>176.05778916426075</v>
+        <v>162.65189256554473</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -6585,19 +6639,19 @@
       <c r="C36" s="2"/>
       <c r="D36" s="2">
         <f t="shared" si="1"/>
-        <v>56.169200000000004</v>
+        <v>63.968799999999995</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="2"/>
-        <v>98.526399999999995</v>
+        <v>103.15040000000002</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" si="3"/>
-        <v>111.4362</v>
+        <v>113.4252</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" si="4"/>
-        <v>199.18066728690596</v>
+        <v>183.57297799317055</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -6611,19 +6665,19 @@
       <c r="C37" s="2"/>
       <c r="D37" s="2">
         <f t="shared" si="1"/>
-        <v>57.733000000000004</v>
+        <v>65.762</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="2"/>
-        <v>104.2655</v>
+        <v>109.2915</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" si="3"/>
-        <v>119.291</v>
+        <v>121.6045</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" si="4"/>
-        <v>225.34043173655073</v>
+        <v>207.18503620055441</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -6637,19 +6691,19 @@
       <c r="C38" s="2"/>
       <c r="D38" s="2">
         <f t="shared" si="1"/>
-        <v>59.296800000000005</v>
+        <v>67.555199999999999</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="2"/>
-        <v>110.172</v>
+        <v>115.61520000000002</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" si="3"/>
-        <v>127.5132</v>
+        <v>130.18080000000003</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" si="4"/>
-        <v>254.93593764334781</v>
+        <v>233.83419332567581</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -6663,19 +6717,19 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2">
         <f t="shared" si="1"/>
-        <v>60.860600000000005</v>
+        <v>69.348399999999998</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="2"/>
-        <v>116.24589999999999</v>
+        <v>122.12150000000001</v>
       </c>
       <c r="F39" s="2">
         <f t="shared" si="3"/>
-        <v>136.1112</v>
+        <v>139.16370000000001</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" si="4"/>
-        <v>288.41842451991261</v>
+        <v>263.91109595067951</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -6689,19 +6743,19 @@
       <c r="C40" s="2"/>
       <c r="D40" s="2">
         <f t="shared" si="1"/>
-        <v>62.424400000000006</v>
+        <v>71.141599999999997</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="2"/>
-        <v>122.48719999999999</v>
+        <v>128.81040000000002</v>
       </c>
       <c r="F40" s="2">
         <f t="shared" si="3"/>
-        <v>145.09340000000003</v>
+        <v>148.56279999999998</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" si="4"/>
-        <v>326.29839626190176</v>
+        <v>297.85663754010523</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -6715,19 +6769,19 @@
       <c r="C41" s="2"/>
       <c r="D41" s="2">
         <f t="shared" si="1"/>
-        <v>63.988200000000006</v>
+        <v>72.934799999999996</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="2"/>
-        <v>128.89589999999998</v>
+        <v>135.68190000000001</v>
       </c>
       <c r="F41" s="2">
         <f t="shared" si="3"/>
-        <v>154.4682</v>
+        <v>158.38770000000002</v>
       </c>
       <c r="G41" s="2">
         <f t="shared" si="4"/>
-        <v>369.15340474629863</v>
+        <v>336.1684214417329</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -6741,19 +6795,19 @@
       <c r="C42" s="2"/>
       <c r="D42" s="2">
         <f t="shared" si="1"/>
-        <v>65.552000000000007</v>
+        <v>74.727999999999994</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="2"/>
-        <v>135.47199999999998</v>
+        <v>142.73600000000002</v>
       </c>
       <c r="F42" s="2">
         <f t="shared" si="3"/>
-        <v>164.244</v>
+        <v>168.648</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" si="4"/>
-        <v>417.63685570309934</v>
+        <v>379.40805519034427</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -6767,19 +6821,19 @@
       <c r="C43" s="2"/>
       <c r="D43" s="2">
         <f t="shared" si="1"/>
-        <v>67.115800000000007</v>
+        <v>76.521199999999993</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="2"/>
-        <v>142.21550000000002</v>
+        <v>149.9727</v>
       </c>
       <c r="F43" s="2">
         <f t="shared" si="3"/>
-        <v>174.42920000000001</v>
+        <v>179.35330000000002</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" si="4"/>
-        <v>472.4879711225804</v>
+        <v>428.20938304066692</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -6793,19 +6847,19 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2">
         <f t="shared" si="1"/>
-        <v>68.679600000000008</v>
+        <v>78.314399999999992</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" si="2"/>
-        <v>149.12639999999999</v>
+        <v>157.392</v>
       </c>
       <c r="F44" s="2">
         <f t="shared" si="3"/>
-        <v>185.03220000000002</v>
+        <v>190.51320000000001</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" si="4"/>
-        <v>534.543060093907</v>
+        <v>483.28777740914688</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -6819,19 +6873,19 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2">
         <f t="shared" si="1"/>
-        <v>70.243400000000008</v>
+        <v>80.107599999999991</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" si="2"/>
-        <v>156.2047</v>
+        <v>164.99390000000002</v>
       </c>
       <c r="F45" s="2">
         <f t="shared" si="3"/>
-        <v>196.06139999999999</v>
+        <v>202.13730000000001</v>
       </c>
       <c r="G45" s="2">
         <f t="shared" si="4"/>
-        <v>604.74826992035378</v>
+        <v>545.45062542660662</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -6845,19 +6899,19 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2">
         <f t="shared" si="1"/>
-        <v>71.807200000000009</v>
+        <v>81.90079999999999</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" si="2"/>
-        <v>163.45039999999997</v>
+        <v>172.7784</v>
       </c>
       <c r="F46" s="2">
         <f t="shared" si="3"/>
-        <v>207.52520000000001</v>
+        <v>214.23519999999999</v>
       </c>
       <c r="G46" s="2">
         <f t="shared" si="4"/>
-        <v>684.17401192602188</v>
+        <v>615.60916432281715</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -6871,19 +6925,19 @@
       <c r="C47" s="2"/>
       <c r="D47" s="2">
         <f t="shared" si="1"/>
-        <v>73.371000000000009</v>
+        <v>83.694000000000003</v>
       </c>
       <c r="E47" s="2">
         <f t="shared" si="2"/>
-        <v>170.86350000000002</v>
+        <v>180.74550000000002</v>
       </c>
       <c r="F47" s="2">
         <f t="shared" si="3"/>
-        <v>219.43200000000002</v>
+        <v>226.81649999999999</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" si="4"/>
-        <v>774.03128190279415</v>
+        <v>694.79183913637371</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -6897,19 +6951,19 @@
       <c r="C48" s="2"/>
       <c r="D48" s="2">
         <f t="shared" si="1"/>
-        <v>74.93480000000001</v>
+        <v>85.487200000000001</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" si="2"/>
-        <v>178.44399999999999</v>
+        <v>188.89520000000002</v>
       </c>
       <c r="F48" s="2">
         <f t="shared" si="3"/>
-        <v>231.79019999999997</v>
+        <v>239.89080000000001</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="4"/>
-        <v>875.69012403362763</v>
+        <v>784.15937855883521</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -6923,19 +6977,19 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2">
         <f t="shared" si="1"/>
-        <v>76.49860000000001</v>
+        <v>87.2804</v>
       </c>
       <c r="E49" s="2">
         <f t="shared" si="2"/>
-        <v>186.19189999999998</v>
+        <v>197.22750000000002</v>
       </c>
       <c r="F49" s="2">
         <f t="shared" si="3"/>
-        <v>244.60820000000001</v>
+        <v>253.46770000000004</v>
       </c>
       <c r="G49" s="2">
         <f t="shared" si="4"/>
-        <v>990.70051980965195</v>
+        <v>885.02180990799593</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -6949,19 +7003,19 @@
       <c r="C50" s="2"/>
       <c r="D50" s="2">
         <f t="shared" si="1"/>
-        <v>78.062399999999997</v>
+        <v>89.073599999999999</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" si="2"/>
-        <v>194.10720000000001</v>
+        <v>205.74240000000003</v>
       </c>
       <c r="F50" s="2">
         <f t="shared" si="3"/>
-        <v>257.89440000000002</v>
+        <v>267.55680000000001</v>
       </c>
       <c r="G50" s="2">
         <f t="shared" si="4"/>
-        <v>1120.8160204321607</v>
+        <v>998.85766265060033</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -6975,19 +7029,194 @@
       <c r="C51" s="2"/>
       <c r="D51" s="2">
         <f t="shared" si="1"/>
-        <v>79.626199999999997</v>
+        <v>90.866799999999998</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" si="2"/>
-        <v>202.18989999999999</v>
+        <v>214.43990000000002</v>
       </c>
       <c r="F51" s="2">
         <f t="shared" si="3"/>
-        <v>271.65719999999999</v>
+        <v>282.16770000000002</v>
       </c>
       <c r="G51" s="2">
         <f t="shared" si="4"/>
-        <v>1268.0204830201872</v>
+        <v>1127.3356419764843</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43675</v>
+      </c>
+      <c r="B52" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D52" s="2">
+        <f t="shared" si="1"/>
+        <v>92.66</v>
+      </c>
+      <c r="E52" s="2">
+        <f t="shared" si="2"/>
+        <v>223.32000000000002</v>
+      </c>
+      <c r="F52" s="2">
+        <f t="shared" si="3"/>
+        <v>297.31</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="4"/>
+        <v>1272.3390901342925</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43676</v>
+      </c>
+      <c r="B53" s="2">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="D53" s="2">
+        <f t="shared" si="1"/>
+        <v>94.453199999999995</v>
+      </c>
+      <c r="E53" s="2">
+        <f t="shared" si="2"/>
+        <v>232.3827</v>
+      </c>
+      <c r="F53" s="2">
+        <f t="shared" si="3"/>
+        <v>312.99329999999998</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="4"/>
+        <v>1435.9935941043614</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>43677</v>
+      </c>
+      <c r="B54" s="2">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="D54" s="2">
+        <f t="shared" si="1"/>
+        <v>96.246399999999994</v>
+      </c>
+      <c r="E54" s="2">
+        <f t="shared" si="2"/>
+        <v>241.62800000000001</v>
+      </c>
+      <c r="F54" s="2">
+        <f t="shared" si="3"/>
+        <v>329.22719999999998</v>
+      </c>
+      <c r="G54" s="2">
+        <f t="shared" si="4"/>
+        <v>1620.6981443061027</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43678</v>
+      </c>
+      <c r="B55" s="2">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="D55" s="2">
+        <f t="shared" si="1"/>
+        <v>98.039599999999993</v>
+      </c>
+      <c r="E55" s="2">
+        <f t="shared" si="2"/>
+        <v>251.05590000000001</v>
+      </c>
+      <c r="F55" s="2">
+        <f t="shared" si="3"/>
+        <v>346.0213</v>
+      </c>
+      <c r="G55" s="2">
+        <f t="shared" si="4"/>
+        <v>1829.1603010913932</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43679</v>
+      </c>
+      <c r="B56" s="2">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="1"/>
+        <v>99.832799999999992</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="2"/>
+        <v>260.66640000000007</v>
+      </c>
+      <c r="F56" s="2">
+        <f t="shared" si="3"/>
+        <v>363.3852</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="4"/>
+        <v>2064.4358845250972</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43680</v>
+      </c>
+      <c r="B57" s="2">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="D57" s="2">
+        <f t="shared" si="1"/>
+        <v>101.62599999999999</v>
+      </c>
+      <c r="E57" s="2">
+        <f t="shared" si="2"/>
+        <v>270.45949999999999</v>
+      </c>
+      <c r="F57" s="2">
+        <f t="shared" si="3"/>
+        <v>381.32849999999996</v>
+      </c>
+      <c r="G57" s="2">
+        <f t="shared" si="4"/>
+        <v>2329.973769260137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>43681</v>
+      </c>
+      <c r="B58" s="2">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="1"/>
+        <v>103.41919999999999</v>
+      </c>
+      <c r="E58" s="2">
+        <f t="shared" si="2"/>
+        <v>280.43520000000001</v>
+      </c>
+      <c r="F58" s="2">
+        <f t="shared" si="3"/>
+        <v>399.86079999999998</v>
+      </c>
+      <c r="G58" s="2">
+        <f t="shared" si="4"/>
+        <v>2629.6664411494335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the install tracker with the new values
</commit_message>
<xml_diff>
--- a/InstallTracker.xlsx
+++ b/InstallTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53A896AB-D22A-40A8-9D8E-92034CB2B45E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3478EB8-EEC2-45F3-9A57-29948944021E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,43 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -235,8 +271,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.18488167104111985"/>
-                  <c:y val="-1.232137649460484E-4"/>
+                  <c:x val="-0.36004811898512684"/>
+                  <c:y val="9.243183143773695E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -523,6 +559,24 @@
                 </c:pt>
                 <c:pt idx="28" formatCode="General">
                   <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1248,6 +1302,24 @@
                 <c:pt idx="28" formatCode="General">
                   <c:v>72</c:v>
                 </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>206</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1972,6 +2044,24 @@
                 <c:pt idx="28" formatCode="General">
                   <c:v>72</c:v>
                 </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>206</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2694,6 +2784,24 @@
                 </c:pt>
                 <c:pt idx="28" formatCode="General">
                   <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>183</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>195</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>211</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5644,7 +5752,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5695,19 +5803,19 @@
         <v>3</v>
       </c>
       <c r="D2" s="2">
-        <f>1.7932*B2+3</f>
+        <f>3.5486*B2+3</f>
         <v>3</v>
       </c>
       <c r="E2" s="2">
-        <f>0.0913*B2^2-0.1586*B2+3</f>
+        <f>0.2709*B2^2-3.4582*B2+3</f>
         <v>3</v>
       </c>
       <c r="F2" s="2">
-        <f>0.0016*B2^3 + 0.0305*B2^2 + 0.3612*B2 + 3</f>
+        <f>0.0143*B2^3 -0.3857*B2^2 + 3.3325*B2 + 3</f>
         <v>3</v>
       </c>
       <c r="G2" s="2">
-        <f>3*EXP(0.121*B2)</f>
+        <f>3*EXP(0.1251*B2)</f>
         <v>3</v>
       </c>
       <c r="H2" s="1">
@@ -5726,20 +5834,20 @@
         <v>4</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D58" si="1">1.7932*B3+3</f>
-        <v>4.7931999999999997</v>
+        <f t="shared" ref="D3:D58" si="1">3.5486*B3+3</f>
+        <v>6.5486000000000004</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E58" si="2">0.0913*B3^2-0.1586*B3+3</f>
-        <v>2.9327000000000001</v>
+        <f t="shared" ref="E3:E58" si="2">0.2709*B3^2-3.4582*B3+3</f>
+        <v>-0.18730000000000002</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" ref="F3:F58" si="3">0.0016*B3^3 + 0.0305*B3^2 + 0.3612*B3 + 3</f>
-        <v>3.3933</v>
+        <f t="shared" ref="F3:F58" si="3">0.0143*B3^3 -0.3857*B3^2 + 3.3325*B3 + 3</f>
+        <v>5.9611000000000001</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G58" si="4">3*EXP(0.121*B3)</f>
-        <v>3.3858747371020321</v>
+        <f t="shared" ref="G3:G58" si="4">3*EXP(0.1251*B3)</f>
+        <v>3.3997853207341926</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5755,19 +5863,19 @@
       </c>
       <c r="D4" s="2">
         <f t="shared" si="1"/>
-        <v>6.5863999999999994</v>
+        <v>10.097200000000001</v>
       </c>
       <c r="E4" s="2">
         <f t="shared" si="2"/>
-        <v>3.048</v>
+        <v>-2.8328000000000007</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" si="3"/>
-        <v>3.8572000000000002</v>
+        <v>8.2365999999999993</v>
       </c>
       <c r="G4" s="2">
         <f t="shared" si="4"/>
-        <v>3.8213825784485849</v>
+        <v>3.8528467423598984</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -5783,19 +5891,19 @@
       </c>
       <c r="D5" s="2">
         <f t="shared" si="1"/>
-        <v>8.3795999999999999</v>
+        <v>13.645799999999999</v>
       </c>
       <c r="E5" s="2">
         <f t="shared" si="2"/>
-        <v>3.3459000000000003</v>
+        <v>-4.9365000000000006</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="3"/>
-        <v>4.4013</v>
+        <v>9.9123000000000001</v>
       </c>
       <c r="G5" s="2">
         <f t="shared" si="4"/>
-        <v>4.3129075777236281</v>
+        <v>4.3662839325712453</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -5811,19 +5919,19 @@
       </c>
       <c r="D6" s="2">
         <f t="shared" si="1"/>
-        <v>10.172799999999999</v>
+        <v>17.194400000000002</v>
       </c>
       <c r="E6" s="2">
         <f t="shared" si="2"/>
-        <v>3.8264</v>
+        <v>-6.4984000000000002</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="3"/>
-        <v>5.0351999999999997</v>
+        <v>11.074</v>
       </c>
       <c r="G6" s="2">
         <f t="shared" si="4"/>
-        <v>4.8676549369567841</v>
+        <v>4.9481426733710929</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -5839,19 +5947,19 @@
       </c>
       <c r="D7" s="2">
         <f t="shared" si="1"/>
-        <v>11.965999999999999</v>
+        <v>20.742999999999999</v>
       </c>
       <c r="E7" s="2">
         <f t="shared" si="2"/>
-        <v>4.4895000000000005</v>
+        <v>-7.5185000000000013</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="3"/>
-        <v>5.7684999999999995</v>
+        <v>11.807500000000001</v>
       </c>
       <c r="G7" s="2">
         <f t="shared" si="4"/>
-        <v>5.4937566266573192</v>
+        <v>5.6075409419418296</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -5867,19 +5975,19 @@
       </c>
       <c r="D8" s="2">
         <f t="shared" si="1"/>
-        <v>13.7592</v>
+        <v>24.291599999999999</v>
       </c>
       <c r="E8" s="2">
         <f t="shared" si="2"/>
-        <v>5.3352000000000004</v>
+        <v>-7.9968000000000021</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="3"/>
-        <v>6.6108000000000002</v>
+        <v>12.198600000000003</v>
       </c>
       <c r="G8" s="2">
         <f t="shared" si="4"/>
-        <v>6.2003905913286319</v>
+        <v>6.3548117932766051</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -5895,19 +6003,19 @@
       </c>
       <c r="D9" s="2">
         <f t="shared" si="1"/>
-        <v>15.552399999999999</v>
+        <v>27.840199999999999</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="2"/>
-        <v>6.3635000000000002</v>
+        <v>-7.9333000000000009</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="3"/>
-        <v>7.5716999999999999</v>
+        <v>12.333100000000002</v>
       </c>
       <c r="G9" s="2">
         <f t="shared" si="4"/>
-        <v>6.9979152877815824</v>
+        <v>7.201665283603444</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -5923,19 +6031,19 @@
       </c>
       <c r="D10" s="2">
         <f t="shared" si="1"/>
-        <v>17.345599999999997</v>
+        <v>31.3888</v>
       </c>
       <c r="E10" s="2">
         <f t="shared" si="2"/>
-        <v>7.5744000000000007</v>
+        <v>-7.328000000000003</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="3"/>
-        <v>8.6608000000000001</v>
+        <v>12.296800000000001</v>
       </c>
       <c r="G10" s="2">
         <f t="shared" si="4"/>
-        <v>7.8980215284265842</v>
+        <v>8.1613719720120113</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -5951,19 +6059,19 @@
       </c>
       <c r="D11" s="2">
         <f t="shared" si="1"/>
-        <v>19.1388</v>
+        <v>34.937399999999997</v>
       </c>
       <c r="E11" s="2">
         <f t="shared" si="2"/>
-        <v>8.9679000000000002</v>
+        <v>-6.1809000000000047</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="3"/>
-        <v>9.8877000000000006</v>
+        <v>12.1755</v>
       </c>
       <c r="G11" s="2">
         <f t="shared" si="4"/>
-        <v>8.9139038553958496</v>
+        <v>9.2489708758326348</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -5979,19 +6087,19 @@
       </c>
       <c r="D12" s="2">
         <f t="shared" si="1"/>
-        <v>20.931999999999999</v>
+        <v>38.485999999999997</v>
       </c>
       <c r="E12" s="2">
         <f t="shared" si="2"/>
-        <v>10.544</v>
+        <v>-4.4920000000000044</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="3"/>
-        <v>11.262</v>
+        <v>12.055000000000003</v>
       </c>
       <c r="G12" s="2">
         <f t="shared" si="4"/>
-        <v>10.06045395764707</v>
+        <v>10.481505138517953</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -6007,19 +6115,19 @@
       </c>
       <c r="D13" s="2">
         <f t="shared" si="1"/>
-        <v>22.725199999999997</v>
+        <v>42.034599999999998</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="2"/>
-        <v>12.3027</v>
+        <v>-2.2612999999999985</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="3"/>
-        <v>12.7933</v>
+        <v>12.021100000000001</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="4"/>
-        <v>11.354478966325123</v>
+        <v>11.878289103044446</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -6035,19 +6143,19 @@
       </c>
       <c r="D14" s="2">
         <f t="shared" si="1"/>
-        <v>24.5184</v>
+        <v>45.583199999999998</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="2"/>
-        <v>14.244000000000002</v>
+        <v>0.51119999999999521</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="3"/>
-        <v>14.491199999999999</v>
+        <v>12.159600000000005</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="4"/>
-        <v>12.814947828345545</v>
+        <v>13.461210975989143</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -6063,19 +6171,19 @@
       </c>
       <c r="D15" s="2">
         <f t="shared" si="1"/>
-        <v>26.311599999999999</v>
+        <v>49.131799999999998</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="2"/>
-        <v>16.367899999999999</v>
+        <v>3.825499999999991</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="3"/>
-        <v>16.365299999999998</v>
+        <v>12.5563</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="4"/>
-        <v>14.463269369758573</v>
+        <v>15.255075825157959</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -6091,19 +6199,19 @@
       </c>
       <c r="D16" s="2">
         <f t="shared" si="1"/>
-        <v>28.104799999999997</v>
+        <v>52.680399999999999</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="2"/>
-        <v>18.674399999999999</v>
+        <v>7.681599999999996</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="3"/>
-        <v>18.4252</v>
+        <v>13.297000000000004</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="4"/>
-        <v>16.323606124989062</v>
+        <v>17.287994285686359</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -6119,19 +6227,19 @@
       </c>
       <c r="D17" s="2">
         <f t="shared" si="1"/>
-        <v>29.898</v>
+        <v>56.228999999999999</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="2"/>
-        <v>21.163499999999999</v>
+        <v>12.079499999999989</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="3"/>
-        <v>20.680499999999999</v>
+        <v>14.467500000000001</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="4"/>
-        <v>18.423228532334818</v>
+        <v>19.591823065804363</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -6147,19 +6255,19 @@
       </c>
       <c r="D18" s="2">
         <f t="shared" si="1"/>
-        <v>31.691199999999998</v>
+        <v>59.7776</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="2"/>
-        <v>23.8352</v>
+        <v>17.019199999999991</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="3"/>
-        <v>23.140799999999999</v>
+        <v>16.153600000000004</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="4"/>
-        <v>20.792914687829935</v>
+        <v>22.202664155181076</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -6175,19 +6283,19 @@
       </c>
       <c r="D19" s="2">
         <f t="shared" si="1"/>
-        <v>33.484399999999994</v>
+        <v>63.3262</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="2"/>
-        <v>26.689500000000002</v>
+        <v>22.500699999999995</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="3"/>
-        <v>25.8157</v>
+        <v>18.441100000000006</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="4"/>
-        <v>23.46740151741372</v>
+        <v>25.161430558658608</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -6203,19 +6311,19 @@
       </c>
       <c r="D20" s="2">
         <f t="shared" si="1"/>
-        <v>35.2776</v>
+        <v>66.874799999999993</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="2"/>
-        <v>29.726400000000002</v>
+        <v>28.523999999999987</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="3"/>
-        <v>28.7148</v>
+        <v>21.415800000000004</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="4"/>
-        <v>26.485893981080331</v>
+        <v>28.514487420666761</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -6231,19 +6339,19 @@
       </c>
       <c r="D21" s="2">
         <f t="shared" si="1"/>
-        <v>37.070799999999998</v>
+        <v>70.423400000000001</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="2"/>
-        <v>32.945899999999995</v>
+        <v>35.089099999999988</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="3"/>
-        <v>31.847700000000003</v>
+        <v>25.16350000000002</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="4"/>
-        <v>29.892639773367556</v>
+        <v>32.314378587014218</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -6259,19 +6367,19 @@
       </c>
       <c r="D22" s="2">
         <f t="shared" si="1"/>
-        <v>38.863999999999997</v>
+        <v>73.971999999999994</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="2"/>
-        <v>36.348000000000006</v>
+        <v>42.195999999999984</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="3"/>
-        <v>35.224000000000004</v>
+        <v>29.77000000000001</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="4"/>
-        <v>33.737577944645537</v>
+        <v>36.620649989592749</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -6287,19 +6395,19 @@
       </c>
       <c r="D23" s="2">
         <f t="shared" si="1"/>
-        <v>40.657199999999996</v>
+        <v>77.520600000000002</v>
       </c>
       <c r="E23" s="2">
         <f t="shared" si="2"/>
-        <v>39.932700000000004</v>
+        <v>49.844699999999989</v>
       </c>
       <c r="F23" s="2">
         <f t="shared" si="3"/>
-        <v>38.853300000000004</v>
+        <v>35.321100000000015</v>
       </c>
       <c r="G23" s="2">
         <f t="shared" si="4"/>
-        <v>38.077070951262002</v>
+        <v>41.500782756787387</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6315,19 +6423,19 @@
       </c>
       <c r="D24" s="2">
         <f t="shared" si="1"/>
-        <v>42.450399999999995</v>
+        <v>81.069199999999995</v>
       </c>
       <c r="E24" s="2">
         <f t="shared" si="2"/>
-        <v>43.7</v>
+        <v>58.035200000000003</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="3"/>
-        <v>42.745199999999997</v>
+        <v>41.902600000000007</v>
       </c>
       <c r="G24" s="2">
         <f t="shared" si="4"/>
-        <v>42.974730865573214</v>
+        <v>47.031250671834826</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -6343,19 +6451,19 @@
       </c>
       <c r="D25" s="2">
         <f t="shared" si="1"/>
-        <v>44.243600000000001</v>
+        <v>84.617800000000003</v>
       </c>
       <c r="E25" s="2">
         <f t="shared" si="2"/>
-        <v>47.649900000000009</v>
+        <v>66.767499999999984</v>
       </c>
       <c r="F25" s="2">
         <f t="shared" si="3"/>
-        <v>46.909300000000002</v>
+        <v>49.60029999999999</v>
       </c>
       <c r="G25" s="2">
         <f t="shared" si="4"/>
-        <v>48.50235185716776</v>
+        <v>53.298718549958053</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -6371,19 +6479,19 @@
       </c>
       <c r="D26" s="2">
         <f t="shared" si="1"/>
-        <v>46.036799999999999</v>
+        <v>88.166399999999996</v>
       </c>
       <c r="E26" s="2">
         <f t="shared" si="2"/>
-        <v>51.78240000000001</v>
+        <v>76.041599999999988</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="3"/>
-        <v>51.355199999999996</v>
+        <v>58.500000000000014</v>
       </c>
       <c r="G26" s="2">
         <f t="shared" si="4"/>
-        <v>54.740962614406051</v>
+        <v>60.401400313363524</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -6399,19 +6507,19 @@
       </c>
       <c r="D27" s="2">
         <f t="shared" si="1"/>
-        <v>47.83</v>
+        <v>91.715000000000003</v>
       </c>
       <c r="E27" s="2">
         <f t="shared" si="2"/>
-        <v>56.097500000000011</v>
+        <v>85.857499999999973</v>
       </c>
       <c r="F27" s="2">
         <f t="shared" si="3"/>
-        <v>56.092500000000001</v>
+        <v>68.6875</v>
       </c>
       <c r="G27" s="2">
         <f t="shared" si="4"/>
-        <v>61.782014133588085</v>
+        <v>68.450598045720966</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -6427,19 +6535,19 @@
       </c>
       <c r="D28" s="2">
         <f t="shared" si="1"/>
-        <v>49.623199999999997</v>
+        <v>95.263599999999997</v>
       </c>
       <c r="E28" s="2">
         <f t="shared" si="2"/>
-        <v>60.595200000000006</v>
+        <v>96.215199999999967</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="3"/>
-        <v>61.130799999999994</v>
+        <v>80.248599999999996</v>
       </c>
       <c r="G28" s="2">
         <f t="shared" si="4"/>
-        <v>69.728720287398858</v>
+        <v>77.572446143772936</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -6455,19 +6563,19 @@
       </c>
       <c r="D29" s="2">
         <f t="shared" si="1"/>
-        <v>51.416399999999996</v>
+        <v>98.812200000000004</v>
       </c>
       <c r="E29" s="2">
         <f t="shared" si="2"/>
-        <v>65.275500000000008</v>
+        <v>107.11469999999998</v>
       </c>
       <c r="F29" s="2">
         <f t="shared" si="3"/>
-        <v>66.479700000000008</v>
+        <v>93.269100000000023</v>
       </c>
       <c r="G29" s="2">
         <f t="shared" si="4"/>
-        <v>78.697570823852573</v>
+        <v>87.909887897680989</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -6483,19 +6591,19 @@
       </c>
       <c r="D30" s="2">
         <f t="shared" si="1"/>
-        <v>53.209599999999995</v>
+        <v>102.3608</v>
       </c>
       <c r="E30" s="2">
         <f t="shared" si="2"/>
-        <v>70.138400000000004</v>
+        <v>118.55599999999998</v>
       </c>
       <c r="F30" s="2">
         <f t="shared" si="3"/>
-        <v>72.148800000000008</v>
+        <v>107.83480000000003</v>
       </c>
       <c r="G30" s="2">
         <f t="shared" si="4"/>
-        <v>88.820038974593459</v>
+        <v>99.624915473974738</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -6506,22 +6614,24 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31">
+        <v>127</v>
+      </c>
       <c r="D31" s="2">
         <f t="shared" si="1"/>
-        <v>55.002800000000001</v>
+        <v>105.90940000000001</v>
       </c>
       <c r="E31" s="2">
         <f t="shared" si="2"/>
-        <v>75.183900000000008</v>
+        <v>130.53909999999996</v>
       </c>
       <c r="F31" s="2">
         <f t="shared" si="3"/>
-        <v>78.1477</v>
+        <v>124.03150000000001</v>
       </c>
       <c r="G31" s="2">
         <f t="shared" si="4"/>
-        <v>100.24450870416462</v>
+        <v>112.90110840260132</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -6532,22 +6642,24 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32">
+        <v>183</v>
+      </c>
       <c r="D32" s="2">
         <f t="shared" si="1"/>
-        <v>56.795999999999999</v>
+        <v>109.458</v>
       </c>
       <c r="E32" s="2">
         <f t="shared" si="2"/>
-        <v>80.412000000000006</v>
+        <v>143.06399999999996</v>
       </c>
       <c r="F32" s="2">
         <f t="shared" si="3"/>
-        <v>84.486000000000004</v>
+        <v>141.94500000000002</v>
       </c>
       <c r="G32" s="2">
         <f t="shared" si="4"/>
-        <v>113.13844985154523</v>
+        <v>127.94651034726127</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -6558,22 +6670,24 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33">
+        <v>195</v>
+      </c>
       <c r="D33" s="2">
         <f t="shared" si="1"/>
-        <v>58.589199999999998</v>
+        <v>113.00660000000001</v>
       </c>
       <c r="E33" s="2">
         <f t="shared" si="2"/>
-        <v>85.822699999999998</v>
+        <v>156.13069999999993</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="3"/>
-        <v>91.173299999999998</v>
+        <v>161.66110000000003</v>
       </c>
       <c r="G33" s="2">
         <f t="shared" si="4"/>
-        <v>127.69087304907738</v>
+        <v>144.99688923926146</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -6584,22 +6698,24 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="C34" s="2"/>
+      <c r="C34">
+        <v>191</v>
+      </c>
       <c r="D34" s="2">
         <f t="shared" si="1"/>
-        <v>60.382399999999997</v>
+        <v>116.5552</v>
       </c>
       <c r="E34" s="2">
         <f t="shared" si="2"/>
-        <v>91.416000000000011</v>
+        <v>169.73919999999998</v>
       </c>
       <c r="F34" s="2">
         <f t="shared" si="3"/>
-        <v>98.219200000000001</v>
+        <v>183.26560000000001</v>
       </c>
       <c r="G34" s="2">
         <f t="shared" si="4"/>
-        <v>144.11510040512459</v>
+        <v>164.31943186258752</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -6610,22 +6726,24 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="C35" s="2"/>
+      <c r="C35">
+        <v>211</v>
+      </c>
       <c r="D35" s="2">
         <f t="shared" si="1"/>
-        <v>62.175599999999996</v>
+        <v>120.10379999999999</v>
       </c>
       <c r="E35" s="2">
         <f t="shared" si="2"/>
-        <v>97.191900000000004</v>
+        <v>183.88949999999994</v>
       </c>
       <c r="F35" s="2">
         <f t="shared" si="3"/>
-        <v>105.63330000000001</v>
+        <v>206.8443</v>
       </c>
       <c r="G35" s="2">
         <f t="shared" si="4"/>
-        <v>162.65189256554473</v>
+        <v>186.21693078593574</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -6636,22 +6754,24 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="C36" s="2"/>
+      <c r="C36">
+        <v>206</v>
+      </c>
       <c r="D36" s="2">
         <f t="shared" si="1"/>
-        <v>63.968799999999995</v>
+        <v>123.6524</v>
       </c>
       <c r="E36" s="2">
         <f t="shared" si="2"/>
-        <v>103.15040000000002</v>
+        <v>198.58159999999998</v>
       </c>
       <c r="F36" s="2">
         <f t="shared" si="3"/>
-        <v>113.4252</v>
+        <v>232.483</v>
       </c>
       <c r="G36" s="2">
         <f t="shared" si="4"/>
-        <v>183.57297799317055</v>
+        <v>211.03252925273313</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -6665,19 +6785,19 @@
       <c r="C37" s="2"/>
       <c r="D37" s="2">
         <f t="shared" si="1"/>
-        <v>65.762</v>
+        <v>127.20099999999999</v>
       </c>
       <c r="E37" s="2">
         <f t="shared" si="2"/>
-        <v>109.2915</v>
+        <v>213.81549999999996</v>
       </c>
       <c r="F37" s="2">
         <f t="shared" si="3"/>
-        <v>121.6045</v>
+        <v>260.26749999999998</v>
       </c>
       <c r="G37" s="2">
         <f t="shared" si="4"/>
-        <v>207.18503620055441</v>
+        <v>239.1550983836172</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -6691,19 +6811,19 @@
       <c r="C38" s="2"/>
       <c r="D38" s="2">
         <f t="shared" si="1"/>
-        <v>67.555199999999999</v>
+        <v>130.74959999999999</v>
       </c>
       <c r="E38" s="2">
         <f t="shared" si="2"/>
-        <v>115.61520000000002</v>
+        <v>229.59119999999996</v>
       </c>
       <c r="F38" s="2">
         <f t="shared" si="3"/>
-        <v>130.18080000000003</v>
+        <v>290.28359999999998</v>
       </c>
       <c r="G38" s="2">
         <f t="shared" si="4"/>
-        <v>233.83419332567581</v>
+        <v>271.02533095445438</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -6717,19 +6837,19 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2">
         <f t="shared" si="1"/>
-        <v>69.348399999999998</v>
+        <v>134.29820000000001</v>
       </c>
       <c r="E39" s="2">
         <f t="shared" si="2"/>
-        <v>122.12150000000001</v>
+        <v>245.90869999999995</v>
       </c>
       <c r="F39" s="2">
         <f t="shared" si="3"/>
-        <v>139.16370000000001</v>
+        <v>322.61710000000005</v>
       </c>
       <c r="G39" s="2">
         <f t="shared" si="4"/>
-        <v>263.91109595067951</v>
+        <v>307.14264724202667</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -6743,19 +6863,19 @@
       <c r="C40" s="2"/>
       <c r="D40" s="2">
         <f t="shared" si="1"/>
-        <v>71.141599999999997</v>
+        <v>137.8468</v>
       </c>
       <c r="E40" s="2">
         <f t="shared" si="2"/>
-        <v>128.81040000000002</v>
+        <v>262.76799999999992</v>
       </c>
       <c r="F40" s="2">
         <f t="shared" si="3"/>
-        <v>148.56279999999998</v>
+        <v>357.35380000000009</v>
       </c>
       <c r="G40" s="2">
         <f t="shared" si="4"/>
-        <v>297.85663754010523</v>
+        <v>348.07302115496111</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -6769,19 +6889,19 @@
       <c r="C41" s="2"/>
       <c r="D41" s="2">
         <f t="shared" si="1"/>
-        <v>72.934799999999996</v>
+        <v>141.3954</v>
       </c>
       <c r="E41" s="2">
         <f t="shared" si="2"/>
-        <v>135.68190000000001</v>
+        <v>280.16909999999996</v>
       </c>
       <c r="F41" s="2">
         <f t="shared" si="3"/>
-        <v>158.38770000000002</v>
+        <v>394.57950000000005</v>
       </c>
       <c r="G41" s="2">
         <f t="shared" si="4"/>
-        <v>336.1684214417329</v>
+        <v>394.45784928874616</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -6795,19 +6915,19 @@
       <c r="C42" s="2"/>
       <c r="D42" s="2">
         <f t="shared" si="1"/>
-        <v>74.727999999999994</v>
+        <v>144.94399999999999</v>
       </c>
       <c r="E42" s="2">
         <f t="shared" si="2"/>
-        <v>142.73600000000002</v>
+        <v>298.11199999999997</v>
       </c>
       <c r="F42" s="2">
         <f t="shared" si="3"/>
-        <v>168.648</v>
+        <v>434.38000000000005</v>
       </c>
       <c r="G42" s="2">
         <f t="shared" si="4"/>
-        <v>379.40805519034427</v>
+        <v>447.02400188675313</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -6821,19 +6941,19 @@
       <c r="C43" s="2"/>
       <c r="D43" s="2">
         <f t="shared" si="1"/>
-        <v>76.521199999999993</v>
+        <v>148.49260000000001</v>
       </c>
       <c r="E43" s="2">
         <f t="shared" si="2"/>
-        <v>149.9727</v>
+        <v>316.59669999999994</v>
       </c>
       <c r="F43" s="2">
         <f t="shared" si="3"/>
-        <v>179.35330000000002</v>
+        <v>476.84110000000004</v>
       </c>
       <c r="G43" s="2">
         <f t="shared" si="4"/>
-        <v>428.20938304066692</v>
+        <v>506.59521321014563</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -6847,19 +6967,19 @@
       <c r="C44" s="2"/>
       <c r="D44" s="2">
         <f t="shared" si="1"/>
-        <v>78.314399999999992</v>
+        <v>152.0412</v>
       </c>
       <c r="E44" s="2">
         <f t="shared" si="2"/>
-        <v>157.392</v>
+        <v>335.6232</v>
       </c>
       <c r="F44" s="2">
         <f t="shared" si="3"/>
-        <v>190.51320000000001</v>
+        <v>522.04860000000008</v>
       </c>
       <c r="G44" s="2">
         <f t="shared" si="4"/>
-        <v>483.28777740914688</v>
+        <v>574.10498980868704</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -6873,19 +6993,19 @@
       <c r="C45" s="2"/>
       <c r="D45" s="2">
         <f t="shared" si="1"/>
-        <v>80.107599999999991</v>
+        <v>155.5898</v>
       </c>
       <c r="E45" s="2">
         <f t="shared" si="2"/>
-        <v>164.99390000000002</v>
+        <v>355.19149999999996</v>
       </c>
       <c r="F45" s="2">
         <f t="shared" si="3"/>
-        <v>202.13730000000001</v>
+        <v>570.0883</v>
       </c>
       <c r="G45" s="2">
         <f t="shared" si="4"/>
-        <v>545.45062542660662</v>
+        <v>650.61123897060952</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -6899,19 +7019,19 @@
       <c r="C46" s="2"/>
       <c r="D46" s="2">
         <f t="shared" si="1"/>
-        <v>81.90079999999999</v>
+        <v>159.13839999999999</v>
       </c>
       <c r="E46" s="2">
         <f t="shared" si="2"/>
-        <v>172.7784</v>
+        <v>375.30160000000001</v>
       </c>
       <c r="F46" s="2">
         <f t="shared" si="3"/>
-        <v>214.23519999999999</v>
+        <v>621.04600000000005</v>
       </c>
       <c r="G46" s="2">
         <f t="shared" si="4"/>
-        <v>615.60916432281715</v>
+        <v>737.31284658565448</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -6925,19 +7045,19 @@
       <c r="C47" s="2"/>
       <c r="D47" s="2">
         <f t="shared" si="1"/>
-        <v>83.694000000000003</v>
+        <v>162.68700000000001</v>
       </c>
       <c r="E47" s="2">
         <f t="shared" si="2"/>
-        <v>180.74550000000002</v>
+        <v>395.95349999999996</v>
       </c>
       <c r="F47" s="2">
         <f t="shared" si="3"/>
-        <v>226.81649999999999</v>
+        <v>675.00750000000005</v>
       </c>
       <c r="G47" s="2">
         <f t="shared" si="4"/>
-        <v>694.79183913637371</v>
+        <v>835.56846420354975</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -6951,19 +7071,19 @@
       <c r="C48" s="2"/>
       <c r="D48" s="2">
         <f t="shared" si="1"/>
-        <v>85.487200000000001</v>
+        <v>166.23560000000001</v>
       </c>
       <c r="E48" s="2">
         <f t="shared" si="2"/>
-        <v>188.89520000000002</v>
+        <v>417.14719999999994</v>
       </c>
       <c r="F48" s="2">
         <f t="shared" si="3"/>
-        <v>239.89080000000001</v>
+        <v>732.05859999999996</v>
       </c>
       <c r="G48" s="2">
         <f t="shared" si="4"/>
-        <v>784.15937855883521</v>
+        <v>946.91779968921446</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -6977,19 +7097,19 @@
       <c r="C49" s="2"/>
       <c r="D49" s="2">
         <f t="shared" si="1"/>
-        <v>87.2804</v>
+        <v>169.7842</v>
       </c>
       <c r="E49" s="2">
         <f t="shared" si="2"/>
-        <v>197.22750000000002</v>
+        <v>438.8827</v>
       </c>
       <c r="F49" s="2">
         <f t="shared" si="3"/>
-        <v>253.46770000000004</v>
+        <v>792.28510000000006</v>
       </c>
       <c r="G49" s="2">
         <f t="shared" si="4"/>
-        <v>885.02180990799593</v>
+        <v>1073.1057451084371</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -7003,19 +7123,19 @@
       <c r="C50" s="2"/>
       <c r="D50" s="2">
         <f t="shared" si="1"/>
-        <v>89.073599999999999</v>
+        <v>173.33279999999999</v>
       </c>
       <c r="E50" s="2">
         <f t="shared" si="2"/>
-        <v>205.74240000000003</v>
+        <v>461.15999999999997</v>
       </c>
       <c r="F50" s="2">
         <f t="shared" si="3"/>
-        <v>267.55680000000001</v>
+        <v>855.77280000000007</v>
       </c>
       <c r="G50" s="2">
         <f t="shared" si="4"/>
-        <v>998.85766265060033</v>
+        <v>1216.1097199383971</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -7029,19 +7149,19 @@
       <c r="C51" s="2"/>
       <c r="D51" s="2">
         <f t="shared" si="1"/>
-        <v>90.866799999999998</v>
+        <v>176.88139999999999</v>
       </c>
       <c r="E51" s="2">
         <f t="shared" si="2"/>
-        <v>214.43990000000002</v>
+        <v>483.9790999999999</v>
       </c>
       <c r="F51" s="2">
         <f t="shared" si="3"/>
-        <v>282.16770000000002</v>
+        <v>922.60749999999996</v>
       </c>
       <c r="G51" s="2">
         <f t="shared" si="4"/>
-        <v>1127.3356419764843</v>
+        <v>1378.1706580829104</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -7054,19 +7174,19 @@
       </c>
       <c r="D52" s="2">
         <f t="shared" si="1"/>
-        <v>92.66</v>
+        <v>180.43</v>
       </c>
       <c r="E52" s="2">
         <f t="shared" si="2"/>
-        <v>223.32000000000002</v>
+        <v>507.33999999999992</v>
       </c>
       <c r="F52" s="2">
         <f t="shared" si="3"/>
-        <v>297.31</v>
+        <v>992.875</v>
       </c>
       <c r="G52" s="2">
         <f t="shared" si="4"/>
-        <v>1272.3390901342925</v>
+        <v>1561.8281242722865</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -7079,19 +7199,19 @@
       </c>
       <c r="D53" s="2">
         <f t="shared" si="1"/>
-        <v>94.453199999999995</v>
+        <v>183.9786</v>
       </c>
       <c r="E53" s="2">
         <f t="shared" si="2"/>
-        <v>232.3827</v>
+        <v>531.2426999999999</v>
       </c>
       <c r="F53" s="2">
         <f t="shared" si="3"/>
-        <v>312.99329999999998</v>
+        <v>1066.6611</v>
       </c>
       <c r="G53" s="2">
         <f t="shared" si="4"/>
-        <v>1435.9935941043614</v>
+        <v>1769.9601101369137</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -7104,19 +7224,19 @@
       </c>
       <c r="D54" s="2">
         <f t="shared" si="1"/>
-        <v>96.246399999999994</v>
+        <v>187.52719999999999</v>
       </c>
       <c r="E54" s="2">
         <f t="shared" si="2"/>
-        <v>241.62800000000001</v>
+        <v>555.68719999999985</v>
       </c>
       <c r="F54" s="2">
         <f t="shared" si="3"/>
-        <v>329.22719999999998</v>
+        <v>1144.0516</v>
       </c>
       <c r="G54" s="2">
         <f t="shared" si="4"/>
-        <v>1620.6981443061027</v>
+        <v>2005.8281335761842</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -7129,19 +7249,19 @@
       </c>
       <c r="D55" s="2">
         <f t="shared" si="1"/>
-        <v>98.039599999999993</v>
+        <v>191.07579999999999</v>
       </c>
       <c r="E55" s="2">
         <f t="shared" si="2"/>
-        <v>251.05590000000001</v>
+        <v>580.67349999999988</v>
       </c>
       <c r="F55" s="2">
         <f t="shared" si="3"/>
-        <v>346.0213</v>
+        <v>1225.1323</v>
       </c>
       <c r="G55" s="2">
         <f t="shared" si="4"/>
-        <v>1829.1603010913932</v>
+        <v>2273.1283481493238</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -7154,19 +7274,19 @@
       </c>
       <c r="D56" s="2">
         <f t="shared" si="1"/>
-        <v>99.832799999999992</v>
+        <v>194.62440000000001</v>
       </c>
       <c r="E56" s="2">
         <f t="shared" si="2"/>
-        <v>260.66640000000007</v>
+        <v>606.20159999999998</v>
       </c>
       <c r="F56" s="2">
         <f t="shared" si="3"/>
-        <v>363.3852</v>
+        <v>1309.989</v>
       </c>
       <c r="G56" s="2">
         <f t="shared" si="4"/>
-        <v>2064.4358845250972</v>
+        <v>2576.0494633942799</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -7179,19 +7299,19 @@
       </c>
       <c r="D57" s="2">
         <f t="shared" si="1"/>
-        <v>101.62599999999999</v>
+        <v>198.173</v>
       </c>
       <c r="E57" s="2">
         <f t="shared" si="2"/>
-        <v>270.45949999999999</v>
+        <v>632.27149999999995</v>
       </c>
       <c r="F57" s="2">
         <f t="shared" si="3"/>
-        <v>381.32849999999996</v>
+        <v>1398.7074999999998</v>
       </c>
       <c r="G57" s="2">
         <f t="shared" si="4"/>
-        <v>2329.973769260137</v>
+        <v>2919.3383837110214</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -7204,22 +7324,34 @@
       </c>
       <c r="D58" s="2">
         <f t="shared" si="1"/>
-        <v>103.41919999999999</v>
+        <v>201.7216</v>
       </c>
       <c r="E58" s="2">
         <f t="shared" si="2"/>
-        <v>280.43520000000001</v>
+        <v>658.88319999999999</v>
       </c>
       <c r="F58" s="2">
         <f t="shared" si="3"/>
-        <v>399.86079999999998</v>
+        <v>1491.3736000000004</v>
       </c>
       <c r="G58" s="2">
         <f t="shared" si="4"/>
-        <v>2629.6664411494335</v>
+        <v>3308.3745943988702</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:G1048576">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+      <formula>$C1*0.75</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+      <formula>$C1*0.75</formula>
+      <formula>$C1*1.25</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>$C1*1.25</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Did a bunch of small changes to make the display of the app better when you rotate the screen
Started to move the updown stuff into the aggregate roller
</commit_message>
<xml_diff>
--- a/InstallTracker.xlsx
+++ b/InstallTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3478EB8-EEC2-45F3-9A57-29948944021E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368963CB-D3B4-4426-8A5B-6FD571269196}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Days Since Release</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>Last Updated</t>
   </si>
 </sst>
 </file>
@@ -92,7 +89,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -104,20 +101,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -577,6 +560,12 @@
                 </c:pt>
                 <c:pt idx="34" formatCode="General">
                   <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1320,6 +1309,12 @@
                 <c:pt idx="34" formatCode="General">
                   <c:v>206</c:v>
                 </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>227</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2062,6 +2057,12 @@
                 <c:pt idx="34" formatCode="General">
                   <c:v>206</c:v>
                 </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>227</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2802,6 +2803,12 @@
                 </c:pt>
                 <c:pt idx="34" formatCode="General">
                   <c:v>206</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>219</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>227</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5372,15 +5379,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>57150</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
+      <xdr:colOff>361950</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5752,7 +5759,7 @@
   <dimension ref="A1:H58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5787,9 +5794,6 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -5818,9 +5822,7 @@
         <f>3*EXP(0.1251*B2)</f>
         <v>3</v>
       </c>
-      <c r="H2" s="1">
-        <v>43655</v>
-      </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -6782,7 +6784,9 @@
         <f>B36+1</f>
         <v>35</v>
       </c>
-      <c r="C37" s="2"/>
+      <c r="C37">
+        <v>219</v>
+      </c>
       <c r="D37" s="2">
         <f t="shared" si="1"/>
         <v>127.20099999999999</v>
@@ -6808,7 +6812,9 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38">
+        <v>227</v>
+      </c>
       <c r="D38" s="2">
         <f t="shared" si="1"/>
         <v>130.74959999999999</v>

</xml_diff>

<commit_message>
Did some more work on the behind the scenes logic for advantage/disadvantage & drop high/low rolls
Fixed a bug where the name of the class was saved and not the name of the string for saved rolls
</commit_message>
<xml_diff>
--- a/InstallTracker.xlsx
+++ b/InstallTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D761890-44E8-4438-8EA0-AF9E6026709C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1935073B-E73C-402B-B768-084905AEF88E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -593,6 +593,18 @@
                 </c:pt>
                 <c:pt idx="44" formatCode="General">
                   <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1366,6 +1378,18 @@
                 <c:pt idx="44" formatCode="General">
                   <c:v>315</c:v>
                 </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>386</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2138,6 +2162,18 @@
                 <c:pt idx="44" formatCode="General">
                   <c:v>315</c:v>
                 </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>386</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2908,6 +2944,18 @@
                 </c:pt>
                 <c:pt idx="44" formatCode="General">
                   <c:v>315</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>334</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>331</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>356</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>386</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3333,6 +3381,86 @@
             <c:trendlineType val="log"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:intercept val="0"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.37881430446194225"/>
+                  <c:y val="-4.6180373286672502E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
           </c:trendline>
           <c:xVal>
             <c:numRef>
@@ -7177,8 +7305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8666,8 +8794,13 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
+      <c r="C47">
+        <v>334</v>
+      </c>
+      <c r="D47" s="2">
+        <f t="shared" si="5"/>
+        <v>11.714285714285714</v>
+      </c>
       <c r="E47" s="2">
         <f t="shared" si="1"/>
         <v>237.73350000000002</v>
@@ -8693,8 +8826,13 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
+      <c r="C48">
+        <v>331</v>
+      </c>
+      <c r="D48" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
       <c r="E48" s="2">
         <f t="shared" si="1"/>
         <v>242.94980000000001</v>
@@ -8720,8 +8858,13 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
+      <c r="C49">
+        <v>356</v>
+      </c>
+      <c r="D49" s="2">
+        <f t="shared" si="5"/>
+        <v>12.571428571428571</v>
+      </c>
       <c r="E49" s="2">
         <f t="shared" si="1"/>
         <v>248.16610000000003</v>
@@ -8747,8 +8890,13 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="C50">
+        <v>386</v>
+      </c>
+      <c r="D50" s="2">
+        <f t="shared" si="5"/>
+        <v>14.142857142857142</v>
+      </c>
       <c r="E50" s="2">
         <f t="shared" si="1"/>
         <v>253.38240000000002</v>
@@ -8775,7 +8923,10 @@
         <v>49</v>
       </c>
       <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
+      <c r="D51" s="2">
+        <f t="shared" si="5"/>
+        <v>-41.285714285714285</v>
+      </c>
       <c r="E51" s="2">
         <f t="shared" si="1"/>
         <v>258.59870000000001</v>
@@ -8801,7 +8952,10 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="D52" s="2"/>
+      <c r="D52" s="2">
+        <f t="shared" si="5"/>
+        <v>-43</v>
+      </c>
       <c r="E52" s="2">
         <f t="shared" si="1"/>
         <v>263.815</v>
@@ -8827,7 +8981,10 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2">
+        <f t="shared" si="5"/>
+        <v>-45</v>
+      </c>
       <c r="E53" s="2">
         <f t="shared" si="1"/>
         <v>269.03130000000004</v>
@@ -8853,7 +9010,10 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="D54" s="2"/>
+      <c r="D54" s="2">
+        <f t="shared" si="5"/>
+        <v>-47.714285714285715</v>
+      </c>
       <c r="E54" s="2">
         <f t="shared" si="1"/>
         <v>274.24760000000003</v>
@@ -8879,7 +9039,10 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="D55" s="2"/>
+      <c r="D55" s="2">
+        <f t="shared" si="5"/>
+        <v>-47.285714285714285</v>
+      </c>
       <c r="E55" s="2">
         <f t="shared" si="1"/>
         <v>279.46390000000002</v>
@@ -8905,7 +9068,10 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="D56" s="2"/>
+      <c r="D56" s="2">
+        <f t="shared" si="5"/>
+        <v>-50.857142857142854</v>
+      </c>
       <c r="E56" s="2">
         <f t="shared" si="1"/>
         <v>284.68020000000001</v>
@@ -8931,7 +9097,10 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="D57" s="2"/>
+      <c r="D57" s="2">
+        <f t="shared" si="5"/>
+        <v>-55.142857142857146</v>
+      </c>
       <c r="E57" s="2">
         <f t="shared" si="1"/>
         <v>289.8965</v>
@@ -8957,7 +9126,10 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="D58" s="2">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
       <c r="E58" s="2">
         <f t="shared" si="1"/>
         <v>295.11279999999999</v>

</xml_diff>

<commit_message>
Added a remove die button to the custom die holder. Made it so you can never have 0 dice being rolled.
</commit_message>
<xml_diff>
--- a/InstallTracker.xlsx
+++ b/InstallTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD876A9-986E-4270-B10C-9937847584F8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62978B7-3A4D-4144-AAAE-5CEBCFEE5E06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -89,28 +89,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -737,6 +716,15 @@
                 </c:pt>
                 <c:pt idx="55" formatCode="General">
                   <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="General">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="General">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="General">
+                  <c:v>592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1636,6 +1624,15 @@
                 <c:pt idx="55" formatCode="General">
                   <c:v>522</c:v>
                 </c:pt>
+                <c:pt idx="56" formatCode="General">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="General">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="General">
+                  <c:v>592</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2533,6 +2530,15 @@
                 </c:pt>
                 <c:pt idx="55" formatCode="General">
                   <c:v>522</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="General">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="General">
+                  <c:v>573</c:v>
+                </c:pt>
+                <c:pt idx="58" formatCode="General">
+                  <c:v>592</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3476,6 +3482,15 @@
                 <c:pt idx="55">
                   <c:v>19.428571428571427</c:v>
                 </c:pt>
+                <c:pt idx="56">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>25.428571428571427</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -6423,7 +6438,7 @@
   <dimension ref="A1:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8092,7 +8107,13 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="D58" s="2"/>
+      <c r="C58">
+        <v>546</v>
+      </c>
+      <c r="D58" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
       <c r="E58" s="2">
         <f t="shared" si="1"/>
         <v>374.30239999999998</v>
@@ -8115,7 +8136,13 @@
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="D59" s="2"/>
+      <c r="C59">
+        <v>573</v>
+      </c>
+      <c r="D59" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
       <c r="E59" s="2">
         <f t="shared" si="1"/>
         <v>380.93279999999999</v>
@@ -8137,7 +8164,13 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="D60" s="2"/>
+      <c r="C60">
+        <v>592</v>
+      </c>
+      <c r="D60" s="2">
+        <f t="shared" si="4"/>
+        <v>25.428571428571427</v>
+      </c>
       <c r="E60" s="2">
         <f t="shared" si="1"/>
         <v>387.56319999999999</v>
@@ -9363,14 +9396,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E1:G1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>$C1*1.25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>$C1*0.75</formula>
       <formula>$C1*1.25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="lessThan">
       <formula>$C1*0.75</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated install tracker and renamed a bunch of svgs to make more sense
</commit_message>
<xml_diff>
--- a/InstallTracker.xlsx
+++ b/InstallTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16FF9FC8-43D6-4ED5-A547-5A8804DFE6E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5252BFB7-F318-4847-8652-24C86ABCEE59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12643" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Actual</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Average/Ever</t>
+  </si>
+  <si>
+    <t>Poly2 Expected to hit 5k - 10/25/19</t>
+  </si>
+  <si>
+    <t>Poly3 Expected to hit 5k - 10/25/19</t>
   </si>
 </sst>
 </file>
@@ -1162,13 +1168,37 @@
                   <c:v>3507</c:v>
                 </c:pt>
                 <c:pt idx="126" formatCode="#,##0">
-                  <c:v>3561</c:v>
+                  <c:v>3533</c:v>
                 </c:pt>
                 <c:pt idx="127" formatCode="#,##0">
-                  <c:v>3609</c:v>
+                  <c:v>3601</c:v>
                 </c:pt>
                 <c:pt idx="128" formatCode="#,##0">
-                  <c:v>3632</c:v>
+                  <c:v>3636</c:v>
+                </c:pt>
+                <c:pt idx="129" formatCode="#,##0">
+                  <c:v>3705</c:v>
+                </c:pt>
+                <c:pt idx="130" formatCode="#,##0">
+                  <c:v>3723</c:v>
+                </c:pt>
+                <c:pt idx="131" formatCode="#,##0">
+                  <c:v>3806</c:v>
+                </c:pt>
+                <c:pt idx="132" formatCode="#,##0">
+                  <c:v>3822</c:v>
+                </c:pt>
+                <c:pt idx="133" formatCode="#,##0">
+                  <c:v>3873</c:v>
+                </c:pt>
+                <c:pt idx="134" formatCode="#,##0">
+                  <c:v>3908</c:v>
+                </c:pt>
+                <c:pt idx="135" formatCode="#,##0">
+                  <c:v>3961</c:v>
+                </c:pt>
+                <c:pt idx="136" formatCode="#,##0">
+                  <c:v>4023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2468,13 +2498,37 @@
                   <c:v>3507</c:v>
                 </c:pt>
                 <c:pt idx="126" formatCode="#,##0">
-                  <c:v>3561</c:v>
+                  <c:v>3533</c:v>
                 </c:pt>
                 <c:pt idx="127" formatCode="#,##0">
-                  <c:v>3609</c:v>
+                  <c:v>3601</c:v>
                 </c:pt>
                 <c:pt idx="128" formatCode="#,##0">
-                  <c:v>3632</c:v>
+                  <c:v>3636</c:v>
+                </c:pt>
+                <c:pt idx="129" formatCode="#,##0">
+                  <c:v>3705</c:v>
+                </c:pt>
+                <c:pt idx="130" formatCode="#,##0">
+                  <c:v>3723</c:v>
+                </c:pt>
+                <c:pt idx="131" formatCode="#,##0">
+                  <c:v>3806</c:v>
+                </c:pt>
+                <c:pt idx="132" formatCode="#,##0">
+                  <c:v>3822</c:v>
+                </c:pt>
+                <c:pt idx="133" formatCode="#,##0">
+                  <c:v>3873</c:v>
+                </c:pt>
+                <c:pt idx="134" formatCode="#,##0">
+                  <c:v>3908</c:v>
+                </c:pt>
+                <c:pt idx="135" formatCode="#,##0">
+                  <c:v>3961</c:v>
+                </c:pt>
+                <c:pt idx="136" formatCode="#,##0">
+                  <c:v>4023</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3818,13 +3872,37 @@
                   <c:v>57.428571428571431</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>53.142857142857146</c:v>
+                  <c:v>49.142857142857146</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>55</c:v>
+                  <c:v>53.857142857142854</c:v>
                 </c:pt>
                 <c:pt idx="128">
+                  <c:v>52.142857142857146</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>49.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="130">
                   <c:v>51.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>48.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>43.857142857142854</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>46.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>45.428571428571431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5121,13 +5199,37 @@
                   <c:v>65</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>54</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>48</c:v>
+                  <c:v>68</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>23</c:v>
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>62</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6477,13 +6579,37 @@
                   <c:v>27.80952380952381</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>28.015748031496063</c:v>
+                  <c:v>27.795275590551181</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>28.171875</c:v>
+                  <c:v>28.109375</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>28.131782945736433</c:v>
+                  <c:v>28.162790697674417</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>28.476923076923075</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>28.396946564885496</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>28.810606060606062</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>28.714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>28.880597014925375</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>28.925925925925927</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>29.102941176470587</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>29.343065693430656</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10027,7 +10153,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S36" sqref="S36"/>
+      <selection pane="bottomLeft" activeCell="C138" sqref="C138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -10091,11 +10217,11 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <f>0.2511*B2^2-3.2838*B2+3</f>
+        <f>0.2429*B2^2-2.6363*B2+3</f>
         <v>3</v>
       </c>
       <c r="H2" s="2">
-        <f>-0.0003*B2^3+0.2972*B2^2-4.9611*B2+3</f>
+        <f>-0.0004*B2^3+0.3111*B2^2-5.4294*B2+3</f>
         <v>3</v>
       </c>
       <c r="I2" s="2"/>
@@ -10125,12 +10251,12 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G66" si="1">0.2511*B3^2-3.2838*B3+3</f>
-        <v>-3.2699999999999729E-2</v>
+        <f t="shared" ref="G3:G66" si="1">0.2429*B3^2-2.6363*B3+3</f>
+        <v>0.60660000000000025</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H66" si="2">-0.0003*B3^3+0.2972*B3^2-4.9611*B3+3</f>
-        <v>-1.6642000000000001</v>
+        <f t="shared" ref="H3:H66" si="2">-0.0004*B3^3+0.3111*B3^2-5.4294*B3+3</f>
+        <v>-2.1187000000000005</v>
       </c>
       <c r="I3" s="2"/>
     </row>
@@ -10159,11 +10285,11 @@
       </c>
       <c r="G4" s="2">
         <f t="shared" si="1"/>
-        <v>-2.5632000000000001</v>
+        <v>-1.3010000000000002</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="2"/>
-        <v>-5.7357999999999993</v>
+        <v>-6.6176000000000013</v>
       </c>
       <c r="I4" s="2"/>
     </row>
@@ -10192,11 +10318,11 @@
       </c>
       <c r="G5" s="2">
         <f t="shared" si="1"/>
-        <v>-4.5914999999999999</v>
+        <v>-2.7227999999999994</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="2"/>
-        <v>-9.2165999999999997</v>
+        <v>-10.4991</v>
       </c>
       <c r="I5" s="2"/>
     </row>
@@ -10225,11 +10351,11 @@
       </c>
       <c r="G6" s="2">
         <f t="shared" si="1"/>
-        <v>-6.1175999999999995</v>
+        <v>-3.6587999999999994</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="2"/>
-        <v>-12.1084</v>
+        <v>-13.765599999999999</v>
       </c>
       <c r="I6" s="2"/>
     </row>
@@ -10258,11 +10384,11 @@
       </c>
       <c r="G7" s="2">
         <f t="shared" si="1"/>
-        <v>-7.1415000000000006</v>
+        <v>-4.109</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="2"/>
-        <v>-14.413</v>
+        <v>-16.419500000000003</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -10291,11 +10417,11 @@
       </c>
       <c r="G8" s="2">
         <f t="shared" si="1"/>
-        <v>-7.6631999999999998</v>
+        <v>-4.0733999999999977</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>-16.132199999999997</v>
+        <v>-18.463200000000001</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -10324,11 +10450,11 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" si="1"/>
-        <v>-7.6827000000000005</v>
+        <v>-3.5519999999999996</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="2"/>
-        <v>-17.267799999999998</v>
+        <v>-19.899100000000001</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -10357,11 +10483,11 @@
       </c>
       <c r="G10" s="2">
         <f t="shared" si="1"/>
-        <v>-7.1999999999999993</v>
+        <v>-2.5447999999999986</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="2"/>
-        <v>-17.8216</v>
+        <v>-20.729600000000001</v>
       </c>
       <c r="I10" s="2"/>
     </row>
@@ -10390,11 +10516,11 @@
       </c>
       <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>-6.2150999999999996</v>
+        <v>-1.0517999999999965</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="2"/>
-        <v>-17.795400000000001</v>
+        <v>-20.957100000000004</v>
       </c>
       <c r="I11" s="2"/>
     </row>
@@ -10423,11 +10549,11 @@
       </c>
       <c r="G12" s="2">
         <f t="shared" si="1"/>
-        <v>-4.7280000000000015</v>
+        <v>0.9269999999999996</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="2"/>
-        <v>-17.191000000000003</v>
+        <v>-20.584000000000003</v>
       </c>
       <c r="I12" s="2"/>
     </row>
@@ -10456,11 +10582,11 @@
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>-2.7387000000000015</v>
+        <v>3.3916000000000039</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="2"/>
-        <v>-16.01019999999999</v>
+        <v>-19.612700000000011</v>
       </c>
       <c r="I13" s="2"/>
     </row>
@@ -10489,11 +10615,11 @@
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
-        <v>-0.24719999999999942</v>
+        <v>6.3420000000000059</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="2"/>
-        <v>-14.254799999999996</v>
+        <v>-18.0456</v>
       </c>
       <c r="I14" s="2"/>
     </row>
@@ -10522,11 +10648,11 @@
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>2.7464999999999975</v>
+        <v>9.7782000000000053</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="2"/>
-        <v>-11.926599999999993</v>
+        <v>-15.885100000000001</v>
       </c>
       <c r="I15" s="2"/>
     </row>
@@ -10555,11 +10681,11 @@
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
-        <v>6.2423999999999964</v>
+        <v>13.700200000000002</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="2"/>
-        <v>-9.027399999999993</v>
+        <v>-13.133600000000001</v>
       </c>
       <c r="I16" s="2"/>
     </row>
@@ -10588,11 +10714,11 @@
       </c>
       <c r="G17" s="2">
         <f t="shared" si="1"/>
-        <v>10.240499999999997</v>
+        <v>18.108000000000004</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="2"/>
-        <v>-5.5589999999999975</v>
+        <v>-9.7934999999999945</v>
       </c>
       <c r="I17" s="2"/>
     </row>
@@ -10621,11 +10747,11 @@
       </c>
       <c r="G18" s="2">
         <f t="shared" si="1"/>
-        <v>14.7408</v>
+        <v>23.001600000000003</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>-1.5232000000000028</v>
+        <v>-5.8672000000000111</v>
       </c>
       <c r="I18" s="2"/>
     </row>
@@ -10654,11 +10780,11 @@
       </c>
       <c r="G19" s="2">
         <f t="shared" si="1"/>
-        <v>19.743299999999998</v>
+        <v>28.381</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>3.0781999999999954</v>
+        <v>-1.3571000000000026</v>
       </c>
       <c r="I19" s="2"/>
     </row>
@@ -10687,11 +10813,11 @@
       </c>
       <c r="G20" s="2">
         <f t="shared" si="1"/>
-        <v>25.247999999999998</v>
+        <v>34.246200000000009</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>8.2433999999999941</v>
+        <v>3.7343999999999795</v>
       </c>
       <c r="I20" s="2"/>
     </row>
@@ -10720,11 +10846,11 @@
       </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
-        <v>31.254899999999999</v>
+        <v>40.597200000000008</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>13.970600000000005</v>
+        <v>9.4048999999999836</v>
       </c>
       <c r="I21" s="2"/>
     </row>
@@ -10753,11 +10879,11 @@
       </c>
       <c r="G22" s="2">
         <f t="shared" si="1"/>
-        <v>37.763999999999996</v>
+        <v>47.433999999999997</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>20.257999999999996</v>
+        <v>15.651999999999987</v>
       </c>
       <c r="I22" s="2"/>
     </row>
@@ -10786,11 +10912,11 @@
       </c>
       <c r="G23" s="2">
         <f t="shared" si="1"/>
-        <v>44.775299999999987</v>
+        <v>54.756599999999999</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="2"/>
-        <v>27.103800000000007</v>
+        <v>22.473299999999995</v>
       </c>
       <c r="I23" s="2"/>
     </row>
@@ -10819,11 +10945,11 @@
       </c>
       <c r="G24" s="2">
         <f t="shared" si="1"/>
-        <v>52.288799999999995</v>
+        <v>62.565000000000012</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="2"/>
-        <v>34.506200000000021</v>
+        <v>29.866399999999985</v>
       </c>
       <c r="I24" s="2"/>
     </row>
@@ -10852,11 +10978,11 @@
       </c>
       <c r="G25" s="2">
         <f t="shared" si="1"/>
-        <v>60.30449999999999</v>
+        <v>70.859200000000016</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="2"/>
-        <v>42.463400000000007</v>
+        <v>37.828899999999976</v>
       </c>
       <c r="I25" s="2"/>
     </row>
@@ -10885,11 +11011,11 @@
       </c>
       <c r="G26" s="2">
         <f t="shared" si="1"/>
-        <v>68.822400000000002</v>
+        <v>79.639200000000017</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="2"/>
-        <v>50.973600000000019</v>
+        <v>46.358400000000017</v>
       </c>
       <c r="I26" s="2"/>
     </row>
@@ -10918,11 +11044,11 @@
       </c>
       <c r="G27" s="2">
         <f t="shared" si="1"/>
-        <v>77.842500000000001</v>
+        <v>88.905000000000001</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="2"/>
-        <v>60.034999999999997</v>
+        <v>55.452499999999986</v>
       </c>
       <c r="I27" s="2"/>
     </row>
@@ -10951,11 +11077,11 @@
       </c>
       <c r="G28" s="2">
         <f t="shared" si="1"/>
-        <v>87.364799999999988</v>
+        <v>98.656600000000012</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="2"/>
-        <v>69.645800000000037</v>
+        <v>65.108799999999974</v>
       </c>
       <c r="I28" s="2"/>
     </row>
@@ -10984,11 +11110,11 @@
       </c>
       <c r="G29" s="2">
         <f t="shared" si="1"/>
-        <v>97.389299999999992</v>
+        <v>108.89400000000002</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="2"/>
-        <v>79.804200000000009</v>
+        <v>75.324899999999985</v>
       </c>
       <c r="I29" s="2"/>
     </row>
@@ -11017,11 +11143,11 @@
       </c>
       <c r="G30" s="2">
         <f t="shared" si="1"/>
-        <v>107.91599999999998</v>
+        <v>119.61720000000001</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="2"/>
-        <v>90.508400000000023</v>
+        <v>86.098399999999998</v>
       </c>
       <c r="I30" s="2"/>
     </row>
@@ -11050,11 +11176,11 @@
       </c>
       <c r="G31" s="2">
         <f t="shared" si="1"/>
-        <v>118.94489999999999</v>
+        <v>130.8262</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="2"/>
-        <v>101.75660000000002</v>
+        <v>97.426899999999932</v>
       </c>
       <c r="I31" s="2"/>
     </row>
@@ -11083,11 +11209,11 @@
       </c>
       <c r="G32" s="2">
         <f t="shared" si="1"/>
-        <v>130.476</v>
+        <v>142.52100000000002</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" si="2"/>
-        <v>113.547</v>
+        <v>109.30799999999999</v>
       </c>
       <c r="I32" s="2"/>
     </row>
@@ -11116,11 +11242,11 @@
       </c>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
-        <v>142.5093</v>
+        <v>154.70160000000004</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="2"/>
-        <v>125.87780000000004</v>
+        <v>121.73929999999999</v>
       </c>
       <c r="I33" s="2"/>
     </row>
@@ -11149,11 +11275,11 @@
       </c>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>155.04480000000001</v>
+        <v>167.36799999999999</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" si="2"/>
-        <v>138.74720000000002</v>
+        <v>134.7184</v>
       </c>
       <c r="I34" s="2"/>
     </row>
@@ -11182,11 +11308,11 @@
       </c>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>168.08250000000001</v>
+        <v>180.52019999999999</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="2"/>
-        <v>152.15340000000003</v>
+        <v>148.24289999999999</v>
       </c>
       <c r="I35" s="2"/>
     </row>
@@ -11215,11 +11341,11 @@
       </c>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>181.62239999999997</v>
+        <v>194.15819999999999</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" si="2"/>
-        <v>166.09459999999999</v>
+        <v>162.31039999999996</v>
       </c>
       <c r="I36" s="2"/>
     </row>
@@ -11248,11 +11374,11 @@
       </c>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
-        <v>195.66449999999998</v>
+        <v>208.28200000000001</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" si="2"/>
-        <v>180.56900000000005</v>
+        <v>176.91849999999999</v>
       </c>
       <c r="I37" s="2"/>
     </row>
@@ -11281,11 +11407,11 @@
       </c>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>210.2088</v>
+        <v>222.89160000000004</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" si="2"/>
-        <v>195.57479999999998</v>
+        <v>192.06479999999996</v>
       </c>
       <c r="I38" s="2"/>
     </row>
@@ -11314,11 +11440,11 @@
       </c>
       <c r="G39" s="2">
         <f t="shared" si="1"/>
-        <v>225.25530000000001</v>
+        <v>237.98700000000002</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="2"/>
-        <v>211.11020000000002</v>
+        <v>207.74689999999995</v>
       </c>
       <c r="I39" s="2"/>
     </row>
@@ -11347,11 +11473,11 @@
       </c>
       <c r="G40" s="2">
         <f t="shared" si="1"/>
-        <v>240.80399999999997</v>
+        <v>253.56820000000005</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" si="2"/>
-        <v>227.17340000000004</v>
+        <v>223.96239999999995</v>
       </c>
       <c r="I40" s="2"/>
     </row>
@@ -11380,11 +11506,11 @@
       </c>
       <c r="G41" s="2">
         <f t="shared" si="1"/>
-        <v>256.85489999999999</v>
+        <v>269.6352</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="2"/>
-        <v>243.76259999999999</v>
+        <v>240.70889999999997</v>
       </c>
       <c r="I41" s="2"/>
     </row>
@@ -11413,11 +11539,11 @@
       </c>
       <c r="G42" s="2">
         <f t="shared" si="1"/>
-        <v>273.40800000000002</v>
+        <v>286.18799999999999</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" si="2"/>
-        <v>260.87600000000003</v>
+        <v>257.98399999999992</v>
       </c>
       <c r="I42" s="2"/>
     </row>
@@ -11446,11 +11572,11 @@
       </c>
       <c r="G43" s="2">
         <f t="shared" si="1"/>
-        <v>290.4633</v>
+        <v>303.22660000000002</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="2"/>
-        <v>278.51180000000005</v>
+        <v>275.78530000000001</v>
       </c>
       <c r="I43" s="2"/>
     </row>
@@ -11479,11 +11605,11 @@
       </c>
       <c r="G44" s="2">
         <f t="shared" si="1"/>
-        <v>308.02079999999995</v>
+        <v>320.75099999999998</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="2"/>
-        <v>296.66820000000001</v>
+        <v>294.11039999999991</v>
       </c>
       <c r="I44" s="2"/>
     </row>
@@ -11512,11 +11638,11 @@
       </c>
       <c r="G45" s="2">
         <f t="shared" si="1"/>
-        <v>326.08049999999997</v>
+        <v>338.76119999999997</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="2"/>
-        <v>315.34340000000009</v>
+        <v>312.95689999999991</v>
       </c>
       <c r="I45" s="2"/>
     </row>
@@ -11545,11 +11671,11 @@
       </c>
       <c r="G46" s="2">
         <f t="shared" si="1"/>
-        <v>344.64239999999995</v>
+        <v>357.25720000000001</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" si="2"/>
-        <v>334.53560000000004</v>
+        <v>332.3223999999999</v>
       </c>
       <c r="I46" s="2"/>
     </row>
@@ -11578,11 +11704,11 @@
       </c>
       <c r="G47" s="2">
         <f t="shared" si="1"/>
-        <v>363.70650000000001</v>
+        <v>376.23900000000003</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="2"/>
-        <v>354.24300000000005</v>
+        <v>352.20449999999994</v>
       </c>
       <c r="I47" s="2"/>
     </row>
@@ -11611,11 +11737,11 @@
       </c>
       <c r="G48" s="2">
         <f t="shared" si="1"/>
-        <v>383.27279999999996</v>
+        <v>395.70660000000004</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="2"/>
-        <v>374.46380000000011</v>
+        <v>372.60079999999999</v>
       </c>
       <c r="I48" s="2"/>
     </row>
@@ -11644,11 +11770,11 @@
       </c>
       <c r="G49" s="2">
         <f t="shared" si="1"/>
-        <v>403.34129999999999</v>
+        <v>415.66</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" si="2"/>
-        <v>395.19620000000009</v>
+        <v>393.50889999999987</v>
       </c>
       <c r="I49" s="2"/>
     </row>
@@ -11677,11 +11803,11 @@
       </c>
       <c r="G50" s="2">
         <f t="shared" si="1"/>
-        <v>423.91200000000003</v>
+        <v>436.09920000000005</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" si="2"/>
-        <v>416.43840000000012</v>
+        <v>414.9264</v>
       </c>
       <c r="I50" s="2"/>
     </row>
@@ -11710,11 +11836,11 @@
       </c>
       <c r="G51" s="2">
         <f t="shared" si="1"/>
-        <v>444.98489999999993</v>
+        <v>457.02420000000001</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" si="2"/>
-        <v>438.18860000000006</v>
+        <v>436.85089999999997</v>
       </c>
       <c r="I51" s="2"/>
     </row>
@@ -11743,11 +11869,11 @@
       </c>
       <c r="G52" s="2">
         <f t="shared" si="1"/>
-        <v>466.56</v>
+        <v>478.435</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" si="2"/>
-        <v>460.44499999999999</v>
+        <v>459.28</v>
       </c>
       <c r="I52" s="2"/>
     </row>
@@ -11776,11 +11902,11 @@
       </c>
       <c r="G53" s="2">
         <f t="shared" si="1"/>
-        <v>488.63729999999998</v>
+        <v>500.33160000000004</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" si="2"/>
-        <v>483.20580000000001</v>
+        <v>482.21130000000005</v>
       </c>
       <c r="I53" s="2"/>
     </row>
@@ -11809,11 +11935,11 @@
       </c>
       <c r="G54" s="2">
         <f t="shared" si="1"/>
-        <v>511.21679999999992</v>
+        <v>522.71400000000006</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" si="2"/>
-        <v>506.46920000000006</v>
+        <v>505.64239999999995</v>
       </c>
       <c r="I54" s="2"/>
     </row>
@@ -11842,11 +11968,11 @@
       </c>
       <c r="G55" s="2">
         <f t="shared" si="1"/>
-        <v>534.29849999999999</v>
+        <v>545.58220000000006</v>
       </c>
       <c r="H55" s="2">
         <f t="shared" si="2"/>
-        <v>530.23340000000007</v>
+        <v>529.57090000000005</v>
       </c>
       <c r="I55" s="2"/>
     </row>
@@ -11875,11 +12001,11 @@
       </c>
       <c r="G56" s="2">
         <f t="shared" si="1"/>
-        <v>557.88239999999996</v>
+        <v>568.9362000000001</v>
       </c>
       <c r="H56" s="2">
         <f t="shared" si="2"/>
-        <v>554.49660000000006</v>
+        <v>553.99440000000004</v>
       </c>
       <c r="I56" s="2"/>
     </row>
@@ -11908,11 +12034,11 @@
       </c>
       <c r="G57" s="2">
         <f t="shared" si="1"/>
-        <v>581.96849999999995</v>
+        <v>592.77600000000007</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" si="2"/>
-        <v>579.25700000000006</v>
+        <v>578.91049999999996</v>
       </c>
       <c r="I57" s="2"/>
     </row>
@@ -11941,11 +12067,11 @@
       </c>
       <c r="G58" s="2">
         <f t="shared" si="1"/>
-        <v>606.55679999999995</v>
+        <v>617.10160000000008</v>
       </c>
       <c r="H58" s="2">
         <f t="shared" si="2"/>
-        <v>604.51280000000008</v>
+        <v>604.31680000000006</v>
       </c>
       <c r="I58" s="2"/>
     </row>
@@ -11974,11 +12100,11 @@
       </c>
       <c r="G59" s="2">
         <f t="shared" si="1"/>
-        <v>631.64729999999997</v>
+        <v>641.91300000000001</v>
       </c>
       <c r="H59" s="2">
         <f t="shared" si="2"/>
-        <v>630.26220000000012</v>
+        <v>630.21090000000004</v>
       </c>
       <c r="I59" s="2"/>
     </row>
@@ -12007,11 +12133,11 @@
       </c>
       <c r="G60" s="2">
         <f t="shared" si="1"/>
-        <v>657.24</v>
+        <v>667.21019999999999</v>
       </c>
       <c r="H60" s="2">
         <f t="shared" si="2"/>
-        <v>656.50340000000006</v>
+        <v>656.59039999999982</v>
       </c>
       <c r="I60" s="2"/>
     </row>
@@ -12040,11 +12166,11 @@
       </c>
       <c r="G61" s="2">
         <f t="shared" si="1"/>
-        <v>683.33489999999995</v>
+        <v>692.9932</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" si="2"/>
-        <v>683.2346</v>
+        <v>683.4529</v>
       </c>
       <c r="I61" s="2"/>
     </row>
@@ -12073,11 +12199,11 @@
       </c>
       <c r="G62" s="2">
         <f t="shared" si="1"/>
-        <v>709.9319999999999</v>
+        <v>719.26200000000006</v>
       </c>
       <c r="H62" s="2">
         <f t="shared" si="2"/>
-        <v>710.45400000000018</v>
+        <v>710.79599999999994</v>
       </c>
       <c r="I62" s="2"/>
     </row>
@@ -12106,11 +12232,11 @@
       </c>
       <c r="G63" s="2">
         <f t="shared" si="1"/>
-        <v>737.03129999999999</v>
+        <v>746.01660000000004</v>
       </c>
       <c r="H63" s="2">
         <f t="shared" si="2"/>
-        <v>738.15980000000013</v>
+        <v>738.6173</v>
       </c>
       <c r="I63" s="2"/>
     </row>
@@ -12139,11 +12265,11 @@
       </c>
       <c r="G64" s="2">
         <f t="shared" si="1"/>
-        <v>764.63279999999997</v>
+        <v>773.25700000000006</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" si="2"/>
-        <v>766.3502000000002</v>
+        <v>766.91439999999989</v>
       </c>
       <c r="I64" s="2"/>
     </row>
@@ -12172,11 +12298,11 @@
       </c>
       <c r="G65" s="2">
         <f t="shared" si="1"/>
-        <v>792.73649999999998</v>
+        <v>800.98320000000001</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" si="2"/>
-        <v>795.02339999999992</v>
+        <v>795.68489999999974</v>
       </c>
       <c r="I65" s="2"/>
     </row>
@@ -12205,11 +12331,11 @@
       </c>
       <c r="G66" s="2">
         <f t="shared" si="1"/>
-        <v>821.3424</v>
+        <v>829.1952</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" si="2"/>
-        <v>824.1776000000001</v>
+        <v>824.92639999999983</v>
       </c>
       <c r="I66" s="2"/>
     </row>
@@ -12237,12 +12363,12 @@
         <v>11.696969696969697</v>
       </c>
       <c r="G67" s="2">
-        <f t="shared" ref="G67:G130" si="6">0.2511*B67^2-3.2838*B67+3</f>
-        <v>850.45050000000003</v>
+        <f t="shared" ref="G67:G130" si="6">0.2429*B67^2-2.6363*B67+3</f>
+        <v>857.89300000000003</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" ref="H67:H130" si="7">-0.0003*B67^3+0.2972*B67^2-4.9611*B67+3</f>
-        <v>853.81100000000004</v>
+        <f t="shared" ref="H67:H130" si="7">-0.0004*B67^3+0.3111*B67^2-5.4294*B67+3</f>
+        <v>854.63650000000007</v>
       </c>
       <c r="I67" s="2"/>
     </row>
@@ -12258,7 +12384,7 @@
         <v>791</v>
       </c>
       <c r="D68" s="2">
-        <f t="shared" ref="D68:D130" si="8">C68-C67</f>
+        <f t="shared" ref="D68:D131" si="8">C68-C67</f>
         <v>16</v>
       </c>
       <c r="E68" s="2">
@@ -12271,11 +12397,11 @@
       </c>
       <c r="G68" s="2">
         <f t="shared" si="6"/>
-        <v>880.06079999999997</v>
+        <v>887.07659999999998</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" si="7"/>
-        <v>883.92179999999996</v>
+        <v>884.81279999999992</v>
       </c>
       <c r="I68" s="2"/>
     </row>
@@ -12304,11 +12430,11 @@
       </c>
       <c r="G69" s="2">
         <f t="shared" si="6"/>
-        <v>910.17329999999993</v>
+        <v>916.74600000000009</v>
       </c>
       <c r="H69" s="2">
         <f t="shared" si="7"/>
-        <v>914.50819999999999</v>
+        <v>915.4529</v>
       </c>
       <c r="I69" s="2"/>
     </row>
@@ -12337,11 +12463,11 @@
       </c>
       <c r="G70" s="2">
         <f t="shared" si="6"/>
-        <v>940.7879999999999</v>
+        <v>946.90120000000002</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" si="7"/>
-        <v>945.56839999999988</v>
+        <v>946.55439999999999</v>
       </c>
       <c r="I70" s="2"/>
     </row>
@@ -12370,11 +12496,11 @@
       </c>
       <c r="G71" s="2">
         <f t="shared" si="6"/>
-        <v>971.9049</v>
+        <v>977.54219999999987</v>
       </c>
       <c r="H71" s="2">
         <f t="shared" si="7"/>
-        <v>977.10059999999999</v>
+        <v>978.11489999999981</v>
       </c>
       <c r="I71" s="2"/>
     </row>
@@ -12403,11 +12529,11 @@
       </c>
       <c r="G72" s="2">
         <f t="shared" si="6"/>
-        <v>1003.5239999999999</v>
+        <v>1008.6690000000001</v>
       </c>
       <c r="H72" s="2">
         <f t="shared" si="7"/>
-        <v>1009.1030000000001</v>
+        <v>1010.1319999999998</v>
       </c>
       <c r="I72" s="2"/>
     </row>
@@ -12436,11 +12562,11 @@
       </c>
       <c r="G73" s="2">
         <f t="shared" si="6"/>
-        <v>1035.6453000000001</v>
+        <v>1040.2816</v>
       </c>
       <c r="H73" s="2">
         <f t="shared" si="7"/>
-        <v>1041.5738000000001</v>
+        <v>1042.6032999999998</v>
       </c>
       <c r="I73" s="2"/>
     </row>
@@ -12469,11 +12595,11 @@
       </c>
       <c r="G74" s="2">
         <f t="shared" si="6"/>
-        <v>1068.2687999999998</v>
+        <v>1072.3800000000001</v>
       </c>
       <c r="H74" s="2">
         <f t="shared" si="7"/>
-        <v>1074.5111999999999</v>
+        <v>1075.5264</v>
       </c>
       <c r="I74" s="2"/>
     </row>
@@ -12502,11 +12628,11 @@
       </c>
       <c r="G75" s="2">
         <f t="shared" si="6"/>
-        <v>1101.3944999999999</v>
+        <v>1104.9641999999999</v>
       </c>
       <c r="H75" s="2">
         <f t="shared" si="7"/>
-        <v>1107.9134000000001</v>
+        <v>1108.8988999999999</v>
       </c>
       <c r="I75" s="2"/>
     </row>
@@ -12535,11 +12661,11 @@
       </c>
       <c r="G76" s="2">
         <f t="shared" si="6"/>
-        <v>1135.0224000000001</v>
+        <v>1138.0342000000001</v>
       </c>
       <c r="H76" s="2">
         <f t="shared" si="7"/>
-        <v>1141.7786000000001</v>
+        <v>1142.7184</v>
       </c>
       <c r="I76" s="2"/>
     </row>
@@ -12568,11 +12694,11 @@
       </c>
       <c r="G77" s="2">
         <f t="shared" si="6"/>
-        <v>1169.1524999999999</v>
+        <v>1171.5899999999999</v>
       </c>
       <c r="H77" s="2">
         <f t="shared" si="7"/>
-        <v>1176.105</v>
+        <v>1176.9825000000001</v>
       </c>
       <c r="I77" s="2"/>
     </row>
@@ -12601,11 +12727,11 @@
       </c>
       <c r="G78" s="2">
         <f t="shared" si="6"/>
-        <v>1203.7847999999999</v>
+        <v>1205.6316000000002</v>
       </c>
       <c r="H78" s="2">
         <f t="shared" si="7"/>
-        <v>1210.8908000000001</v>
+        <v>1211.6887999999999</v>
       </c>
       <c r="I78" s="2"/>
     </row>
@@ -12634,11 +12760,11 @@
       </c>
       <c r="G79" s="2">
         <f t="shared" si="6"/>
-        <v>1238.9193</v>
+        <v>1240.1590000000001</v>
       </c>
       <c r="H79" s="2">
         <f t="shared" si="7"/>
-        <v>1246.1342000000002</v>
+        <v>1246.8348999999998</v>
       </c>
       <c r="I79" s="2"/>
     </row>
@@ -12667,11 +12793,11 @@
       </c>
       <c r="G80" s="2">
         <f t="shared" si="6"/>
-        <v>1274.556</v>
+        <v>1275.1722</v>
       </c>
       <c r="H80" s="2">
         <f t="shared" si="7"/>
-        <v>1281.8334</v>
+        <v>1282.4184</v>
       </c>
       <c r="I80" s="2"/>
     </row>
@@ -12700,11 +12826,11 @@
       </c>
       <c r="G81" s="2">
         <f t="shared" si="6"/>
-        <v>1310.6949</v>
+        <v>1310.6712000000002</v>
       </c>
       <c r="H81" s="2">
         <f t="shared" si="7"/>
-        <v>1317.9866000000002</v>
+        <v>1318.4368999999999</v>
       </c>
       <c r="I81" s="2"/>
     </row>
@@ -12733,11 +12859,11 @@
       </c>
       <c r="G82" s="2">
         <f t="shared" si="6"/>
-        <v>1347.336</v>
+        <v>1346.6559999999999</v>
       </c>
       <c r="H82" s="2">
         <f t="shared" si="7"/>
-        <v>1354.5920000000001</v>
+        <v>1354.8879999999999</v>
       </c>
       <c r="I82" s="2"/>
     </row>
@@ -12766,11 +12892,11 @@
       </c>
       <c r="G83" s="2">
         <f t="shared" si="6"/>
-        <v>1384.4793</v>
+        <v>1383.1266000000001</v>
       </c>
       <c r="H83" s="2">
         <f t="shared" si="7"/>
-        <v>1391.6478000000002</v>
+        <v>1391.7692999999999</v>
       </c>
       <c r="I83" s="2"/>
     </row>
@@ -12799,11 +12925,11 @@
       </c>
       <c r="G84" s="2">
         <f t="shared" si="6"/>
-        <v>1422.1247999999998</v>
+        <v>1420.0830000000001</v>
       </c>
       <c r="H84" s="2">
         <f t="shared" si="7"/>
-        <v>1429.1522</v>
+        <v>1429.0784000000001</v>
       </c>
       <c r="I84" s="2"/>
     </row>
@@ -12832,11 +12958,11 @@
       </c>
       <c r="G85" s="2">
         <f t="shared" si="6"/>
-        <v>1460.2725</v>
+        <v>1457.5252</v>
       </c>
       <c r="H85" s="2">
         <f t="shared" si="7"/>
-        <v>1467.1034</v>
+        <v>1466.8128999999999</v>
       </c>
       <c r="I85" s="2"/>
     </row>
@@ -12865,11 +12991,11 @@
       </c>
       <c r="G86" s="2">
         <f t="shared" si="6"/>
-        <v>1498.9223999999999</v>
+        <v>1495.4531999999999</v>
       </c>
       <c r="H86" s="2">
         <f t="shared" si="7"/>
-        <v>1505.4996000000001</v>
+        <v>1504.9703999999999</v>
       </c>
       <c r="I86" s="2"/>
     </row>
@@ -12898,11 +13024,11 @@
       </c>
       <c r="G87" s="2">
         <f t="shared" si="6"/>
-        <v>1538.0744999999999</v>
+        <v>1533.8670000000002</v>
       </c>
       <c r="H87" s="2">
         <f t="shared" si="7"/>
-        <v>1544.3389999999999</v>
+        <v>1543.5484999999996</v>
       </c>
       <c r="I87" s="2"/>
     </row>
@@ -12931,11 +13057,11 @@
       </c>
       <c r="G88" s="2">
         <f t="shared" si="6"/>
-        <v>1577.7287999999999</v>
+        <v>1572.7665999999999</v>
       </c>
       <c r="H88" s="2">
         <f t="shared" si="7"/>
-        <v>1583.6198000000002</v>
+        <v>1582.5447999999999</v>
       </c>
       <c r="I88" s="2"/>
     </row>
@@ -12964,11 +13090,11 @@
       </c>
       <c r="G89" s="2">
         <f t="shared" si="6"/>
-        <v>1617.8852999999999</v>
+        <v>1612.152</v>
       </c>
       <c r="H89" s="2">
         <f t="shared" si="7"/>
-        <v>1623.3401999999999</v>
+        <v>1621.9568999999999</v>
       </c>
       <c r="I89" s="2"/>
     </row>
@@ -12997,11 +13123,11 @@
       </c>
       <c r="G90" s="2">
         <f t="shared" si="6"/>
-        <v>1658.5439999999999</v>
+        <v>1652.0232000000001</v>
       </c>
       <c r="H90" s="2">
         <f t="shared" si="7"/>
-        <v>1663.4984000000002</v>
+        <v>1661.7823999999998</v>
       </c>
       <c r="I90" s="2"/>
     </row>
@@ -13030,11 +13156,11 @@
       </c>
       <c r="G91" s="2">
         <f t="shared" si="6"/>
-        <v>1699.7049</v>
+        <v>1692.3802000000001</v>
       </c>
       <c r="H91" s="2">
         <f t="shared" si="7"/>
-        <v>1704.0926000000002</v>
+        <v>1702.0188999999998</v>
       </c>
       <c r="I91" s="2"/>
     </row>
@@ -13063,11 +13189,11 @@
       </c>
       <c r="G92" s="2">
         <f t="shared" si="6"/>
-        <v>1741.3679999999999</v>
+        <v>1733.223</v>
       </c>
       <c r="H92" s="2">
         <f t="shared" si="7"/>
-        <v>1745.1210000000003</v>
+        <v>1742.664</v>
       </c>
       <c r="I92" t="s">
         <v>7</v>
@@ -13098,11 +13224,11 @@
       </c>
       <c r="G93" s="2">
         <f t="shared" si="6"/>
-        <v>1783.5333000000001</v>
+        <v>1774.5516</v>
       </c>
       <c r="H93" s="2">
         <f t="shared" si="7"/>
-        <v>1786.5818000000002</v>
+        <v>1783.7152999999996</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.4">
@@ -13130,11 +13256,11 @@
       </c>
       <c r="G94" s="2">
         <f t="shared" si="6"/>
-        <v>1826.2007999999998</v>
+        <v>1816.366</v>
       </c>
       <c r="H94" s="2">
         <f t="shared" si="7"/>
-        <v>1828.4732000000001</v>
+        <v>1825.1704</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.4">
@@ -13162,11 +13288,11 @@
       </c>
       <c r="G95" s="2">
         <f t="shared" si="6"/>
-        <v>1869.3705</v>
+        <v>1858.6661999999999</v>
       </c>
       <c r="H95" s="2">
         <f t="shared" si="7"/>
-        <v>1870.7934000000002</v>
+        <v>1867.0268999999998</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.4">
@@ -13194,11 +13320,11 @@
       </c>
       <c r="G96" s="2">
         <f t="shared" si="6"/>
-        <v>1913.0423999999998</v>
+        <v>1901.4521999999999</v>
       </c>
       <c r="H96" s="2">
         <f t="shared" si="7"/>
-        <v>1913.5406</v>
+        <v>1909.2823999999996</v>
       </c>
       <c r="I96" t="s">
         <v>6</v>
@@ -13229,11 +13355,11 @@
       </c>
       <c r="G97" s="2">
         <f t="shared" si="6"/>
-        <v>1957.2164999999998</v>
+        <v>1944.7240000000002</v>
       </c>
       <c r="H97" s="2">
         <f t="shared" si="7"/>
-        <v>1956.713</v>
+        <v>1951.9344999999998</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.4">
@@ -13261,11 +13387,11 @@
       </c>
       <c r="G98" s="2">
         <f t="shared" si="6"/>
-        <v>2001.8928000000001</v>
+        <v>1988.4816000000001</v>
       </c>
       <c r="H98" s="2">
         <f t="shared" si="7"/>
-        <v>2000.3088000000005</v>
+        <v>1994.9807999999998</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.4">
@@ -13293,11 +13419,11 @@
       </c>
       <c r="G99" s="2">
         <f t="shared" si="6"/>
-        <v>2047.0712999999996</v>
+        <v>2032.7250000000001</v>
       </c>
       <c r="H99" s="2">
         <f t="shared" si="7"/>
-        <v>2044.3262000000002</v>
+        <v>2038.4188999999997</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.4">
@@ -13325,11 +13451,11 @@
       </c>
       <c r="G100" s="2">
         <f t="shared" si="6"/>
-        <v>2092.752</v>
+        <v>2077.4542000000001</v>
       </c>
       <c r="H100" s="2">
         <f t="shared" si="7"/>
-        <v>2088.7634000000003</v>
+        <v>2082.2464</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.4">
@@ -13357,11 +13483,11 @@
       </c>
       <c r="G101" s="2">
         <f t="shared" si="6"/>
-        <v>2138.9348999999997</v>
+        <v>2122.6692000000003</v>
       </c>
       <c r="H101" s="2">
         <f t="shared" si="7"/>
-        <v>2133.6186000000002</v>
+        <v>2126.4609</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.4">
@@ -13389,11 +13515,11 @@
       </c>
       <c r="G102" s="2">
         <f t="shared" si="6"/>
-        <v>2185.62</v>
+        <v>2168.37</v>
       </c>
       <c r="H102" s="2">
         <f t="shared" si="7"/>
-        <v>2178.89</v>
+        <v>2171.06</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.4">
@@ -13421,11 +13547,11 @@
       </c>
       <c r="G103" s="2">
         <f t="shared" si="6"/>
-        <v>2232.8072999999999</v>
+        <v>2214.5565999999999</v>
       </c>
       <c r="H103" s="2">
         <f t="shared" si="7"/>
-        <v>2224.5758000000001</v>
+        <v>2216.0412999999994</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.4">
@@ -13453,11 +13579,11 @@
       </c>
       <c r="G104" s="2">
         <f t="shared" si="6"/>
-        <v>2280.4967999999999</v>
+        <v>2261.2290000000003</v>
       </c>
       <c r="H104" s="2">
         <f t="shared" si="7"/>
-        <v>2270.6741999999999</v>
+        <v>2261.4023999999999</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.4">
@@ -13485,11 +13611,11 @@
       </c>
       <c r="G105" s="2">
         <f t="shared" si="6"/>
-        <v>2328.6884999999997</v>
+        <v>2308.3872000000001</v>
       </c>
       <c r="H105" s="2">
         <f t="shared" si="7"/>
-        <v>2317.1834000000003</v>
+        <v>2307.1408999999999</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.4">
@@ -13517,11 +13643,11 @@
       </c>
       <c r="G106" s="2">
         <f t="shared" si="6"/>
-        <v>2377.3824</v>
+        <v>2356.0311999999999</v>
       </c>
       <c r="H106" s="2">
         <f t="shared" si="7"/>
-        <v>2364.1016000000004</v>
+        <v>2353.2543999999998</v>
       </c>
       <c r="I106" t="s">
         <v>9</v>
@@ -13552,11 +13678,11 @@
       </c>
       <c r="G107" s="2">
         <f t="shared" si="6"/>
-        <v>2426.5785000000001</v>
+        <v>2404.1610000000001</v>
       </c>
       <c r="H107" s="2">
         <f t="shared" si="7"/>
-        <v>2411.4270000000001</v>
+        <v>2399.7404999999999</v>
       </c>
       <c r="I107" t="s">
         <v>8</v>
@@ -13587,11 +13713,11 @@
       </c>
       <c r="G108" s="2">
         <f t="shared" si="6"/>
-        <v>2476.2767999999996</v>
+        <v>2452.7766000000001</v>
       </c>
       <c r="H108" s="2">
         <f t="shared" si="7"/>
-        <v>2459.1578000000004</v>
+        <v>2446.5968000000003</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.4">
@@ -13619,11 +13745,11 @@
       </c>
       <c r="G109" s="2">
         <f t="shared" si="6"/>
-        <v>2526.4773</v>
+        <v>2501.8780000000002</v>
       </c>
       <c r="H109" s="2">
         <f t="shared" si="7"/>
-        <v>2507.2921999999999</v>
+        <v>2493.8209000000002</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.4">
@@ -13651,11 +13777,11 @@
       </c>
       <c r="G110" s="2">
         <f t="shared" si="6"/>
-        <v>2577.1799999999998</v>
+        <v>2551.4652000000001</v>
       </c>
       <c r="H110" s="2">
         <f t="shared" si="7"/>
-        <v>2555.8284000000003</v>
+        <v>2541.4104000000002</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.4">
@@ -13683,11 +13809,11 @@
       </c>
       <c r="G111" s="2">
         <f t="shared" si="6"/>
-        <v>2628.3848999999996</v>
+        <v>2601.5382000000004</v>
       </c>
       <c r="H111" s="2">
         <f t="shared" si="7"/>
-        <v>2604.7646000000004</v>
+        <v>2589.3628999999996</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.4">
@@ -13715,11 +13841,11 @@
       </c>
       <c r="G112" s="2">
         <f t="shared" si="6"/>
-        <v>2680.0920000000001</v>
+        <v>2652.0970000000002</v>
       </c>
       <c r="H112" s="2">
         <f t="shared" si="7"/>
-        <v>2654.0990000000006</v>
+        <v>2637.6759999999999</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.4">
@@ -13747,11 +13873,11 @@
       </c>
       <c r="G113" s="2">
         <f t="shared" si="6"/>
-        <v>2732.3013000000001</v>
+        <v>2703.1415999999999</v>
       </c>
       <c r="H113" s="2">
         <f t="shared" si="7"/>
-        <v>2703.8298000000004</v>
+        <v>2686.3472999999999</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.4">
@@ -13779,11 +13905,11 @@
       </c>
       <c r="G114" s="2">
         <f t="shared" si="6"/>
-        <v>2785.0127999999995</v>
+        <v>2754.672</v>
       </c>
       <c r="H114" s="2">
         <f t="shared" si="7"/>
-        <v>2753.9552000000003</v>
+        <v>2735.3744000000002</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.4">
@@ -13811,11 +13937,11 @@
       </c>
       <c r="G115" s="2">
         <f t="shared" si="6"/>
-        <v>2838.2265000000002</v>
+        <v>2806.6882000000001</v>
       </c>
       <c r="H115" s="2">
         <f t="shared" si="7"/>
-        <v>2804.4734000000003</v>
+        <v>2784.7548999999999</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.4">
@@ -13843,11 +13969,11 @@
       </c>
       <c r="G116" s="2">
         <f t="shared" si="6"/>
-        <v>2891.9423999999999</v>
+        <v>2859.1902</v>
       </c>
       <c r="H116" s="2">
         <f t="shared" si="7"/>
-        <v>2855.3826000000004</v>
+        <v>2834.4863999999998</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.4">
@@ -13875,11 +14001,11 @@
       </c>
       <c r="G117" s="2">
         <f t="shared" si="6"/>
-        <v>2946.1604999999995</v>
+        <v>2912.1779999999999</v>
       </c>
       <c r="H117" s="2">
         <f t="shared" si="7"/>
-        <v>2906.6810000000005</v>
+        <v>2884.5664999999999</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.4">
@@ -13907,11 +14033,11 @@
       </c>
       <c r="G118" s="2">
         <f t="shared" si="6"/>
-        <v>3000.8807999999999</v>
+        <v>2965.6516000000001</v>
       </c>
       <c r="H118" s="2">
         <f t="shared" si="7"/>
-        <v>2958.3668000000007</v>
+        <v>2934.9927999999991</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.4">
@@ -13939,11 +14065,11 @@
       </c>
       <c r="G119" s="2">
         <f t="shared" si="6"/>
-        <v>3056.1032999999998</v>
+        <v>3019.6110000000003</v>
       </c>
       <c r="H119" s="2">
         <f t="shared" si="7"/>
-        <v>3010.4382000000005</v>
+        <v>2985.7628999999997</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.4">
@@ -13971,11 +14097,11 @@
       </c>
       <c r="G120" s="2">
         <f t="shared" si="6"/>
-        <v>3111.8279999999995</v>
+        <v>3074.0562</v>
       </c>
       <c r="H120" s="2">
         <f t="shared" si="7"/>
-        <v>3062.8934000000004</v>
+        <v>3036.8743999999997</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.4">
@@ -14003,11 +14129,11 @@
       </c>
       <c r="G121" s="2">
         <f t="shared" si="6"/>
-        <v>3168.0549000000001</v>
+        <v>3128.9872</v>
       </c>
       <c r="H121" s="2">
         <f t="shared" si="7"/>
-        <v>3115.7305999999999</v>
+        <v>3088.3248999999996</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.4">
@@ -14035,11 +14161,11 @@
       </c>
       <c r="G122" s="2">
         <f t="shared" si="6"/>
-        <v>3224.7839999999997</v>
+        <v>3184.4040000000005</v>
       </c>
       <c r="H122" s="2">
         <f t="shared" si="7"/>
-        <v>3168.9480000000003</v>
+        <v>3140.1120000000001</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.4">
@@ -14067,11 +14193,11 @@
       </c>
       <c r="G123" s="2">
         <f t="shared" si="6"/>
-        <v>3282.0153</v>
+        <v>3240.3066000000003</v>
       </c>
       <c r="H123" s="2">
         <f t="shared" si="7"/>
-        <v>3222.5438000000008</v>
+        <v>3192.2332999999999</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.4">
@@ -14099,11 +14225,11 @@
       </c>
       <c r="G124" s="2">
         <f t="shared" si="6"/>
-        <v>3339.7487999999998</v>
+        <v>3296.6950000000002</v>
       </c>
       <c r="H124" s="2">
         <f t="shared" si="7"/>
-        <v>3276.5162000000005</v>
+        <v>3244.6864000000005</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.4">
@@ -14131,11 +14257,11 @@
       </c>
       <c r="G125" s="2">
         <f t="shared" si="6"/>
-        <v>3397.9844999999996</v>
+        <v>3353.5691999999999</v>
       </c>
       <c r="H125" s="2">
         <f t="shared" si="7"/>
-        <v>3330.8634000000006</v>
+        <v>3297.4688999999989</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.4">
@@ -14163,11 +14289,11 @@
       </c>
       <c r="G126" s="2">
         <f t="shared" si="6"/>
-        <v>3456.7223999999997</v>
+        <v>3410.9292000000005</v>
       </c>
       <c r="H126" s="2">
         <f t="shared" si="7"/>
-        <v>3385.5836000000008</v>
+        <v>3350.5783999999999</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.4">
@@ -14195,11 +14321,11 @@
       </c>
       <c r="G127" s="2">
         <f t="shared" si="6"/>
-        <v>3515.9625000000001</v>
+        <v>3468.7750000000001</v>
       </c>
       <c r="H127" s="2">
         <f t="shared" si="7"/>
-        <v>3440.6750000000002</v>
+        <v>3404.0124999999998</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.4">
@@ -14211,27 +14337,27 @@
         <v>126</v>
       </c>
       <c r="C128" s="3">
-        <v>3561</v>
+        <v>3533</v>
       </c>
       <c r="D128" s="2">
         <f t="shared" si="8"/>
-        <v>54</v>
+        <v>26</v>
       </c>
       <c r="E128" s="2">
         <f t="shared" si="9"/>
-        <v>53.142857142857146</v>
+        <v>49.142857142857146</v>
       </c>
       <c r="F128" s="2">
         <f>SUM($D$2:$D128)/COUNT($D$2:$D128)</f>
-        <v>28.015748031496063</v>
+        <v>27.795275590551181</v>
       </c>
       <c r="G128" s="2">
         <f t="shared" si="6"/>
-        <v>3575.7048</v>
+        <v>3527.1066000000001</v>
       </c>
       <c r="H128" s="2">
         <f t="shared" si="7"/>
-        <v>3496.1358</v>
+        <v>3457.7687999999998</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.4">
@@ -14243,27 +14369,27 @@
         <v>127</v>
       </c>
       <c r="C129" s="3">
-        <v>3609</v>
+        <v>3601</v>
       </c>
       <c r="D129" s="2">
         <f t="shared" si="8"/>
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="E129" s="2">
         <f t="shared" si="9"/>
-        <v>55</v>
+        <v>53.857142857142854</v>
       </c>
       <c r="F129" s="2">
         <f>SUM($D$2:$D129)/COUNT($D$2:$D129)</f>
-        <v>28.171875</v>
+        <v>28.109375</v>
       </c>
       <c r="G129" s="2">
         <f t="shared" si="6"/>
-        <v>3635.9493000000002</v>
+        <v>3585.924</v>
       </c>
       <c r="H129" s="2">
         <f t="shared" si="7"/>
-        <v>3551.9642000000003</v>
+        <v>3511.8448999999991</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.4">
@@ -14275,27 +14401,27 @@
         <v>128</v>
       </c>
       <c r="C130" s="3">
-        <v>3632</v>
+        <v>3636</v>
       </c>
       <c r="D130" s="2">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="E130" s="2">
         <f t="shared" si="9"/>
-        <v>51.571428571428569</v>
+        <v>52.142857142857146</v>
       </c>
       <c r="F130" s="2">
         <f>SUM($D$2:$D130)/COUNT($D$2:$D130)</f>
-        <v>28.131782945736433</v>
+        <v>28.162790697674417</v>
       </c>
       <c r="G130" s="2">
         <f t="shared" si="6"/>
-        <v>3696.6959999999999</v>
+        <v>3645.2272000000003</v>
       </c>
       <c r="H130" s="2">
         <f t="shared" si="7"/>
-        <v>3608.1584000000003</v>
+        <v>3566.2383999999993</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.4">
@@ -14306,14 +14432,28 @@
         <f t="shared" ref="B131:B176" si="10">B130+1</f>
         <v>129</v>
       </c>
-      <c r="E131" s="2"/>
+      <c r="C131" s="3">
+        <v>3705</v>
+      </c>
+      <c r="D131" s="2">
+        <f t="shared" si="8"/>
+        <v>69</v>
+      </c>
+      <c r="E131" s="2">
+        <f t="shared" si="9"/>
+        <v>49.571428571428569</v>
+      </c>
+      <c r="F131" s="2">
+        <f>SUM($D$2:$D131)/COUNT($D$2:$D131)</f>
+        <v>28.476923076923075</v>
+      </c>
       <c r="G131" s="2">
-        <f t="shared" ref="G131:G176" si="11">0.2511*B131^2-3.2838*B131+3</f>
-        <v>3757.9448999999995</v>
+        <f t="shared" ref="G131:G176" si="11">0.2429*B131^2-2.6363*B131+3</f>
+        <v>3705.0162</v>
       </c>
       <c r="H131" s="2">
-        <f t="shared" ref="H131:H176" si="12">-0.0003*B131^3+0.2972*B131^2-4.9611*B131+3</f>
-        <v>3664.7166000000007</v>
+        <f t="shared" ref="H131:H176" si="12">-0.0004*B131^3+0.3111*B131^2-5.4294*B131+3</f>
+        <v>3620.9468999999999</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.4">
@@ -14324,14 +14464,28 @@
         <f t="shared" si="10"/>
         <v>130</v>
       </c>
-      <c r="E132" s="2"/>
+      <c r="C132" s="3">
+        <v>3723</v>
+      </c>
+      <c r="D132" s="2">
+        <f t="shared" ref="D132:D138" si="13">C132-C131</f>
+        <v>18</v>
+      </c>
+      <c r="E132" s="2">
+        <f t="shared" si="9"/>
+        <v>51.571428571428569</v>
+      </c>
+      <c r="F132" s="2">
+        <f>SUM($D$2:$D132)/COUNT($D$2:$D132)</f>
+        <v>28.396946564885496</v>
+      </c>
       <c r="G132" s="2">
         <f t="shared" si="11"/>
-        <v>3819.6959999999999</v>
+        <v>3765.2910000000002</v>
       </c>
       <c r="H132" s="2">
         <f t="shared" si="12"/>
-        <v>3721.6369999999997</v>
+        <v>3675.9679999999998</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.4">
@@ -14342,14 +14496,28 @@
         <f t="shared" si="10"/>
         <v>131</v>
       </c>
-      <c r="E133" s="2"/>
+      <c r="C133" s="3">
+        <v>3806</v>
+      </c>
+      <c r="D133" s="2">
+        <f t="shared" si="13"/>
+        <v>83</v>
+      </c>
+      <c r="E133" s="2">
+        <f t="shared" si="9"/>
+        <v>52</v>
+      </c>
+      <c r="F133" s="2">
+        <f>SUM($D$2:$D133)/COUNT($D$2:$D133)</f>
+        <v>28.810606060606062</v>
+      </c>
       <c r="G133" s="2">
         <f t="shared" si="11"/>
-        <v>3881.9492999999998</v>
+        <v>3826.0515999999998</v>
       </c>
       <c r="H133" s="2">
         <f t="shared" si="12"/>
-        <v>3778.9178000000002</v>
+        <v>3731.2992999999997</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.4">
@@ -14360,14 +14528,28 @@
         <f t="shared" si="10"/>
         <v>132</v>
       </c>
-      <c r="E134" s="2"/>
+      <c r="C134" s="3">
+        <v>3822</v>
+      </c>
+      <c r="D134" s="2">
+        <f t="shared" si="13"/>
+        <v>16</v>
+      </c>
+      <c r="E134" s="2">
+        <f t="shared" si="9"/>
+        <v>45</v>
+      </c>
+      <c r="F134" s="2">
+        <f>SUM($D$2:$D134)/COUNT($D$2:$D134)</f>
+        <v>28.714285714285715</v>
+      </c>
       <c r="G134" s="2">
         <f t="shared" si="11"/>
-        <v>3944.7048</v>
+        <v>3887.2980000000002</v>
       </c>
       <c r="H134" s="2">
         <f t="shared" si="12"/>
-        <v>3836.5572000000002</v>
+        <v>3786.9383999999991</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.4">
@@ -14378,14 +14560,28 @@
         <f t="shared" si="10"/>
         <v>133</v>
       </c>
-      <c r="E135" s="2"/>
+      <c r="C135" s="3">
+        <v>3873</v>
+      </c>
+      <c r="D135" s="2">
+        <f t="shared" si="13"/>
+        <v>51</v>
+      </c>
+      <c r="E135" s="2">
+        <f t="shared" si="9"/>
+        <v>48.571428571428569</v>
+      </c>
+      <c r="F135" s="2">
+        <f>SUM($D$2:$D135)/COUNT($D$2:$D135)</f>
+        <v>28.880597014925375</v>
+      </c>
       <c r="G135" s="2">
         <f t="shared" si="11"/>
-        <v>4007.9624999999996</v>
+        <v>3949.0301999999997</v>
       </c>
       <c r="H135" s="2">
         <f t="shared" si="12"/>
-        <v>3894.5534000000011</v>
+        <v>3842.8828999999996</v>
       </c>
       <c r="I135" t="s">
         <v>10</v>
@@ -14399,14 +14595,28 @@
         <f t="shared" si="10"/>
         <v>134</v>
       </c>
-      <c r="E136" s="2"/>
+      <c r="C136" s="3">
+        <v>3908</v>
+      </c>
+      <c r="D136" s="2">
+        <f t="shared" si="13"/>
+        <v>35</v>
+      </c>
+      <c r="E136" s="2">
+        <f t="shared" si="9"/>
+        <v>43.857142857142854</v>
+      </c>
+      <c r="F136" s="2">
+        <f>SUM($D$2:$D136)/COUNT($D$2:$D136)</f>
+        <v>28.925925925925927</v>
+      </c>
       <c r="G136" s="2">
         <f t="shared" si="11"/>
-        <v>4071.7223999999997</v>
+        <v>4011.2482000000005</v>
       </c>
       <c r="H136" s="2">
         <f t="shared" si="12"/>
-        <v>3952.9046000000008</v>
+        <v>3899.1304</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.4">
@@ -14417,14 +14627,28 @@
         <f t="shared" si="10"/>
         <v>135</v>
       </c>
-      <c r="E137" s="2"/>
+      <c r="C137" s="3">
+        <v>3961</v>
+      </c>
+      <c r="D137" s="2">
+        <f t="shared" si="13"/>
+        <v>53</v>
+      </c>
+      <c r="E137" s="2">
+        <f t="shared" si="9"/>
+        <v>46.428571428571431</v>
+      </c>
+      <c r="F137" s="2">
+        <f>SUM($D$2:$D137)/COUNT($D$2:$D137)</f>
+        <v>29.102941176470587</v>
+      </c>
       <c r="G137" s="2">
         <f t="shared" si="11"/>
-        <v>4135.9844999999996</v>
+        <v>4073.9520000000002</v>
       </c>
       <c r="H137" s="2">
         <f t="shared" si="12"/>
-        <v>4011.6089999999999</v>
+        <v>3955.6784999999991</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.4">
@@ -14435,14 +14659,28 @@
         <f t="shared" si="10"/>
         <v>136</v>
       </c>
-      <c r="E138" s="2"/>
+      <c r="C138" s="3">
+        <v>4023</v>
+      </c>
+      <c r="D138" s="2">
+        <f t="shared" si="13"/>
+        <v>62</v>
+      </c>
+      <c r="E138" s="2">
+        <f t="shared" ref="E138" si="14">(C138-C131)/7</f>
+        <v>45.428571428571431</v>
+      </c>
+      <c r="F138" s="2">
+        <f>SUM($D$2:$D138)/COUNT($D$2:$D138)</f>
+        <v>29.343065693430656</v>
+      </c>
       <c r="G138" s="2">
         <f t="shared" si="11"/>
-        <v>4200.7487999999994</v>
+        <v>4137.1415999999999</v>
       </c>
       <c r="H138" s="2">
         <f t="shared" si="12"/>
-        <v>4070.6647999999996</v>
+        <v>4012.5248000000001</v>
       </c>
       <c r="I138" t="s">
         <v>11</v>
@@ -14459,11 +14697,11 @@
       <c r="E139" s="2"/>
       <c r="G139" s="2">
         <f t="shared" si="11"/>
-        <v>4266.0152999999991</v>
+        <v>4200.817</v>
       </c>
       <c r="H139" s="2">
         <f t="shared" si="12"/>
-        <v>4130.070200000001</v>
+        <v>4069.6668999999993</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.4">
@@ -14477,11 +14715,11 @@
       <c r="E140" s="2"/>
       <c r="G140" s="2">
         <f t="shared" si="11"/>
-        <v>4331.7840000000006</v>
+        <v>4264.9781999999996</v>
       </c>
       <c r="H140" s="2">
         <f t="shared" si="12"/>
-        <v>4189.8234000000002</v>
+        <v>4127.1023999999998</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.4">
@@ -14495,11 +14733,11 @@
       <c r="E141" s="2"/>
       <c r="G141" s="2">
         <f t="shared" si="11"/>
-        <v>4398.0549000000001</v>
+        <v>4329.6251999999995</v>
       </c>
       <c r="H141" s="2">
         <f t="shared" si="12"/>
-        <v>4249.9226000000008</v>
+        <v>4184.8288999999995</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.4">
@@ -14513,11 +14751,11 @@
       <c r="E142" s="2"/>
       <c r="G142" s="2">
         <f t="shared" si="11"/>
-        <v>4464.8279999999995</v>
+        <v>4394.7579999999998</v>
       </c>
       <c r="H142" s="2">
         <f t="shared" si="12"/>
-        <v>4310.3660000000009</v>
+        <v>4242.8439999999991</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.4">
@@ -14531,11 +14769,11 @@
       <c r="E143" s="2"/>
       <c r="G143" s="2">
         <f t="shared" si="11"/>
-        <v>4532.1032999999998</v>
+        <v>4460.3765999999996</v>
       </c>
       <c r="H143" s="2">
         <f t="shared" si="12"/>
-        <v>4371.1518000000005</v>
+        <v>4301.1452999999992</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.4">
@@ -14549,14 +14787,14 @@
       <c r="E144" s="2"/>
       <c r="G144" s="2">
         <f t="shared" si="11"/>
-        <v>4599.8807999999999</v>
+        <v>4526.4810000000007</v>
       </c>
       <c r="H144" s="2">
         <f t="shared" si="12"/>
-        <v>4432.2782000000007</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4359.7303999999995</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A145" s="1">
         <v>43768</v>
       </c>
@@ -14567,14 +14805,14 @@
       <c r="E145" s="2"/>
       <c r="G145" s="2">
         <f t="shared" si="11"/>
-        <v>4668.1605</v>
+        <v>4593.0712000000003</v>
       </c>
       <c r="H145" s="2">
         <f t="shared" si="12"/>
-        <v>4493.7434000000012</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4418.5968999999996</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A146" s="1">
         <v>43769</v>
       </c>
@@ -14585,14 +14823,14 @@
       <c r="E146" s="2"/>
       <c r="G146" s="2">
         <f t="shared" si="11"/>
-        <v>4736.9423999999999</v>
+        <v>4660.1472000000003</v>
       </c>
       <c r="H146" s="2">
         <f t="shared" si="12"/>
-        <v>4555.5456000000004</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4477.7423999999992</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A147" s="1">
         <v>43770</v>
       </c>
@@ -14603,14 +14841,14 @@
       <c r="E147" s="2"/>
       <c r="G147" s="2">
         <f t="shared" si="11"/>
-        <v>4806.2264999999998</v>
+        <v>4727.7089999999998</v>
       </c>
       <c r="H147" s="2">
         <f t="shared" si="12"/>
-        <v>4617.6830000000009</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4537.1644999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A148" s="1">
         <v>43771</v>
       </c>
@@ -14621,14 +14859,14 @@
       <c r="E148" s="2"/>
       <c r="G148" s="2">
         <f t="shared" si="11"/>
-        <v>4876.0127999999995</v>
+        <v>4795.7565999999997</v>
       </c>
       <c r="H148" s="2">
         <f t="shared" si="12"/>
-        <v>4680.1538</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4596.8607999999995</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A149" s="1">
         <v>43772</v>
       </c>
@@ -14639,14 +14877,14 @@
       <c r="E149" s="2"/>
       <c r="G149" s="2">
         <f t="shared" si="11"/>
-        <v>4946.3013000000001</v>
+        <v>4864.29</v>
       </c>
       <c r="H149" s="2">
         <f t="shared" si="12"/>
-        <v>4742.9562000000005</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4656.8288999999995</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A150" s="1">
         <v>43773</v>
       </c>
@@ -14657,14 +14895,14 @@
       <c r="E150" s="2"/>
       <c r="G150" s="2">
         <f t="shared" si="11"/>
-        <v>5017.0919999999996</v>
+        <v>4933.3091999999997</v>
       </c>
       <c r="H150" s="2">
         <f t="shared" si="12"/>
-        <v>4806.0884000000005</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4717.0663999999997</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A151" s="1">
         <v>43774</v>
       </c>
@@ -14675,14 +14913,17 @@
       <c r="E151" s="2"/>
       <c r="G151" s="2">
         <f t="shared" si="11"/>
-        <v>5088.3849</v>
+        <v>5002.8142000000007</v>
       </c>
       <c r="H151" s="2">
         <f t="shared" si="12"/>
-        <v>4869.5486000000001</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4777.5708999999997</v>
+      </c>
+      <c r="I151" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A152" s="1">
         <v>43775</v>
       </c>
@@ -14693,14 +14934,14 @@
       <c r="E152" s="2"/>
       <c r="G152" s="2">
         <f t="shared" si="11"/>
-        <v>5160.18</v>
+        <v>5072.8050000000003</v>
       </c>
       <c r="H152" s="2">
         <f t="shared" si="12"/>
-        <v>4933.335</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4838.34</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A153" s="1">
         <v>43776</v>
       </c>
@@ -14711,14 +14952,14 @@
       <c r="E153" s="2"/>
       <c r="G153" s="2">
         <f t="shared" si="11"/>
-        <v>5232.4772999999996</v>
+        <v>5143.2816000000003</v>
       </c>
       <c r="H153" s="2">
         <f t="shared" si="12"/>
-        <v>4997.4458000000004</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4899.3712999999998</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A154" s="1">
         <v>43777</v>
       </c>
@@ -14729,14 +14970,14 @@
       <c r="E154" s="2"/>
       <c r="G154" s="2">
         <f t="shared" si="11"/>
-        <v>5305.2767999999996</v>
+        <v>5214.2440000000006</v>
       </c>
       <c r="H154" s="2">
         <f t="shared" si="12"/>
-        <v>5061.8792000000012</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.4">
+        <v>4960.6623999999993</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A155" s="1">
         <v>43778</v>
       </c>
@@ -14747,14 +14988,17 @@
       <c r="E155" s="2"/>
       <c r="G155" s="2">
         <f t="shared" si="11"/>
-        <v>5378.5784999999996</v>
+        <v>5285.6922000000004</v>
       </c>
       <c r="H155" s="2">
         <f t="shared" si="12"/>
-        <v>5126.6333999999997</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.4">
+        <v>5022.2109</v>
+      </c>
+      <c r="I155" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A156" s="1">
         <v>43779</v>
       </c>
@@ -14765,14 +15009,14 @@
       <c r="E156" s="2"/>
       <c r="G156" s="2">
         <f t="shared" si="11"/>
-        <v>5452.3823999999995</v>
+        <v>5357.6261999999997</v>
       </c>
       <c r="H156" s="2">
         <f t="shared" si="12"/>
-        <v>5191.7066000000013</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.4">
+        <v>5084.0144</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A157" s="1">
         <v>43780</v>
       </c>
@@ -14783,14 +15027,14 @@
       <c r="E157" s="2"/>
       <c r="G157" s="2">
         <f t="shared" si="11"/>
-        <v>5526.6885000000002</v>
+        <v>5430.0459999999994</v>
       </c>
       <c r="H157" s="2">
         <f t="shared" si="12"/>
-        <v>5257.0970000000007</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.4">
+        <v>5146.0704999999998</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A158" s="1">
         <v>43781</v>
       </c>
@@ -14801,14 +15045,14 @@
       <c r="E158" s="2"/>
       <c r="G158" s="2">
         <f t="shared" si="11"/>
-        <v>5601.4967999999999</v>
+        <v>5502.9516000000003</v>
       </c>
       <c r="H158" s="2">
         <f t="shared" si="12"/>
-        <v>5322.8028000000004</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.4">
+        <v>5208.3768</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A159" s="1">
         <v>43782</v>
       </c>
@@ -14819,14 +15063,14 @@
       <c r="E159" s="2"/>
       <c r="G159" s="2">
         <f t="shared" si="11"/>
-        <v>5676.8072999999995</v>
+        <v>5576.3430000000008</v>
       </c>
       <c r="H159" s="2">
         <f t="shared" si="12"/>
-        <v>5388.8222000000005</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.4">
+        <v>5270.9309000000003</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A160" s="1">
         <v>43783</v>
       </c>
@@ -14837,11 +15081,11 @@
       <c r="E160" s="2"/>
       <c r="G160" s="2">
         <f t="shared" si="11"/>
-        <v>5752.62</v>
+        <v>5650.2202000000007</v>
       </c>
       <c r="H160" s="2">
         <f t="shared" si="12"/>
-        <v>5455.1534000000011</v>
+        <v>5333.7304000000004</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.4">
@@ -14855,11 +15099,11 @@
       <c r="E161" s="2"/>
       <c r="G161" s="2">
         <f t="shared" si="11"/>
-        <v>5828.9348999999993</v>
+        <v>5724.5832</v>
       </c>
       <c r="H161" s="2">
         <f t="shared" si="12"/>
-        <v>5521.7946000000002</v>
+        <v>5396.7728999999999</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.4">
@@ -14873,11 +15117,11 @@
       <c r="E162" s="2"/>
       <c r="G162" s="2">
         <f t="shared" si="11"/>
-        <v>5905.7519999999995</v>
+        <v>5799.4319999999998</v>
       </c>
       <c r="H162" s="2">
         <f t="shared" si="12"/>
-        <v>5588.7440000000006</v>
+        <v>5460.0560000000005</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.4">
@@ -14891,11 +15135,11 @@
       <c r="E163" s="2"/>
       <c r="G163" s="2">
         <f t="shared" si="11"/>
-        <v>5983.0713000000005</v>
+        <v>5874.7665999999999</v>
       </c>
       <c r="H163" s="2">
         <f t="shared" si="12"/>
-        <v>5655.9998000000005</v>
+        <v>5523.5772999999999</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.4">
@@ -14909,11 +15153,11 @@
       <c r="E164" s="2"/>
       <c r="G164" s="2">
         <f t="shared" si="11"/>
-        <v>6060.8927999999996</v>
+        <v>5950.5869999999995</v>
       </c>
       <c r="H164" s="2">
         <f t="shared" si="12"/>
-        <v>5723.5602000000008</v>
+        <v>5587.3343999999997</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.4">
@@ -14927,11 +15171,11 @@
       <c r="E165" s="2"/>
       <c r="G165" s="2">
         <f t="shared" si="11"/>
-        <v>6139.2164999999995</v>
+        <v>6026.8931999999995</v>
       </c>
       <c r="H165" s="2">
         <f t="shared" si="12"/>
-        <v>5791.4234000000006</v>
+        <v>5651.3248999999987</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.4">
@@ -14945,11 +15189,11 @@
       <c r="E166" s="2"/>
       <c r="G166" s="2">
         <f t="shared" si="11"/>
-        <v>6218.0423999999994</v>
+        <v>6103.6852000000008</v>
       </c>
       <c r="H166" s="2">
         <f t="shared" si="12"/>
-        <v>5859.5876000000007</v>
+        <v>5715.5464000000011</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.4">
@@ -14963,11 +15207,11 @@
       <c r="E167" s="2"/>
       <c r="G167" s="2">
         <f t="shared" si="11"/>
-        <v>6297.3704999999991</v>
+        <v>6180.9630000000006</v>
       </c>
       <c r="H167" s="2">
         <f t="shared" si="12"/>
-        <v>5928.0510000000004</v>
+        <v>5779.9965000000002</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.4">
@@ -14981,11 +15225,11 @@
       <c r="E168" s="2"/>
       <c r="G168" s="2">
         <f t="shared" si="11"/>
-        <v>6377.2008000000005</v>
+        <v>6258.7266</v>
       </c>
       <c r="H168" s="2">
         <f t="shared" si="12"/>
-        <v>5996.8118000000004</v>
+        <v>5844.6728000000003</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.4">
@@ -14999,11 +15243,11 @@
       <c r="E169" s="2"/>
       <c r="G169" s="2">
         <f t="shared" si="11"/>
-        <v>6457.5333000000001</v>
+        <v>6336.9760000000006</v>
       </c>
       <c r="H169" s="2">
         <f t="shared" si="12"/>
-        <v>6065.8681999999999</v>
+        <v>5909.5728999999992</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.4">
@@ -15017,11 +15261,11 @@
       <c r="E170" s="2"/>
       <c r="G170" s="2">
         <f t="shared" si="11"/>
-        <v>6538.3679999999995</v>
+        <v>6415.7111999999997</v>
       </c>
       <c r="H170" s="2">
         <f t="shared" si="12"/>
-        <v>6135.2184000000007</v>
+        <v>5974.6944000000003</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.4">
@@ -15035,11 +15279,11 @@
       <c r="E171" s="2"/>
       <c r="G171" s="2">
         <f t="shared" si="11"/>
-        <v>6619.7048999999997</v>
+        <v>6494.9322000000002</v>
       </c>
       <c r="H171" s="2">
         <f t="shared" si="12"/>
-        <v>6204.8606</v>
+        <v>6040.0349000000006</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.4">
@@ -15053,11 +15297,11 @@
       <c r="E172" s="2"/>
       <c r="G172" s="2">
         <f t="shared" si="11"/>
-        <v>6701.5439999999999</v>
+        <v>6574.6390000000001</v>
       </c>
       <c r="H172" s="2">
         <f t="shared" si="12"/>
-        <v>6274.7930000000006</v>
+        <v>6105.5919999999987</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.4">
@@ -15071,11 +15315,11 @@
       <c r="E173" s="2"/>
       <c r="G173" s="2">
         <f t="shared" si="11"/>
-        <v>6783.885299999999</v>
+        <v>6654.8315999999995</v>
       </c>
       <c r="H173" s="2">
         <f t="shared" si="12"/>
-        <v>6345.0137999999997</v>
+        <v>6171.3632999999991</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.4">
@@ -15089,11 +15333,11 @@
       <c r="E174" s="2"/>
       <c r="G174" s="2">
         <f t="shared" si="11"/>
-        <v>6866.728799999999</v>
+        <v>6735.51</v>
       </c>
       <c r="H174" s="2">
         <f t="shared" si="12"/>
-        <v>6415.521200000002</v>
+        <v>6237.3463999999985</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.4">
@@ -15107,11 +15351,11 @@
       <c r="E175" s="2"/>
       <c r="G175" s="2">
         <f t="shared" si="11"/>
-        <v>6950.0744999999997</v>
+        <v>6816.6742000000004</v>
       </c>
       <c r="H175" s="2">
         <f t="shared" si="12"/>
-        <v>6486.3134000000009</v>
+        <v>6303.5388999999996</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.4">
@@ -15125,15 +15369,15 @@
       <c r="E176" s="2"/>
       <c r="G176" s="2">
         <f t="shared" si="11"/>
-        <v>7033.9223999999995</v>
+        <v>6898.3242</v>
       </c>
       <c r="H176" s="2">
         <f t="shared" si="12"/>
-        <v>6557.3886000000011</v>
+        <v>6369.9383999999991</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G1:H1048576 I1">
+  <conditionalFormatting sqref="I1 G1:H1048576">
     <cfRule type="cellIs" dxfId="5" priority="9" operator="greaterThan">
       <formula>$C1*1.1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Attempt to fix crash on open for some devices.
</commit_message>
<xml_diff>
--- a/InstallTracker.xlsx
+++ b/InstallTracker.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4E9FC9-AAE1-49A9-8E31-4D6F8A496C59}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24AF740-A249-47E7-AA52-74E99B8F2A11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1324,13 +1324,46 @@
                   <c:v>4540</c:v>
                 </c:pt>
                 <c:pt idx="148" formatCode="#,##0">
-                  <c:v>4630</c:v>
+                  <c:v>4627</c:v>
                 </c:pt>
                 <c:pt idx="149" formatCode="#,##0">
-                  <c:v>4644</c:v>
+                  <c:v>4687</c:v>
                 </c:pt>
                 <c:pt idx="150" formatCode="#,##0">
-                  <c:v>4708</c:v>
+                  <c:v>4702</c:v>
+                </c:pt>
+                <c:pt idx="151" formatCode="#,##0">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="152" formatCode="#,##0">
+                  <c:v>4819</c:v>
+                </c:pt>
+                <c:pt idx="153" formatCode="#,##0">
+                  <c:v>4898</c:v>
+                </c:pt>
+                <c:pt idx="154" formatCode="#,##0">
+                  <c:v>4923</c:v>
+                </c:pt>
+                <c:pt idx="155" formatCode="#,##0">
+                  <c:v>4987</c:v>
+                </c:pt>
+                <c:pt idx="156" formatCode="#,##0">
+                  <c:v>5037</c:v>
+                </c:pt>
+                <c:pt idx="157" formatCode="#,##0">
+                  <c:v>5031</c:v>
+                </c:pt>
+                <c:pt idx="158" formatCode="#,##0">
+                  <c:v>5079</c:v>
+                </c:pt>
+                <c:pt idx="159" formatCode="#,##0">
+                  <c:v>5115</c:v>
+                </c:pt>
+                <c:pt idx="160" formatCode="#,##0">
+                  <c:v>5204</c:v>
+                </c:pt>
+                <c:pt idx="161" formatCode="#,##0">
+                  <c:v>5249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2786,13 +2819,46 @@
                   <c:v>4540</c:v>
                 </c:pt>
                 <c:pt idx="148" formatCode="#,##0">
-                  <c:v>4630</c:v>
+                  <c:v>4627</c:v>
                 </c:pt>
                 <c:pt idx="149" formatCode="#,##0">
-                  <c:v>4644</c:v>
+                  <c:v>4687</c:v>
                 </c:pt>
                 <c:pt idx="150" formatCode="#,##0">
-                  <c:v>4708</c:v>
+                  <c:v>4702</c:v>
+                </c:pt>
+                <c:pt idx="151" formatCode="#,##0">
+                  <c:v>4750</c:v>
+                </c:pt>
+                <c:pt idx="152" formatCode="#,##0">
+                  <c:v>4819</c:v>
+                </c:pt>
+                <c:pt idx="153" formatCode="#,##0">
+                  <c:v>4898</c:v>
+                </c:pt>
+                <c:pt idx="154" formatCode="#,##0">
+                  <c:v>4923</c:v>
+                </c:pt>
+                <c:pt idx="155" formatCode="#,##0">
+                  <c:v>4987</c:v>
+                </c:pt>
+                <c:pt idx="156" formatCode="#,##0">
+                  <c:v>5037</c:v>
+                </c:pt>
+                <c:pt idx="157" formatCode="#,##0">
+                  <c:v>5031</c:v>
+                </c:pt>
+                <c:pt idx="158" formatCode="#,##0">
+                  <c:v>5079</c:v>
+                </c:pt>
+                <c:pt idx="159" formatCode="#,##0">
+                  <c:v>5115</c:v>
+                </c:pt>
+                <c:pt idx="160" formatCode="#,##0">
+                  <c:v>5204</c:v>
+                </c:pt>
+                <c:pt idx="161" formatCode="#,##0">
+                  <c:v>5249</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4292,13 +4358,46 @@
                   <c:v>39.285714285714285</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>47.285714285714285</c:v>
+                  <c:v>46.857142857142854</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>44</c:v>
+                  <c:v>50.142857142857146</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>47.428571428571431</c:v>
+                  <c:v>46.571428571428569</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>42.714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>51.714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>51.285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>54.714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>51.428571428571431</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>42.285714285714285</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>43.714285714285715</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>46.571428571428569</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5751,13 +5850,46 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>90</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>14</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="150">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="155">
                   <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>-6</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7263,13 +7395,46 @@
                   <c:v>30.655405405405407</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>31.053691275167786</c:v>
+                  <c:v>31.033557046979865</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>30.94</c:v>
+                  <c:v>31.226666666666667</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>31.158940397350992</c:v>
+                  <c:v>31.119205298013245</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>31.230263157894736</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>31.477124183006534</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>31.785714285714285</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>31.741935483870968</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>31.948717948717949</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>32.06369426751592</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>31.822784810126581</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>31.924528301886792</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>31.95</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>32.304347826086953</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>32.382716049382715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10812,23 +10977,23 @@
   <dimension ref="A1:J207"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="U38" sqref="U38"/>
+      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T172" sqref="T172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.54296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -10854,7 +11019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>43625</v>
       </c>
@@ -10877,17 +11042,17 @@
         <v>0</v>
       </c>
       <c r="G2" s="2">
-        <f>0.2429*B2^2-2.6363*B2+3</f>
+        <f>0.2129*B2^2+0.0613*B2+3</f>
         <v>3</v>
       </c>
       <c r="H2" s="2">
-        <f>-0.0004*B2^3+0.3111*B2^2-5.4294*B2+3</f>
+        <f>-0.0008*B2^3+0.3777*B2^2-7.9187*B2+3</f>
         <v>3</v>
       </c>
       <c r="I2" s="2"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>43626</v>
       </c>
@@ -10911,16 +11076,16 @@
         <v>0.5</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" ref="G3:G66" si="1">0.2429*B3^2-2.6363*B3+3</f>
-        <v>0.60660000000000025</v>
+        <f t="shared" ref="G3:G66" si="1">0.2129*B3^2+0.0613*B3+3</f>
+        <v>3.2742</v>
       </c>
       <c r="H3" s="2">
-        <f t="shared" ref="H3:H66" si="2">-0.0004*B3^3+0.3111*B3^2-5.4294*B3+3</f>
-        <v>-2.1187000000000005</v>
+        <f t="shared" ref="H3:H66" si="2">-0.0008*B3^3+0.3777*B3^2-7.9187*B3+3</f>
+        <v>-4.5418000000000003</v>
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>43627</v>
       </c>
@@ -10945,15 +11110,15 @@
       </c>
       <c r="G4" s="2">
         <f t="shared" si="1"/>
-        <v>-1.3010000000000002</v>
+        <v>3.9742000000000002</v>
       </c>
       <c r="H4" s="2">
         <f t="shared" si="2"/>
-        <v>-6.6176000000000013</v>
+        <v>-11.333</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>43628</v>
       </c>
@@ -10978,15 +11143,15 @@
       </c>
       <c r="G5" s="2">
         <f t="shared" si="1"/>
-        <v>-2.7227999999999994</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="2"/>
-        <v>-10.4991</v>
+        <v>-17.378399999999999</v>
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>43629</v>
       </c>
@@ -11011,15 +11176,15 @@
       </c>
       <c r="G6" s="2">
         <f t="shared" si="1"/>
-        <v>-3.6587999999999994</v>
+        <v>6.6516000000000002</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="2"/>
-        <v>-13.765599999999999</v>
+        <v>-22.6828</v>
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>43630</v>
       </c>
@@ -11044,15 +11209,15 @@
       </c>
       <c r="G7" s="2">
         <f t="shared" si="1"/>
-        <v>-4.109</v>
+        <v>8.6289999999999996</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="2"/>
-        <v>-16.419500000000003</v>
+        <v>-27.250999999999998</v>
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>43631</v>
       </c>
@@ -11077,15 +11242,15 @@
       </c>
       <c r="G8" s="2">
         <f t="shared" si="1"/>
-        <v>-4.0733999999999977</v>
+        <v>11.032200000000001</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="2"/>
-        <v>-18.463200000000001</v>
+        <v>-31.087800000000001</v>
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>43632</v>
       </c>
@@ -11110,15 +11275,15 @@
       </c>
       <c r="G9" s="2">
         <f t="shared" si="1"/>
-        <v>-3.5519999999999996</v>
+        <v>13.8612</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="2"/>
-        <v>-19.899100000000001</v>
+        <v>-34.198</v>
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>43633</v>
       </c>
@@ -11143,15 +11308,15 @@
       </c>
       <c r="G10" s="2">
         <f t="shared" si="1"/>
-        <v>-2.5447999999999986</v>
+        <v>17.116</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="2"/>
-        <v>-20.729600000000001</v>
+        <v>-36.586400000000005</v>
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>43634</v>
       </c>
@@ -11176,15 +11341,15 @@
       </c>
       <c r="G11" s="2">
         <f t="shared" si="1"/>
-        <v>-1.0517999999999965</v>
+        <v>20.796600000000002</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="2"/>
-        <v>-20.957100000000004</v>
+        <v>-38.257800000000003</v>
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>43635</v>
       </c>
@@ -11209,15 +11374,15 @@
       </c>
       <c r="G12" s="2">
         <f t="shared" si="1"/>
-        <v>0.9269999999999996</v>
+        <v>24.902999999999999</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="2"/>
-        <v>-20.584000000000003</v>
+        <v>-39.216999999999999</v>
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>43636</v>
       </c>
@@ -11242,15 +11407,15 @@
       </c>
       <c r="G13" s="2">
         <f t="shared" si="1"/>
-        <v>3.3916000000000039</v>
+        <v>29.435199999999998</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="2"/>
-        <v>-19.612700000000011</v>
+        <v>-39.468800000000002</v>
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>43637</v>
       </c>
@@ -11275,15 +11440,15 @@
       </c>
       <c r="G14" s="2">
         <f t="shared" si="1"/>
-        <v>6.3420000000000059</v>
+        <v>34.393200000000007</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="2"/>
-        <v>-18.0456</v>
+        <v>-39.018000000000001</v>
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>43638</v>
       </c>
@@ -11308,15 +11473,15 @@
       </c>
       <c r="G15" s="2">
         <f t="shared" si="1"/>
-        <v>9.7782000000000053</v>
+        <v>39.777000000000001</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="2"/>
-        <v>-15.885100000000001</v>
+        <v>-37.869399999999999</v>
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>43639</v>
       </c>
@@ -11341,15 +11506,15 @@
       </c>
       <c r="G16" s="2">
         <f t="shared" si="1"/>
-        <v>13.700200000000002</v>
+        <v>45.586599999999997</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="2"/>
-        <v>-13.133600000000001</v>
+        <v>-36.027799999999999</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>43640</v>
       </c>
@@ -11374,15 +11539,15 @@
       </c>
       <c r="G17" s="2">
         <f t="shared" si="1"/>
-        <v>18.108000000000004</v>
+        <v>51.822000000000003</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="2"/>
-        <v>-9.7934999999999945</v>
+        <v>-33.498000000000005</v>
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>43641</v>
       </c>
@@ -11407,15 +11572,15 @@
       </c>
       <c r="G18" s="2">
         <f t="shared" si="1"/>
-        <v>23.001600000000003</v>
+        <v>58.483200000000004</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="2"/>
-        <v>-5.8672000000000111</v>
+        <v>-30.284800000000004</v>
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>43642</v>
       </c>
@@ -11440,15 +11605,15 @@
       </c>
       <c r="G19" s="2">
         <f t="shared" si="1"/>
-        <v>28.381</v>
+        <v>65.5702</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="2"/>
-        <v>-1.3571000000000026</v>
+        <v>-26.393000000000001</v>
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>43643</v>
       </c>
@@ -11473,15 +11638,15 @@
       </c>
       <c r="G20" s="2">
         <f t="shared" si="1"/>
-        <v>34.246200000000009</v>
+        <v>73.082999999999998</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="2"/>
-        <v>3.7343999999999795</v>
+        <v>-21.827399999999997</v>
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>43644</v>
       </c>
@@ -11506,15 +11671,15 @@
       </c>
       <c r="G21" s="2">
         <f t="shared" si="1"/>
-        <v>40.597200000000008</v>
+        <v>81.021599999999992</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="2"/>
-        <v>9.4048999999999836</v>
+        <v>-16.592800000000011</v>
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>43645</v>
       </c>
@@ -11539,15 +11704,15 @@
       </c>
       <c r="G22" s="2">
         <f t="shared" si="1"/>
-        <v>47.433999999999997</v>
+        <v>89.385999999999996</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="2"/>
-        <v>15.651999999999987</v>
+        <v>-10.694000000000017</v>
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>43646</v>
       </c>
@@ -11572,15 +11737,15 @@
       </c>
       <c r="G23" s="2">
         <f t="shared" si="1"/>
-        <v>54.756599999999999</v>
+        <v>98.176200000000009</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="2"/>
-        <v>22.473299999999995</v>
+        <v>-4.1358000000000175</v>
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>43647</v>
       </c>
@@ -11605,15 +11770,15 @@
       </c>
       <c r="G24" s="2">
         <f t="shared" si="1"/>
-        <v>62.565000000000012</v>
+        <v>107.3922</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="2"/>
-        <v>29.866399999999985</v>
+        <v>3.0769999999999698</v>
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>43648</v>
       </c>
@@ -11638,15 +11803,15 @@
       </c>
       <c r="G25" s="2">
         <f t="shared" si="1"/>
-        <v>70.859200000000016</v>
+        <v>117.03399999999999</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="2"/>
-        <v>37.828899999999976</v>
+        <v>10.939599999999984</v>
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>43649</v>
       </c>
@@ -11671,15 +11836,15 @@
       </c>
       <c r="G26" s="2">
         <f t="shared" si="1"/>
-        <v>79.639200000000017</v>
+        <v>127.1016</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="2"/>
-        <v>46.358400000000017</v>
+        <v>19.447199999999981</v>
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>43650</v>
       </c>
@@ -11704,15 +11869,15 @@
       </c>
       <c r="G27" s="2">
         <f t="shared" si="1"/>
-        <v>88.905000000000001</v>
+        <v>137.595</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="2"/>
-        <v>55.452499999999986</v>
+        <v>28.594999999999999</v>
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>43651</v>
       </c>
@@ -11737,15 +11902,15 @@
       </c>
       <c r="G28" s="2">
         <f t="shared" si="1"/>
-        <v>98.656600000000012</v>
+        <v>148.51419999999999</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="2"/>
-        <v>65.108799999999974</v>
+        <v>38.378199999999993</v>
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>43652</v>
       </c>
@@ -11770,15 +11935,15 @@
       </c>
       <c r="G29" s="2">
         <f t="shared" si="1"/>
-        <v>108.89400000000002</v>
+        <v>159.85920000000002</v>
       </c>
       <c r="H29" s="2">
         <f t="shared" si="2"/>
-        <v>75.324899999999985</v>
+        <v>48.792000000000002</v>
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>43653</v>
       </c>
@@ -11803,15 +11968,15 @@
       </c>
       <c r="G30" s="2">
         <f t="shared" si="1"/>
-        <v>119.61720000000001</v>
+        <v>171.63</v>
       </c>
       <c r="H30" s="2">
         <f t="shared" si="2"/>
-        <v>86.098399999999998</v>
+        <v>59.831600000000009</v>
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>43654</v>
       </c>
@@ -11836,15 +12001,15 @@
       </c>
       <c r="G31" s="2">
         <f t="shared" si="1"/>
-        <v>130.8262</v>
+        <v>183.82660000000001</v>
       </c>
       <c r="H31" s="2">
         <f t="shared" si="2"/>
-        <v>97.426899999999932</v>
+        <v>71.492199999999997</v>
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>43655</v>
       </c>
@@ -11869,15 +12034,15 @@
       </c>
       <c r="G32" s="2">
         <f t="shared" si="1"/>
-        <v>142.52100000000002</v>
+        <v>196.44900000000001</v>
       </c>
       <c r="H32" s="2">
         <f t="shared" si="2"/>
-        <v>109.30799999999999</v>
+        <v>83.768999999999977</v>
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>43656</v>
       </c>
@@ -11902,15 +12067,15 @@
       </c>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
-        <v>154.70160000000004</v>
+        <v>209.49719999999999</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="2"/>
-        <v>121.73929999999999</v>
+        <v>96.65719999999996</v>
       </c>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>43657</v>
       </c>
@@ -11935,15 +12100,15 @@
       </c>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
-        <v>167.36799999999999</v>
+        <v>222.97120000000001</v>
       </c>
       <c r="H34" s="2">
         <f t="shared" si="2"/>
-        <v>134.7184</v>
+        <v>110.15199999999996</v>
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>43658</v>
       </c>
@@ -11968,15 +12133,15 @@
       </c>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
-        <v>180.52019999999999</v>
+        <v>236.87100000000001</v>
       </c>
       <c r="H35" s="2">
         <f t="shared" si="2"/>
-        <v>148.24289999999999</v>
+        <v>124.24860000000001</v>
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>43659</v>
       </c>
@@ -12001,15 +12166,15 @@
       </c>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
-        <v>194.15819999999999</v>
+        <v>251.19660000000002</v>
       </c>
       <c r="H36" s="2">
         <f t="shared" si="2"/>
-        <v>162.31039999999996</v>
+        <v>138.94220000000001</v>
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>43660</v>
       </c>
@@ -12034,15 +12199,15 @@
       </c>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
-        <v>208.28200000000001</v>
+        <v>265.94800000000004</v>
       </c>
       <c r="H37" s="2">
         <f t="shared" si="2"/>
-        <v>176.91849999999999</v>
+        <v>154.22799999999995</v>
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>43661</v>
       </c>
@@ -12067,15 +12232,15 @@
       </c>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
-        <v>222.89160000000004</v>
+        <v>281.12520000000001</v>
       </c>
       <c r="H38" s="2">
         <f t="shared" si="2"/>
-        <v>192.06479999999996</v>
+        <v>170.10120000000001</v>
       </c>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>43662</v>
       </c>
@@ -12100,15 +12265,15 @@
       </c>
       <c r="G39" s="2">
         <f t="shared" si="1"/>
-        <v>237.98700000000002</v>
+        <v>296.72820000000002</v>
       </c>
       <c r="H39" s="2">
         <f t="shared" si="2"/>
-        <v>207.74689999999995</v>
+        <v>186.55699999999996</v>
       </c>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>43663</v>
       </c>
@@ -12133,15 +12298,15 @@
       </c>
       <c r="G40" s="2">
         <f t="shared" si="1"/>
-        <v>253.56820000000005</v>
+        <v>312.75700000000001</v>
       </c>
       <c r="H40" s="2">
         <f t="shared" si="2"/>
-        <v>223.96239999999995</v>
+        <v>203.59059999999994</v>
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>43664</v>
       </c>
@@ -12166,15 +12331,15 @@
       </c>
       <c r="G41" s="2">
         <f t="shared" si="1"/>
-        <v>269.6352</v>
+        <v>329.21159999999998</v>
       </c>
       <c r="H41" s="2">
         <f t="shared" si="2"/>
-        <v>240.70889999999997</v>
+        <v>221.19719999999995</v>
       </c>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>43665</v>
       </c>
@@ -12199,15 +12364,15 @@
       </c>
       <c r="G42" s="2">
         <f t="shared" si="1"/>
-        <v>286.18799999999999</v>
+        <v>346.09199999999998</v>
       </c>
       <c r="H42" s="2">
         <f t="shared" si="2"/>
-        <v>257.98399999999992</v>
+        <v>239.3719999999999</v>
       </c>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>43666</v>
       </c>
@@ -12232,15 +12397,15 @@
       </c>
       <c r="G43" s="2">
         <f t="shared" si="1"/>
-        <v>303.22660000000002</v>
+        <v>363.39820000000003</v>
       </c>
       <c r="H43" s="2">
         <f t="shared" si="2"/>
-        <v>275.78530000000001</v>
+        <v>258.11019999999996</v>
       </c>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43667</v>
       </c>
@@ -12265,15 +12430,15 @@
       </c>
       <c r="G44" s="2">
         <f t="shared" si="1"/>
-        <v>320.75099999999998</v>
+        <v>381.1302</v>
       </c>
       <c r="H44" s="2">
         <f t="shared" si="2"/>
-        <v>294.11039999999991</v>
+        <v>277.40699999999998</v>
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43668</v>
       </c>
@@ -12298,15 +12463,15 @@
       </c>
       <c r="G45" s="2">
         <f t="shared" si="1"/>
-        <v>338.76119999999997</v>
+        <v>399.28800000000001</v>
       </c>
       <c r="H45" s="2">
         <f t="shared" si="2"/>
-        <v>312.95689999999991</v>
+        <v>297.25760000000002</v>
       </c>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>43669</v>
       </c>
@@ -12331,15 +12496,15 @@
       </c>
       <c r="G46" s="2">
         <f t="shared" si="1"/>
-        <v>357.25720000000001</v>
+        <v>417.8716</v>
       </c>
       <c r="H46" s="2">
         <f t="shared" si="2"/>
-        <v>332.3223999999999</v>
+        <v>317.65719999999993</v>
       </c>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>43670</v>
       </c>
@@ -12364,15 +12529,15 @@
       </c>
       <c r="G47" s="2">
         <f t="shared" si="1"/>
-        <v>376.23900000000003</v>
+        <v>436.88100000000003</v>
       </c>
       <c r="H47" s="2">
         <f t="shared" si="2"/>
-        <v>352.20449999999994</v>
+        <v>338.601</v>
       </c>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>43671</v>
       </c>
@@ -12397,15 +12562,15 @@
       </c>
       <c r="G48" s="2">
         <f t="shared" si="1"/>
-        <v>395.70660000000004</v>
+        <v>456.31619999999998</v>
       </c>
       <c r="H48" s="2">
         <f t="shared" si="2"/>
-        <v>372.60079999999999</v>
+        <v>360.08419999999995</v>
       </c>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>43672</v>
       </c>
@@ -12430,15 +12595,15 @@
       </c>
       <c r="G49" s="2">
         <f t="shared" si="1"/>
-        <v>415.66</v>
+        <v>476.17720000000003</v>
       </c>
       <c r="H49" s="2">
         <f t="shared" si="2"/>
-        <v>393.50889999999987</v>
+        <v>382.10199999999998</v>
       </c>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>43673</v>
       </c>
@@ -12463,15 +12628,15 @@
       </c>
       <c r="G50" s="2">
         <f t="shared" si="1"/>
-        <v>436.09920000000005</v>
+        <v>496.46400000000006</v>
       </c>
       <c r="H50" s="2">
         <f t="shared" si="2"/>
-        <v>414.9264</v>
+        <v>404.64959999999991</v>
       </c>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>43674</v>
       </c>
@@ -12496,15 +12661,15 @@
       </c>
       <c r="G51" s="2">
         <f t="shared" si="1"/>
-        <v>457.02420000000001</v>
+        <v>517.17660000000001</v>
       </c>
       <c r="H51" s="2">
         <f t="shared" si="2"/>
-        <v>436.85089999999997</v>
+        <v>427.72219999999993</v>
       </c>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>43675</v>
       </c>
@@ -12529,15 +12694,15 @@
       </c>
       <c r="G52" s="2">
         <f t="shared" si="1"/>
-        <v>478.435</v>
+        <v>538.31500000000005</v>
       </c>
       <c r="H52" s="2">
         <f t="shared" si="2"/>
-        <v>459.28</v>
+        <v>451.315</v>
       </c>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>43676</v>
       </c>
@@ -12562,15 +12727,15 @@
       </c>
       <c r="G53" s="2">
         <f t="shared" si="1"/>
-        <v>500.33160000000004</v>
+        <v>559.87920000000008</v>
       </c>
       <c r="H53" s="2">
         <f t="shared" si="2"/>
-        <v>482.21130000000005</v>
+        <v>475.42319999999995</v>
       </c>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>43677</v>
       </c>
@@ -12595,15 +12760,15 @@
       </c>
       <c r="G54" s="2">
         <f t="shared" si="1"/>
-        <v>522.71400000000006</v>
+        <v>581.86919999999998</v>
       </c>
       <c r="H54" s="2">
         <f t="shared" si="2"/>
-        <v>505.64239999999995</v>
+        <v>500.04199999999997</v>
       </c>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>43678</v>
       </c>
@@ -12628,15 +12793,15 @@
       </c>
       <c r="G55" s="2">
         <f t="shared" si="1"/>
-        <v>545.58220000000006</v>
+        <v>604.28500000000008</v>
       </c>
       <c r="H55" s="2">
         <f t="shared" si="2"/>
-        <v>529.57090000000005</v>
+        <v>525.16660000000002</v>
       </c>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>43679</v>
       </c>
@@ -12661,15 +12826,15 @@
       </c>
       <c r="G56" s="2">
         <f t="shared" si="1"/>
-        <v>568.9362000000001</v>
+        <v>627.12660000000005</v>
       </c>
       <c r="H56" s="2">
         <f t="shared" si="2"/>
-        <v>553.99440000000004</v>
+        <v>550.79220000000009</v>
       </c>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>43680</v>
       </c>
@@ -12694,15 +12859,15 @@
       </c>
       <c r="G57" s="2">
         <f t="shared" si="1"/>
-        <v>592.77600000000007</v>
+        <v>650.39400000000001</v>
       </c>
       <c r="H57" s="2">
         <f t="shared" si="2"/>
-        <v>578.91049999999996</v>
+        <v>576.91399999999999</v>
       </c>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>43681</v>
       </c>
@@ -12727,15 +12892,15 @@
       </c>
       <c r="G58" s="2">
         <f t="shared" si="1"/>
-        <v>617.10160000000008</v>
+        <v>674.08720000000005</v>
       </c>
       <c r="H58" s="2">
         <f t="shared" si="2"/>
-        <v>604.31680000000006</v>
+        <v>603.52719999999999</v>
       </c>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>43682</v>
       </c>
@@ -12760,15 +12925,15 @@
       </c>
       <c r="G59" s="2">
         <f t="shared" si="1"/>
-        <v>641.91300000000001</v>
+        <v>698.20619999999997</v>
       </c>
       <c r="H59" s="2">
         <f t="shared" si="2"/>
-        <v>630.21090000000004</v>
+        <v>630.62699999999973</v>
       </c>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>43683</v>
       </c>
@@ -12793,15 +12958,15 @@
       </c>
       <c r="G60" s="2">
         <f t="shared" si="1"/>
-        <v>667.21019999999999</v>
+        <v>722.75099999999998</v>
       </c>
       <c r="H60" s="2">
         <f t="shared" si="2"/>
-        <v>656.59039999999982</v>
+        <v>658.20859999999993</v>
       </c>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>43684</v>
       </c>
@@ -12826,15 +12991,15 @@
       </c>
       <c r="G61" s="2">
         <f t="shared" si="1"/>
-        <v>692.9932</v>
+        <v>747.72160000000008</v>
       </c>
       <c r="H61" s="2">
         <f t="shared" si="2"/>
-        <v>683.4529</v>
+        <v>686.26719999999989</v>
       </c>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>43685</v>
       </c>
@@ -12859,15 +13024,15 @@
       </c>
       <c r="G62" s="2">
         <f t="shared" si="1"/>
-        <v>719.26200000000006</v>
+        <v>773.11800000000005</v>
       </c>
       <c r="H62" s="2">
         <f t="shared" si="2"/>
-        <v>710.79599999999994</v>
+        <v>714.798</v>
       </c>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>43686</v>
       </c>
@@ -12892,15 +13057,15 @@
       </c>
       <c r="G63" s="2">
         <f t="shared" si="1"/>
-        <v>746.01660000000004</v>
+        <v>798.9402</v>
       </c>
       <c r="H63" s="2">
         <f t="shared" si="2"/>
-        <v>738.6173</v>
+        <v>743.79619999999977</v>
       </c>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>43687</v>
       </c>
@@ -12925,15 +13090,15 @@
       </c>
       <c r="G64" s="2">
         <f t="shared" si="1"/>
-        <v>773.25700000000006</v>
+        <v>825.18820000000005</v>
       </c>
       <c r="H64" s="2">
         <f t="shared" si="2"/>
-        <v>766.91439999999989</v>
+        <v>773.25700000000006</v>
       </c>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>43688</v>
       </c>
@@ -12958,15 +13123,15 @@
       </c>
       <c r="G65" s="2">
         <f t="shared" si="1"/>
-        <v>800.98320000000001</v>
+        <v>851.86199999999997</v>
       </c>
       <c r="H65" s="2">
         <f t="shared" si="2"/>
-        <v>795.68489999999974</v>
+        <v>803.17559999999992</v>
       </c>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>43689</v>
       </c>
@@ -12991,15 +13156,15 @@
       </c>
       <c r="G66" s="2">
         <f t="shared" si="1"/>
-        <v>829.1952</v>
+        <v>878.96159999999998</v>
       </c>
       <c r="H66" s="2">
         <f t="shared" si="2"/>
-        <v>824.92639999999983</v>
+        <v>833.54719999999975</v>
       </c>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>43690</v>
       </c>
@@ -13023,16 +13188,16 @@
         <v>11.696969696969697</v>
       </c>
       <c r="G67" s="2">
-        <f t="shared" ref="G67:G130" si="6">0.2429*B67^2-2.6363*B67+3</f>
-        <v>857.89300000000003</v>
+        <f t="shared" ref="G67:G130" si="6">0.2129*B67^2+0.0613*B67+3</f>
+        <v>906.48700000000008</v>
       </c>
       <c r="H67" s="2">
-        <f t="shared" ref="H67:H130" si="7">-0.0004*B67^3+0.3111*B67^2-5.4294*B67+3</f>
-        <v>854.63650000000007</v>
+        <f t="shared" ref="H67:H130" si="7">-0.0008*B67^3+0.3777*B67^2-7.9187*B67+3</f>
+        <v>864.36699999999996</v>
       </c>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>43691</v>
       </c>
@@ -13057,15 +13222,15 @@
       </c>
       <c r="G68" s="2">
         <f t="shared" si="6"/>
-        <v>887.07659999999998</v>
+        <v>934.43820000000005</v>
       </c>
       <c r="H68" s="2">
         <f t="shared" si="7"/>
-        <v>884.81279999999992</v>
+        <v>895.63020000000006</v>
       </c>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>43692</v>
       </c>
@@ -13090,15 +13255,15 @@
       </c>
       <c r="G69" s="2">
         <f t="shared" si="6"/>
-        <v>916.74600000000009</v>
+        <v>962.8152</v>
       </c>
       <c r="H69" s="2">
         <f t="shared" si="7"/>
-        <v>915.4529</v>
+        <v>927.33199999999977</v>
       </c>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>43693</v>
       </c>
@@ -13123,15 +13288,15 @@
       </c>
       <c r="G70" s="2">
         <f t="shared" si="6"/>
-        <v>946.90120000000002</v>
+        <v>991.61800000000005</v>
       </c>
       <c r="H70" s="2">
         <f t="shared" si="7"/>
-        <v>946.55439999999999</v>
+        <v>959.46760000000006</v>
       </c>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>43694</v>
       </c>
@@ -13156,15 +13321,15 @@
       </c>
       <c r="G71" s="2">
         <f t="shared" si="6"/>
-        <v>977.54219999999987</v>
+        <v>1020.8466</v>
       </c>
       <c r="H71" s="2">
         <f t="shared" si="7"/>
-        <v>978.11489999999981</v>
+        <v>992.03219999999988</v>
       </c>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>43695</v>
       </c>
@@ -13189,15 +13354,15 @@
       </c>
       <c r="G72" s="2">
         <f t="shared" si="6"/>
-        <v>1008.6690000000001</v>
+        <v>1050.501</v>
       </c>
       <c r="H72" s="2">
         <f t="shared" si="7"/>
-        <v>1010.1319999999998</v>
+        <v>1025.0209999999997</v>
       </c>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>43696</v>
       </c>
@@ -13222,15 +13387,15 @@
       </c>
       <c r="G73" s="2">
         <f t="shared" si="6"/>
-        <v>1040.2816</v>
+        <v>1080.5812000000001</v>
       </c>
       <c r="H73" s="2">
         <f t="shared" si="7"/>
-        <v>1042.6032999999998</v>
+        <v>1058.4292</v>
       </c>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>43697</v>
       </c>
@@ -13255,15 +13420,15 @@
       </c>
       <c r="G74" s="2">
         <f t="shared" si="6"/>
-        <v>1072.3800000000001</v>
+        <v>1111.0872000000002</v>
       </c>
       <c r="H74" s="2">
         <f t="shared" si="7"/>
-        <v>1075.5264</v>
+        <v>1092.252</v>
       </c>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>43698</v>
       </c>
@@ -13288,15 +13453,15 @@
       </c>
       <c r="G75" s="2">
         <f t="shared" si="6"/>
-        <v>1104.9641999999999</v>
+        <v>1142.019</v>
       </c>
       <c r="H75" s="2">
         <f t="shared" si="7"/>
-        <v>1108.8988999999999</v>
+        <v>1126.4845999999998</v>
       </c>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>43699</v>
       </c>
@@ -13321,15 +13486,15 @@
       </c>
       <c r="G76" s="2">
         <f t="shared" si="6"/>
-        <v>1138.0342000000001</v>
+        <v>1173.3766000000001</v>
       </c>
       <c r="H76" s="2">
         <f t="shared" si="7"/>
-        <v>1142.7184</v>
+        <v>1161.1221999999998</v>
       </c>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>43700</v>
       </c>
@@ -13354,15 +13519,15 @@
       </c>
       <c r="G77" s="2">
         <f t="shared" si="6"/>
-        <v>1171.5899999999999</v>
+        <v>1205.1600000000001</v>
       </c>
       <c r="H77" s="2">
         <f t="shared" si="7"/>
-        <v>1176.9825000000001</v>
+        <v>1196.1599999999999</v>
       </c>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>43701</v>
       </c>
@@ -13387,15 +13552,15 @@
       </c>
       <c r="G78" s="2">
         <f t="shared" si="6"/>
-        <v>1205.6316000000002</v>
+        <v>1237.3691999999999</v>
       </c>
       <c r="H78" s="2">
         <f t="shared" si="7"/>
-        <v>1211.6887999999999</v>
+        <v>1231.5931999999998</v>
       </c>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>43702</v>
       </c>
@@ -13420,15 +13585,15 @@
       </c>
       <c r="G79" s="2">
         <f t="shared" si="6"/>
-        <v>1240.1590000000001</v>
+        <v>1270.0042000000001</v>
       </c>
       <c r="H79" s="2">
         <f t="shared" si="7"/>
-        <v>1246.8348999999998</v>
+        <v>1267.4169999999999</v>
       </c>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>43703</v>
       </c>
@@ -13453,15 +13618,15 @@
       </c>
       <c r="G80" s="2">
         <f t="shared" si="6"/>
-        <v>1275.1722</v>
+        <v>1303.0650000000001</v>
       </c>
       <c r="H80" s="2">
         <f t="shared" si="7"/>
-        <v>1282.4184</v>
+        <v>1303.6265999999998</v>
       </c>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>43704</v>
       </c>
@@ -13486,15 +13651,15 @@
       </c>
       <c r="G81" s="2">
         <f t="shared" si="6"/>
-        <v>1310.6712000000002</v>
+        <v>1336.5516</v>
       </c>
       <c r="H81" s="2">
         <f t="shared" si="7"/>
-        <v>1318.4368999999999</v>
+        <v>1340.2172</v>
       </c>
       <c r="I81" s="2"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>43705</v>
       </c>
@@ -13519,15 +13684,15 @@
       </c>
       <c r="G82" s="2">
         <f t="shared" si="6"/>
-        <v>1346.6559999999999</v>
+        <v>1370.4639999999999</v>
       </c>
       <c r="H82" s="2">
         <f t="shared" si="7"/>
-        <v>1354.8879999999999</v>
+        <v>1377.1839999999997</v>
       </c>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>43706</v>
       </c>
@@ -13552,15 +13717,15 @@
       </c>
       <c r="G83" s="2">
         <f t="shared" si="6"/>
-        <v>1383.1266000000001</v>
+        <v>1404.8022000000001</v>
       </c>
       <c r="H83" s="2">
         <f t="shared" si="7"/>
-        <v>1391.7692999999999</v>
+        <v>1414.5222000000001</v>
       </c>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>43707</v>
       </c>
@@ -13585,15 +13750,15 @@
       </c>
       <c r="G84" s="2">
         <f t="shared" si="6"/>
-        <v>1420.0830000000001</v>
+        <v>1439.5662</v>
       </c>
       <c r="H84" s="2">
         <f t="shared" si="7"/>
-        <v>1429.0784000000001</v>
+        <v>1452.2269999999999</v>
       </c>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>43708</v>
       </c>
@@ -13618,15 +13783,15 @@
       </c>
       <c r="G85" s="2">
         <f t="shared" si="6"/>
-        <v>1457.5252</v>
+        <v>1474.7560000000001</v>
       </c>
       <c r="H85" s="2">
         <f t="shared" si="7"/>
-        <v>1466.8128999999999</v>
+        <v>1490.2936</v>
       </c>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>43709</v>
       </c>
@@ -13651,15 +13816,15 @@
       </c>
       <c r="G86" s="2">
         <f t="shared" si="6"/>
-        <v>1495.4531999999999</v>
+        <v>1510.3716000000002</v>
       </c>
       <c r="H86" s="2">
         <f t="shared" si="7"/>
-        <v>1504.9703999999999</v>
+        <v>1528.7172</v>
       </c>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>43710</v>
       </c>
@@ -13684,15 +13849,15 @@
       </c>
       <c r="G87" s="2">
         <f t="shared" si="6"/>
-        <v>1533.8670000000002</v>
+        <v>1546.413</v>
       </c>
       <c r="H87" s="2">
         <f t="shared" si="7"/>
-        <v>1543.5484999999996</v>
+        <v>1567.4929999999995</v>
       </c>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>43711</v>
       </c>
@@ -13717,15 +13882,15 @@
       </c>
       <c r="G88" s="2">
         <f t="shared" si="6"/>
-        <v>1572.7665999999999</v>
+        <v>1582.8802000000001</v>
       </c>
       <c r="H88" s="2">
         <f t="shared" si="7"/>
-        <v>1582.5447999999999</v>
+        <v>1606.6162000000002</v>
       </c>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>43712</v>
       </c>
@@ -13750,15 +13915,15 @@
       </c>
       <c r="G89" s="2">
         <f t="shared" si="6"/>
-        <v>1612.152</v>
+        <v>1619.7732000000001</v>
       </c>
       <c r="H89" s="2">
         <f t="shared" si="7"/>
-        <v>1621.9568999999999</v>
+        <v>1646.0819999999999</v>
       </c>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>43713</v>
       </c>
@@ -13783,15 +13948,15 @@
       </c>
       <c r="G90" s="2">
         <f t="shared" si="6"/>
-        <v>1652.0232000000001</v>
+        <v>1657.0919999999999</v>
       </c>
       <c r="H90" s="2">
         <f t="shared" si="7"/>
-        <v>1661.7823999999998</v>
+        <v>1685.8855999999996</v>
       </c>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>43714</v>
       </c>
@@ -13816,15 +13981,15 @@
       </c>
       <c r="G91" s="2">
         <f t="shared" si="6"/>
-        <v>1692.3802000000001</v>
+        <v>1694.8366000000001</v>
       </c>
       <c r="H91" s="2">
         <f t="shared" si="7"/>
-        <v>1702.0188999999998</v>
+        <v>1726.0222000000001</v>
       </c>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>43715</v>
       </c>
@@ -13849,17 +14014,17 @@
       </c>
       <c r="G92" s="2">
         <f t="shared" si="6"/>
-        <v>1733.223</v>
+        <v>1733.0070000000001</v>
       </c>
       <c r="H92" s="2">
         <f t="shared" si="7"/>
-        <v>1742.664</v>
+        <v>1766.4870000000001</v>
       </c>
       <c r="I92" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>43716</v>
       </c>
@@ -13884,14 +14049,14 @@
       </c>
       <c r="G93" s="2">
         <f t="shared" si="6"/>
-        <v>1774.5516</v>
+        <v>1771.6032</v>
       </c>
       <c r="H93" s="2">
         <f t="shared" si="7"/>
-        <v>1783.7152999999996</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1807.2751999999996</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>43717</v>
       </c>
@@ -13916,14 +14081,14 @@
       </c>
       <c r="G94" s="2">
         <f t="shared" si="6"/>
-        <v>1816.366</v>
+        <v>1810.6251999999999</v>
       </c>
       <c r="H94" s="2">
         <f t="shared" si="7"/>
-        <v>1825.1704</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1848.3819999999996</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>43718</v>
       </c>
@@ -13948,14 +14113,14 @@
       </c>
       <c r="G95" s="2">
         <f t="shared" si="6"/>
-        <v>1858.6661999999999</v>
+        <v>1850.0730000000001</v>
       </c>
       <c r="H95" s="2">
         <f t="shared" si="7"/>
-        <v>1867.0268999999998</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1889.8026</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>43719</v>
       </c>
@@ -13980,17 +14145,17 @@
       </c>
       <c r="G96" s="2">
         <f t="shared" si="6"/>
-        <v>1901.4521999999999</v>
+        <v>1889.9466</v>
       </c>
       <c r="H96" s="2">
         <f t="shared" si="7"/>
-        <v>1909.2823999999996</v>
+        <v>1931.5321999999999</v>
       </c>
       <c r="I96" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>43720</v>
       </c>
@@ -14015,14 +14180,14 @@
       </c>
       <c r="G97" s="2">
         <f t="shared" si="6"/>
-        <v>1944.7240000000002</v>
+        <v>1930.2460000000001</v>
       </c>
       <c r="H97" s="2">
         <f t="shared" si="7"/>
-        <v>1951.9344999999998</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1973.5659999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>43721</v>
       </c>
@@ -14047,14 +14212,14 @@
       </c>
       <c r="G98" s="2">
         <f t="shared" si="6"/>
-        <v>1988.4816000000001</v>
+        <v>1970.9712000000002</v>
       </c>
       <c r="H98" s="2">
         <f t="shared" si="7"/>
-        <v>1994.9807999999998</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2015.8991999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>43722</v>
       </c>
@@ -14079,14 +14244,14 @@
       </c>
       <c r="G99" s="2">
         <f t="shared" si="6"/>
-        <v>2032.7250000000001</v>
+        <v>2012.1222</v>
       </c>
       <c r="H99" s="2">
         <f t="shared" si="7"/>
-        <v>2038.4188999999997</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2058.5269999999991</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>43723</v>
       </c>
@@ -14111,14 +14276,14 @@
       </c>
       <c r="G100" s="2">
         <f t="shared" si="6"/>
-        <v>2077.4542000000001</v>
+        <v>2053.6990000000001</v>
       </c>
       <c r="H100" s="2">
         <f t="shared" si="7"/>
-        <v>2082.2464</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2101.4445999999994</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>43724</v>
       </c>
@@ -14143,14 +14308,14 @@
       </c>
       <c r="G101" s="2">
         <f t="shared" si="6"/>
-        <v>2122.6692000000003</v>
+        <v>2095.7015999999999</v>
       </c>
       <c r="H101" s="2">
         <f t="shared" si="7"/>
-        <v>2126.4609</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2144.6471999999994</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>43725</v>
       </c>
@@ -14175,14 +14340,14 @@
       </c>
       <c r="G102" s="2">
         <f t="shared" si="6"/>
-        <v>2168.37</v>
+        <v>2138.13</v>
       </c>
       <c r="H102" s="2">
         <f t="shared" si="7"/>
-        <v>2171.06</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2188.13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>43726</v>
       </c>
@@ -14207,14 +14372,14 @@
       </c>
       <c r="G103" s="2">
         <f t="shared" si="6"/>
-        <v>2214.5565999999999</v>
+        <v>2180.9841999999999</v>
       </c>
       <c r="H103" s="2">
         <f t="shared" si="7"/>
-        <v>2216.0412999999994</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2231.8881999999999</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>43727</v>
       </c>
@@ -14239,14 +14404,14 @@
       </c>
       <c r="G104" s="2">
         <f t="shared" si="6"/>
-        <v>2261.2290000000003</v>
+        <v>2224.2642000000001</v>
       </c>
       <c r="H104" s="2">
         <f t="shared" si="7"/>
-        <v>2261.4023999999999</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2275.9169999999995</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>43728</v>
       </c>
@@ -14271,14 +14436,14 @@
       </c>
       <c r="G105" s="2">
         <f t="shared" si="6"/>
-        <v>2308.3872000000001</v>
+        <v>2267.9700000000003</v>
       </c>
       <c r="H105" s="2">
         <f t="shared" si="7"/>
-        <v>2307.1408999999999</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2320.2116000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>43729</v>
       </c>
@@ -14303,17 +14468,17 @@
       </c>
       <c r="G106" s="2">
         <f t="shared" si="6"/>
-        <v>2356.0311999999999</v>
+        <v>2312.1016</v>
       </c>
       <c r="H106" s="2">
         <f t="shared" si="7"/>
-        <v>2353.2543999999998</v>
+        <v>2364.7671999999998</v>
       </c>
       <c r="I106" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>43730</v>
       </c>
@@ -14338,17 +14503,17 @@
       </c>
       <c r="G107" s="2">
         <f t="shared" si="6"/>
-        <v>2404.1610000000001</v>
+        <v>2356.6589999999997</v>
       </c>
       <c r="H107" s="2">
         <f t="shared" si="7"/>
-        <v>2399.7404999999999</v>
+        <v>2409.5789999999997</v>
       </c>
       <c r="I107" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>43731</v>
       </c>
@@ -14373,14 +14538,14 @@
       </c>
       <c r="G108" s="2">
         <f t="shared" si="6"/>
-        <v>2452.7766000000001</v>
+        <v>2401.6422000000002</v>
       </c>
       <c r="H108" s="2">
         <f t="shared" si="7"/>
-        <v>2446.5968000000003</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2454.6421999999998</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>43732</v>
       </c>
@@ -14405,14 +14570,14 @@
       </c>
       <c r="G109" s="2">
         <f t="shared" si="6"/>
-        <v>2501.8780000000002</v>
+        <v>2447.0511999999999</v>
       </c>
       <c r="H109" s="2">
         <f t="shared" si="7"/>
-        <v>2493.8209000000002</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2499.9519999999998</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>43733</v>
       </c>
@@ -14437,14 +14602,14 @@
       </c>
       <c r="G110" s="2">
         <f t="shared" si="6"/>
-        <v>2551.4652000000001</v>
+        <v>2492.886</v>
       </c>
       <c r="H110" s="2">
         <f t="shared" si="7"/>
-        <v>2541.4104000000002</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2545.5036</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>43734</v>
       </c>
@@ -14469,14 +14634,14 @@
       </c>
       <c r="G111" s="2">
         <f t="shared" si="6"/>
-        <v>2601.5382000000004</v>
+        <v>2539.1466</v>
       </c>
       <c r="H111" s="2">
         <f t="shared" si="7"/>
-        <v>2589.3628999999996</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+        <v>2591.2921999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>43735</v>
       </c>
@@ -14501,14 +14666,14 @@
       </c>
       <c r="G112" s="2">
         <f t="shared" si="6"/>
-        <v>2652.0970000000002</v>
+        <v>2585.8330000000001</v>
       </c>
       <c r="H112" s="2">
         <f t="shared" si="7"/>
-        <v>2637.6759999999999</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2637.3130000000001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>43736</v>
       </c>
@@ -14533,14 +14698,14 @@
       </c>
       <c r="G113" s="2">
         <f t="shared" si="6"/>
-        <v>2703.1415999999999</v>
+        <v>2632.9451999999997</v>
       </c>
       <c r="H113" s="2">
         <f t="shared" si="7"/>
-        <v>2686.3472999999999</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2683.5612000000001</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>43737</v>
       </c>
@@ -14565,14 +14730,14 @@
       </c>
       <c r="G114" s="2">
         <f t="shared" si="6"/>
-        <v>2754.672</v>
+        <v>2680.4832000000001</v>
       </c>
       <c r="H114" s="2">
         <f t="shared" si="7"/>
-        <v>2735.3744000000002</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2730.0320000000002</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>43738</v>
       </c>
@@ -14597,14 +14762,14 @@
       </c>
       <c r="G115" s="2">
         <f t="shared" si="6"/>
-        <v>2806.6882000000001</v>
+        <v>2728.4470000000001</v>
       </c>
       <c r="H115" s="2">
         <f t="shared" si="7"/>
-        <v>2784.7548999999999</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2776.7205999999987</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>43739</v>
       </c>
@@ -14629,14 +14794,14 @@
       </c>
       <c r="G116" s="2">
         <f t="shared" si="6"/>
-        <v>2859.1902</v>
+        <v>2776.8365999999996</v>
       </c>
       <c r="H116" s="2">
         <f t="shared" si="7"/>
-        <v>2834.4863999999998</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2823.6221999999993</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>43740</v>
       </c>
@@ -14661,14 +14826,14 @@
       </c>
       <c r="G117" s="2">
         <f t="shared" si="6"/>
-        <v>2912.1779999999999</v>
+        <v>2825.652</v>
       </c>
       <c r="H117" s="2">
         <f t="shared" si="7"/>
-        <v>2884.5664999999999</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2870.7319999999995</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>43741</v>
       </c>
@@ -14693,14 +14858,14 @@
       </c>
       <c r="G118" s="2">
         <f t="shared" si="6"/>
-        <v>2965.6516000000001</v>
+        <v>2874.8932</v>
       </c>
       <c r="H118" s="2">
         <f t="shared" si="7"/>
-        <v>2934.9927999999991</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2918.0451999999996</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>43742</v>
       </c>
@@ -14725,14 +14890,14 @@
       </c>
       <c r="G119" s="2">
         <f t="shared" si="6"/>
-        <v>3019.6110000000003</v>
+        <v>2924.5601999999999</v>
       </c>
       <c r="H119" s="2">
         <f t="shared" si="7"/>
-        <v>2985.7628999999997</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2965.5569999999998</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>43743</v>
       </c>
@@ -14757,14 +14922,14 @@
       </c>
       <c r="G120" s="2">
         <f t="shared" si="6"/>
-        <v>3074.0562</v>
+        <v>2974.6530000000002</v>
       </c>
       <c r="H120" s="2">
         <f t="shared" si="7"/>
-        <v>3036.8743999999997</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3013.2626</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>43744</v>
       </c>
@@ -14789,14 +14954,14 @@
       </c>
       <c r="G121" s="2">
         <f t="shared" si="6"/>
-        <v>3128.9872</v>
+        <v>3025.1716000000001</v>
       </c>
       <c r="H121" s="2">
         <f t="shared" si="7"/>
-        <v>3088.3248999999996</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3061.1572000000001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>43745</v>
       </c>
@@ -14821,14 +14986,14 @@
       </c>
       <c r="G122" s="2">
         <f t="shared" si="6"/>
-        <v>3184.4040000000005</v>
+        <v>3076.1160000000004</v>
       </c>
       <c r="H122" s="2">
         <f t="shared" si="7"/>
-        <v>3140.1120000000001</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3109.2359999999999</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>43746</v>
       </c>
@@ -14853,14 +15018,14 @@
       </c>
       <c r="G123" s="2">
         <f t="shared" si="6"/>
-        <v>3240.3066000000003</v>
+        <v>3127.4862000000003</v>
       </c>
       <c r="H123" s="2">
         <f t="shared" si="7"/>
-        <v>3192.2332999999999</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3157.4941999999992</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>43747</v>
       </c>
@@ -14885,14 +15050,14 @@
       </c>
       <c r="G124" s="2">
         <f t="shared" si="6"/>
-        <v>3296.6950000000002</v>
+        <v>3179.2822000000001</v>
       </c>
       <c r="H124" s="2">
         <f t="shared" si="7"/>
-        <v>3244.6864000000005</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3205.9269999999997</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>43748</v>
       </c>
@@ -14917,14 +15082,14 @@
       </c>
       <c r="G125" s="2">
         <f t="shared" si="6"/>
-        <v>3353.5691999999999</v>
+        <v>3231.5040000000004</v>
       </c>
       <c r="H125" s="2">
         <f t="shared" si="7"/>
-        <v>3297.4688999999989</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3254.5295999999989</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>43749</v>
       </c>
@@ -14949,14 +15114,14 @@
       </c>
       <c r="G126" s="2">
         <f t="shared" si="6"/>
-        <v>3410.9292000000005</v>
+        <v>3284.1516000000001</v>
       </c>
       <c r="H126" s="2">
         <f t="shared" si="7"/>
-        <v>3350.5783999999999</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3303.2971999999995</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>43750</v>
       </c>
@@ -14981,14 +15146,14 @@
       </c>
       <c r="G127" s="2">
         <f t="shared" si="6"/>
-        <v>3468.7750000000001</v>
+        <v>3337.2249999999999</v>
       </c>
       <c r="H127" s="2">
         <f t="shared" si="7"/>
-        <v>3404.0124999999998</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+        <v>3352.2249999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>43751</v>
       </c>
@@ -15013,14 +15178,14 @@
       </c>
       <c r="G128" s="2">
         <f t="shared" si="6"/>
-        <v>3527.1066000000001</v>
+        <v>3390.7242000000001</v>
       </c>
       <c r="H128" s="2">
         <f t="shared" si="7"/>
-        <v>3457.7687999999998</v>
-      </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3401.3081999999995</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>43752</v>
       </c>
@@ -15045,14 +15210,14 @@
       </c>
       <c r="G129" s="2">
         <f t="shared" si="6"/>
-        <v>3585.924</v>
+        <v>3444.6492000000003</v>
       </c>
       <c r="H129" s="2">
         <f t="shared" si="7"/>
-        <v>3511.8448999999991</v>
-      </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3450.5419999999995</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>43753</v>
       </c>
@@ -15077,14 +15242,14 @@
       </c>
       <c r="G130" s="2">
         <f t="shared" si="6"/>
-        <v>3645.2272000000003</v>
+        <v>3499</v>
       </c>
       <c r="H130" s="2">
         <f t="shared" si="7"/>
-        <v>3566.2383999999993</v>
-      </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3499.9215999999997</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>43754</v>
       </c>
@@ -15108,15 +15273,15 @@
         <v>28.476923076923075</v>
       </c>
       <c r="G131" s="2">
-        <f t="shared" ref="G131:G176" si="11">0.2429*B131^2-2.6363*B131+3</f>
-        <v>3705.0162</v>
+        <f t="shared" ref="G131:G176" si="11">0.2129*B131^2+0.0613*B131+3</f>
+        <v>3553.7766000000001</v>
       </c>
       <c r="H131" s="2">
-        <f t="shared" ref="H131:H176" si="12">-0.0004*B131^3+0.3111*B131^2-5.4294*B131+3</f>
-        <v>3620.9468999999999</v>
-      </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+        <f t="shared" ref="H131:H176" si="12">-0.0008*B131^3+0.3777*B131^2-7.9187*B131+3</f>
+        <v>3549.4422</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>43755</v>
       </c>
@@ -15128,7 +15293,7 @@
         <v>3723</v>
       </c>
       <c r="D132" s="2">
-        <f t="shared" ref="D132:D152" si="13">C132-C131</f>
+        <f t="shared" ref="D132:D163" si="13">C132-C131</f>
         <v>18</v>
       </c>
       <c r="E132" s="2">
@@ -15141,14 +15306,14 @@
       </c>
       <c r="G132" s="2">
         <f t="shared" si="11"/>
-        <v>3765.2910000000002</v>
+        <v>3608.9790000000003</v>
       </c>
       <c r="H132" s="2">
         <f t="shared" si="12"/>
-        <v>3675.9679999999998</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3599.0989999999997</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>43756</v>
       </c>
@@ -15173,14 +15338,14 @@
       </c>
       <c r="G133" s="2">
         <f t="shared" si="11"/>
-        <v>3826.0515999999998</v>
+        <v>3664.6071999999999</v>
       </c>
       <c r="H133" s="2">
         <f t="shared" si="12"/>
-        <v>3731.2992999999997</v>
-      </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3648.8872000000001</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>43757</v>
       </c>
@@ -15205,14 +15370,14 @@
       </c>
       <c r="G134" s="2">
         <f t="shared" si="11"/>
-        <v>3887.2980000000002</v>
+        <v>3720.6612000000005</v>
       </c>
       <c r="H134" s="2">
         <f t="shared" si="12"/>
-        <v>3786.9383999999991</v>
-      </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3698.8019999999997</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>43758</v>
       </c>
@@ -15237,17 +15402,17 @@
       </c>
       <c r="G135" s="2">
         <f t="shared" si="11"/>
-        <v>3949.0301999999997</v>
+        <v>3777.1410000000001</v>
       </c>
       <c r="H135" s="2">
         <f t="shared" si="12"/>
-        <v>3842.8828999999996</v>
+        <v>3748.8386</v>
       </c>
       <c r="I135" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>43759</v>
       </c>
@@ -15272,14 +15437,14 @@
       </c>
       <c r="G136" s="2">
         <f t="shared" si="11"/>
-        <v>4011.2482000000005</v>
+        <v>3834.0466000000001</v>
       </c>
       <c r="H136" s="2">
         <f t="shared" si="12"/>
-        <v>3899.1304</v>
-      </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3798.9921999999988</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>43760</v>
       </c>
@@ -15304,14 +15469,14 @@
       </c>
       <c r="G137" s="2">
         <f t="shared" si="11"/>
-        <v>4073.9520000000002</v>
+        <v>3891.3780000000002</v>
       </c>
       <c r="H137" s="2">
         <f t="shared" si="12"/>
-        <v>3955.6784999999991</v>
-      </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3849.2579999999994</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>43761</v>
       </c>
@@ -15327,7 +15492,7 @@
         <v>51</v>
       </c>
       <c r="E138" s="2">
-        <f t="shared" ref="E138:E152" si="14">(C138-C131)/7</f>
+        <f t="shared" ref="E138:E163" si="14">(C138-C131)/7</f>
         <v>45.428571428571431</v>
       </c>
       <c r="F138" s="2">
@@ -15336,17 +15501,17 @@
       </c>
       <c r="G138" s="2">
         <f t="shared" si="11"/>
-        <v>4137.1415999999999</v>
+        <v>3949.1352000000002</v>
       </c>
       <c r="H138" s="2">
         <f t="shared" si="12"/>
-        <v>4012.5248000000001</v>
+        <v>3899.6311999999998</v>
       </c>
       <c r="I138" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>43762</v>
       </c>
@@ -15371,14 +15536,14 @@
       </c>
       <c r="G139" s="2">
         <f t="shared" si="11"/>
-        <v>4200.817</v>
+        <v>4007.3182000000002</v>
       </c>
       <c r="H139" s="2">
         <f t="shared" si="12"/>
-        <v>4069.6668999999993</v>
-      </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3950.1069999999991</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>43763</v>
       </c>
@@ -15403,14 +15568,14 @@
       </c>
       <c r="G140" s="2">
         <f t="shared" si="11"/>
-        <v>4264.9781999999996</v>
+        <v>4065.9270000000001</v>
       </c>
       <c r="H140" s="2">
         <f t="shared" si="12"/>
-        <v>4127.1023999999998</v>
-      </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4000.6805999999997</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>43764</v>
       </c>
@@ -15435,14 +15600,14 @@
       </c>
       <c r="G141" s="2">
         <f t="shared" si="11"/>
-        <v>4329.6251999999995</v>
+        <v>4124.9616000000005</v>
       </c>
       <c r="H141" s="2">
         <f t="shared" si="12"/>
-        <v>4184.8288999999995</v>
-      </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4051.3471999999992</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>43765</v>
       </c>
@@ -15467,14 +15632,14 @@
       </c>
       <c r="G142" s="2">
         <f t="shared" si="11"/>
-        <v>4394.7579999999998</v>
+        <v>4184.4220000000005</v>
       </c>
       <c r="H142" s="2">
         <f t="shared" si="12"/>
-        <v>4242.8439999999991</v>
-      </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4102.101999999999</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>43766</v>
       </c>
@@ -15499,14 +15664,14 @@
       </c>
       <c r="G143" s="2">
         <f t="shared" si="11"/>
-        <v>4460.3765999999996</v>
+        <v>4244.3081999999995</v>
       </c>
       <c r="H143" s="2">
         <f t="shared" si="12"/>
-        <v>4301.1452999999992</v>
-      </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4152.9401999999991</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>43767</v>
       </c>
@@ -15531,14 +15696,14 @@
       </c>
       <c r="G144" s="2">
         <f t="shared" si="11"/>
-        <v>4526.4810000000007</v>
+        <v>4304.6202000000003</v>
       </c>
       <c r="H144" s="2">
         <f t="shared" si="12"/>
-        <v>4359.7303999999995</v>
-      </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4203.857</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>43768</v>
       </c>
@@ -15563,14 +15728,14 @@
       </c>
       <c r="G145" s="2">
         <f t="shared" si="11"/>
-        <v>4593.0712000000003</v>
+        <v>4365.3580000000002</v>
       </c>
       <c r="H145" s="2">
         <f t="shared" si="12"/>
-        <v>4418.5968999999996</v>
-      </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4254.8475999999991</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>43769</v>
       </c>
@@ -15595,14 +15760,14 @@
       </c>
       <c r="G146" s="2">
         <f t="shared" si="11"/>
-        <v>4660.1472000000003</v>
+        <v>4426.5216</v>
       </c>
       <c r="H146" s="2">
         <f t="shared" si="12"/>
-        <v>4477.7423999999992</v>
-      </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4305.9071999999987</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>43770</v>
       </c>
@@ -15627,14 +15792,14 @@
       </c>
       <c r="G147" s="2">
         <f t="shared" si="11"/>
-        <v>4727.7089999999998</v>
+        <v>4488.1109999999999</v>
       </c>
       <c r="H147" s="2">
         <f t="shared" si="12"/>
-        <v>4537.1644999999999</v>
-      </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4357.0309999999999</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>43771</v>
       </c>
@@ -15659,14 +15824,14 @@
       </c>
       <c r="G148" s="2">
         <f t="shared" si="11"/>
-        <v>4795.7565999999997</v>
+        <v>4550.1262000000006</v>
       </c>
       <c r="H148" s="2">
         <f t="shared" si="12"/>
-        <v>4596.8607999999995</v>
-      </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4408.2141999999985</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>43772</v>
       </c>
@@ -15691,14 +15856,14 @@
       </c>
       <c r="G149" s="2">
         <f t="shared" si="11"/>
-        <v>4864.29</v>
+        <v>4612.5671999999995</v>
       </c>
       <c r="H149" s="2">
         <f t="shared" si="12"/>
-        <v>4656.8288999999995</v>
-      </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4459.4519999999993</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>43773</v>
       </c>
@@ -15707,30 +15872,30 @@
         <v>148</v>
       </c>
       <c r="C150" s="3">
-        <v>4630</v>
+        <v>4627</v>
       </c>
       <c r="D150" s="2">
         <f t="shared" si="13"/>
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E150" s="2">
         <f t="shared" si="14"/>
-        <v>47.285714285714285</v>
+        <v>46.857142857142854</v>
       </c>
       <c r="F150" s="2">
         <f>SUM($D$2:$D150)/COUNT($D$2:$D150)</f>
-        <v>31.053691275167786</v>
+        <v>31.033557046979865</v>
       </c>
       <c r="G150" s="2">
         <f t="shared" si="11"/>
-        <v>4933.3091999999997</v>
+        <v>4675.4340000000002</v>
       </c>
       <c r="H150" s="2">
         <f t="shared" si="12"/>
-        <v>4717.0663999999997</v>
-      </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4510.739599999999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>43774</v>
       </c>
@@ -15739,33 +15904,33 @@
         <v>149</v>
       </c>
       <c r="C151" s="3">
-        <v>4644</v>
+        <v>4687</v>
       </c>
       <c r="D151" s="2">
         <f t="shared" si="13"/>
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="E151" s="2">
         <f t="shared" si="14"/>
-        <v>44</v>
+        <v>50.142857142857146</v>
       </c>
       <c r="F151" s="2">
         <f>SUM($D$2:$D151)/COUNT($D$2:$D151)</f>
-        <v>30.94</v>
+        <v>31.226666666666667</v>
       </c>
       <c r="G151" s="2">
         <f t="shared" si="11"/>
-        <v>5002.8142000000007</v>
+        <v>4738.7266000000009</v>
       </c>
       <c r="H151" s="2">
         <f t="shared" si="12"/>
-        <v>4777.5708999999997</v>
+        <v>4562.0721999999987</v>
       </c>
       <c r="I151" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>43775</v>
       </c>
@@ -15774,30 +15939,30 @@
         <v>150</v>
       </c>
       <c r="C152" s="3">
-        <v>4708</v>
+        <v>4702</v>
       </c>
       <c r="D152" s="2">
         <f t="shared" si="13"/>
-        <v>64</v>
+        <v>15</v>
       </c>
       <c r="E152" s="2">
         <f t="shared" si="14"/>
-        <v>47.428571428571431</v>
+        <v>46.571428571428569</v>
       </c>
       <c r="F152" s="2">
         <f>SUM($D$2:$D152)/COUNT($D$2:$D152)</f>
-        <v>31.158940397350992</v>
+        <v>31.119205298013245</v>
       </c>
       <c r="G152" s="2">
         <f t="shared" si="11"/>
-        <v>5072.8050000000003</v>
+        <v>4802.4449999999997</v>
       </c>
       <c r="H152" s="2">
         <f t="shared" si="12"/>
-        <v>4838.34</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4613.4449999999997</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>43776</v>
       </c>
@@ -15805,17 +15970,31 @@
         <f t="shared" si="10"/>
         <v>151</v>
       </c>
-      <c r="E153" s="2"/>
+      <c r="C153" s="3">
+        <v>4750</v>
+      </c>
+      <c r="D153" s="2">
+        <f t="shared" si="13"/>
+        <v>48</v>
+      </c>
+      <c r="E153" s="2">
+        <f t="shared" si="14"/>
+        <v>42.714285714285715</v>
+      </c>
+      <c r="F153" s="2">
+        <f>SUM($D$2:$D153)/COUNT($D$2:$D153)</f>
+        <v>31.230263157894736</v>
+      </c>
       <c r="G153" s="2">
         <f t="shared" si="11"/>
-        <v>5143.2816000000003</v>
+        <v>4866.5892000000003</v>
       </c>
       <c r="H153" s="2">
         <f t="shared" si="12"/>
-        <v>4899.3712999999998</v>
-      </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4664.8531999999996</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>43777</v>
       </c>
@@ -15823,17 +16002,31 @@
         <f t="shared" si="10"/>
         <v>152</v>
       </c>
-      <c r="E154" s="2"/>
+      <c r="C154" s="3">
+        <v>4819</v>
+      </c>
+      <c r="D154" s="2">
+        <f t="shared" si="13"/>
+        <v>69</v>
+      </c>
+      <c r="E154" s="2">
+        <f t="shared" si="14"/>
+        <v>51.714285714285715</v>
+      </c>
+      <c r="F154" s="2">
+        <f>SUM($D$2:$D154)/COUNT($D$2:$D154)</f>
+        <v>31.477124183006534</v>
+      </c>
       <c r="G154" s="2">
         <f t="shared" si="11"/>
-        <v>5214.2440000000006</v>
+        <v>4931.1592000000001</v>
       </c>
       <c r="H154" s="2">
         <f t="shared" si="12"/>
-        <v>4960.6623999999993</v>
-      </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4716.2919999999986</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>43778</v>
       </c>
@@ -15841,20 +16034,34 @@
         <f t="shared" si="10"/>
         <v>153</v>
       </c>
-      <c r="E155" s="2"/>
+      <c r="C155" s="3">
+        <v>4898</v>
+      </c>
+      <c r="D155" s="2">
+        <f t="shared" si="13"/>
+        <v>79</v>
+      </c>
+      <c r="E155" s="2">
+        <f t="shared" si="14"/>
+        <v>51.285714285714285</v>
+      </c>
+      <c r="F155" s="2">
+        <f>SUM($D$2:$D155)/COUNT($D$2:$D155)</f>
+        <v>31.785714285714285</v>
+      </c>
       <c r="G155" s="2">
         <f t="shared" si="11"/>
-        <v>5285.6922000000004</v>
+        <v>4996.1549999999997</v>
       </c>
       <c r="H155" s="2">
         <f t="shared" si="12"/>
-        <v>5022.2109</v>
+        <v>4767.7565999999997</v>
       </c>
       <c r="I155" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>43779</v>
       </c>
@@ -15862,17 +16069,31 @@
         <f t="shared" si="10"/>
         <v>154</v>
       </c>
-      <c r="E156" s="2"/>
+      <c r="C156" s="3">
+        <v>4923</v>
+      </c>
+      <c r="D156" s="2">
+        <f t="shared" si="13"/>
+        <v>25</v>
+      </c>
+      <c r="E156" s="2">
+        <f t="shared" si="14"/>
+        <v>54.714285714285715</v>
+      </c>
+      <c r="F156" s="2">
+        <f>SUM($D$2:$D156)/COUNT($D$2:$D156)</f>
+        <v>31.741935483870968</v>
+      </c>
       <c r="G156" s="2">
         <f t="shared" si="11"/>
-        <v>5357.6261999999997</v>
+        <v>5061.5766000000003</v>
       </c>
       <c r="H156" s="2">
         <f t="shared" si="12"/>
-        <v>5084.0144</v>
-      </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4819.2421999999997</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>43780</v>
       </c>
@@ -15880,17 +16101,31 @@
         <f t="shared" si="10"/>
         <v>155</v>
       </c>
-      <c r="E157" s="2"/>
+      <c r="C157" s="3">
+        <v>4987</v>
+      </c>
+      <c r="D157" s="2">
+        <f t="shared" si="13"/>
+        <v>64</v>
+      </c>
+      <c r="E157" s="2">
+        <f t="shared" si="14"/>
+        <v>51.428571428571431</v>
+      </c>
+      <c r="F157" s="2">
+        <f>SUM($D$2:$D157)/COUNT($D$2:$D157)</f>
+        <v>31.948717948717949</v>
+      </c>
       <c r="G157" s="2">
         <f t="shared" si="11"/>
-        <v>5430.0459999999994</v>
+        <v>5127.4240000000009</v>
       </c>
       <c r="H157" s="2">
         <f t="shared" si="12"/>
-        <v>5146.0704999999998</v>
-      </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4870.7439999999997</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>43781</v>
       </c>
@@ -15898,17 +16133,31 @@
         <f t="shared" si="10"/>
         <v>156</v>
       </c>
-      <c r="E158" s="2"/>
+      <c r="C158" s="3">
+        <v>5037</v>
+      </c>
+      <c r="D158" s="2">
+        <f t="shared" si="13"/>
+        <v>50</v>
+      </c>
+      <c r="E158" s="2">
+        <f t="shared" si="14"/>
+        <v>50</v>
+      </c>
+      <c r="F158" s="2">
+        <f>SUM($D$2:$D158)/COUNT($D$2:$D158)</f>
+        <v>32.06369426751592</v>
+      </c>
       <c r="G158" s="2">
         <f t="shared" si="11"/>
-        <v>5502.9516000000003</v>
+        <v>5193.6971999999996</v>
       </c>
       <c r="H158" s="2">
         <f t="shared" si="12"/>
-        <v>5208.3768</v>
-      </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4922.2571999999982</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>43782</v>
       </c>
@@ -15916,17 +16165,31 @@
         <f t="shared" si="10"/>
         <v>157</v>
       </c>
-      <c r="E159" s="2"/>
+      <c r="C159" s="3">
+        <v>5031</v>
+      </c>
+      <c r="D159" s="2">
+        <f t="shared" si="13"/>
+        <v>-6</v>
+      </c>
+      <c r="E159" s="2">
+        <f t="shared" si="14"/>
+        <v>47</v>
+      </c>
+      <c r="F159" s="2">
+        <f>SUM($D$2:$D159)/COUNT($D$2:$D159)</f>
+        <v>31.822784810126581</v>
+      </c>
       <c r="G159" s="2">
         <f t="shared" si="11"/>
-        <v>5576.3430000000008</v>
+        <v>5260.3962000000001</v>
       </c>
       <c r="H159" s="2">
         <f t="shared" si="12"/>
-        <v>5270.9309000000003</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4973.777</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>43783</v>
       </c>
@@ -15934,17 +16197,31 @@
         <f t="shared" si="10"/>
         <v>158</v>
       </c>
-      <c r="E160" s="2"/>
+      <c r="C160" s="3">
+        <v>5079</v>
+      </c>
+      <c r="D160" s="2">
+        <f t="shared" si="13"/>
+        <v>48</v>
+      </c>
+      <c r="E160" s="2">
+        <f t="shared" si="14"/>
+        <v>47</v>
+      </c>
+      <c r="F160" s="2">
+        <f>SUM($D$2:$D160)/COUNT($D$2:$D160)</f>
+        <v>31.924528301886792</v>
+      </c>
       <c r="G160" s="2">
         <f t="shared" si="11"/>
-        <v>5650.2202000000007</v>
+        <v>5327.5210000000006</v>
       </c>
       <c r="H160" s="2">
         <f t="shared" si="12"/>
-        <v>5333.7304000000004</v>
-      </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5025.2986000000001</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>43784</v>
       </c>
@@ -15952,17 +16229,31 @@
         <f t="shared" si="10"/>
         <v>159</v>
       </c>
-      <c r="E161" s="2"/>
+      <c r="C161" s="3">
+        <v>5115</v>
+      </c>
+      <c r="D161" s="2">
+        <f t="shared" si="13"/>
+        <v>36</v>
+      </c>
+      <c r="E161" s="2">
+        <f t="shared" si="14"/>
+        <v>42.285714285714285</v>
+      </c>
+      <c r="F161" s="2">
+        <f>SUM($D$2:$D161)/COUNT($D$2:$D161)</f>
+        <v>31.95</v>
+      </c>
       <c r="G161" s="2">
         <f t="shared" si="11"/>
-        <v>5724.5832</v>
+        <v>5395.0716000000002</v>
       </c>
       <c r="H161" s="2">
         <f t="shared" si="12"/>
-        <v>5396.7728999999999</v>
-      </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5076.8171999999995</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>43785</v>
       </c>
@@ -15970,17 +16261,31 @@
         <f t="shared" si="10"/>
         <v>160</v>
       </c>
-      <c r="E162" s="2"/>
+      <c r="C162" s="3">
+        <v>5204</v>
+      </c>
+      <c r="D162" s="2">
+        <f t="shared" si="13"/>
+        <v>89</v>
+      </c>
+      <c r="E162" s="2">
+        <f t="shared" si="14"/>
+        <v>43.714285714285715</v>
+      </c>
+      <c r="F162" s="2">
+        <f>SUM($D$2:$D162)/COUNT($D$2:$D162)</f>
+        <v>32.304347826086953</v>
+      </c>
       <c r="G162" s="2">
         <f t="shared" si="11"/>
-        <v>5799.4319999999998</v>
+        <v>5463.0479999999998</v>
       </c>
       <c r="H162" s="2">
         <f t="shared" si="12"/>
-        <v>5460.0560000000005</v>
-      </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5128.3279999999986</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>43786</v>
       </c>
@@ -15988,17 +16293,31 @@
         <f t="shared" si="10"/>
         <v>161</v>
       </c>
-      <c r="E163" s="2"/>
+      <c r="C163" s="3">
+        <v>5249</v>
+      </c>
+      <c r="D163" s="2">
+        <f t="shared" si="13"/>
+        <v>45</v>
+      </c>
+      <c r="E163" s="2">
+        <f t="shared" si="14"/>
+        <v>46.571428571428569</v>
+      </c>
+      <c r="F163" s="2">
+        <f>SUM($D$2:$D163)/COUNT($D$2:$D163)</f>
+        <v>32.382716049382715</v>
+      </c>
       <c r="G163" s="2">
         <f t="shared" si="11"/>
-        <v>5874.7665999999999</v>
+        <v>5531.4502000000002</v>
       </c>
       <c r="H163" s="2">
         <f t="shared" si="12"/>
-        <v>5523.5772999999999</v>
-      </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5179.8261999999995</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>43787</v>
       </c>
@@ -16009,14 +16328,14 @@
       <c r="E164" s="2"/>
       <c r="G164" s="2">
         <f t="shared" si="11"/>
-        <v>5950.5869999999995</v>
+        <v>5600.2781999999997</v>
       </c>
       <c r="H164" s="2">
         <f t="shared" si="12"/>
-        <v>5587.3343999999997</v>
-      </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5231.3069999999989</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>43788</v>
       </c>
@@ -16027,14 +16346,14 @@
       <c r="E165" s="2"/>
       <c r="G165" s="2">
         <f t="shared" si="11"/>
-        <v>6026.8931999999995</v>
+        <v>5669.5320000000002</v>
       </c>
       <c r="H165" s="2">
         <f t="shared" si="12"/>
-        <v>5651.3248999999987</v>
-      </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5282.7655999999988</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>43789</v>
       </c>
@@ -16045,14 +16364,14 @@
       <c r="E166" s="2"/>
       <c r="G166" s="2">
         <f t="shared" si="11"/>
-        <v>6103.6852000000008</v>
+        <v>5739.2116000000005</v>
       </c>
       <c r="H166" s="2">
         <f t="shared" si="12"/>
-        <v>5715.5464000000011</v>
-      </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5334.1971999999996</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>43790</v>
       </c>
@@ -16063,14 +16382,14 @@
       <c r="E167" s="2"/>
       <c r="G167" s="2">
         <f t="shared" si="11"/>
-        <v>6180.9630000000006</v>
+        <v>5809.317</v>
       </c>
       <c r="H167" s="2">
         <f t="shared" si="12"/>
-        <v>5779.9965000000002</v>
-      </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5385.5969999999988</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>43791</v>
       </c>
@@ -16081,14 +16400,14 @@
       <c r="E168" s="2"/>
       <c r="G168" s="2">
         <f t="shared" si="11"/>
-        <v>6258.7266</v>
+        <v>5879.8482000000004</v>
       </c>
       <c r="H168" s="2">
         <f t="shared" si="12"/>
-        <v>5844.6728000000003</v>
-      </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5436.9602000000004</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>43792</v>
       </c>
@@ -16099,14 +16418,14 @@
       <c r="E169" s="2"/>
       <c r="G169" s="2">
         <f t="shared" si="11"/>
-        <v>6336.9760000000006</v>
+        <v>5950.8052000000007</v>
       </c>
       <c r="H169" s="2">
         <f t="shared" si="12"/>
-        <v>5909.5728999999992</v>
-      </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5488.2819999999992</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>43793</v>
       </c>
@@ -16117,14 +16436,14 @@
       <c r="E170" s="2"/>
       <c r="G170" s="2">
         <f t="shared" si="11"/>
-        <v>6415.7111999999997</v>
+        <v>6022.1880000000001</v>
       </c>
       <c r="H170" s="2">
         <f t="shared" si="12"/>
-        <v>5974.6944000000003</v>
-      </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5539.5576000000001</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>43794</v>
       </c>
@@ -16135,14 +16454,14 @@
       <c r="E171" s="2"/>
       <c r="G171" s="2">
         <f t="shared" si="11"/>
-        <v>6494.9322000000002</v>
+        <v>6093.9966000000004</v>
       </c>
       <c r="H171" s="2">
         <f t="shared" si="12"/>
-        <v>6040.0349000000006</v>
-      </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5590.7821999999996</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>43795</v>
       </c>
@@ -16153,14 +16472,14 @@
       <c r="E172" s="2"/>
       <c r="G172" s="2">
         <f t="shared" si="11"/>
-        <v>6574.6390000000001</v>
+        <v>6166.2310000000007</v>
       </c>
       <c r="H172" s="2">
         <f t="shared" si="12"/>
-        <v>6105.5919999999987</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5641.9509999999991</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>43796</v>
       </c>
@@ -16171,14 +16490,14 @@
       <c r="E173" s="2"/>
       <c r="G173" s="2">
         <f t="shared" si="11"/>
-        <v>6654.8315999999995</v>
+        <v>6238.8912</v>
       </c>
       <c r="H173" s="2">
         <f t="shared" si="12"/>
-        <v>6171.3632999999991</v>
-      </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5693.0591999999988</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>43797</v>
       </c>
@@ -16189,14 +16508,14 @@
       <c r="E174" s="2"/>
       <c r="G174" s="2">
         <f t="shared" si="11"/>
-        <v>6735.51</v>
+        <v>6311.9772000000003</v>
       </c>
       <c r="H174" s="2">
         <f t="shared" si="12"/>
-        <v>6237.3463999999985</v>
-      </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5744.101999999999</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>43798</v>
       </c>
@@ -16207,14 +16526,14 @@
       <c r="E175" s="2"/>
       <c r="G175" s="2">
         <f t="shared" si="11"/>
-        <v>6816.6742000000004</v>
+        <v>6385.4890000000005</v>
       </c>
       <c r="H175" s="2">
         <f t="shared" si="12"/>
-        <v>6303.5388999999996</v>
-      </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5795.0745999999981</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>43799</v>
       </c>
@@ -16225,14 +16544,14 @@
       <c r="E176" s="2"/>
       <c r="G176" s="2">
         <f t="shared" si="11"/>
-        <v>6898.3242</v>
+        <v>6459.4265999999998</v>
       </c>
       <c r="H176" s="2">
         <f t="shared" si="12"/>
-        <v>6369.9383999999991</v>
-      </c>
-    </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+        <v>5845.9721999999992</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>43800</v>
       </c>
@@ -16241,7 +16560,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>43801</v>
       </c>
@@ -16250,7 +16569,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>43802</v>
       </c>
@@ -16259,7 +16578,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>43803</v>
       </c>
@@ -16268,7 +16587,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>43804</v>
       </c>
@@ -16277,7 +16596,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>43805</v>
       </c>
@@ -16286,7 +16605,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>43806</v>
       </c>
@@ -16295,7 +16614,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>43807</v>
       </c>
@@ -16304,7 +16623,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>43808</v>
       </c>
@@ -16313,7 +16632,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>43809</v>
       </c>
@@ -16322,7 +16641,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>43810</v>
       </c>
@@ -16331,7 +16650,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>43811</v>
       </c>
@@ -16340,7 +16659,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>43812</v>
       </c>
@@ -16349,7 +16668,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>43813</v>
       </c>
@@ -16358,7 +16677,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>43814</v>
       </c>
@@ -16367,7 +16686,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>43815</v>
       </c>
@@ -16376,7 +16695,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>43816</v>
       </c>
@@ -16385,7 +16704,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>43817</v>
       </c>
@@ -16394,7 +16713,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>43818</v>
       </c>
@@ -16403,7 +16722,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>43819</v>
       </c>
@@ -16412,7 +16731,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>43820</v>
       </c>
@@ -16421,7 +16740,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>43821</v>
       </c>
@@ -16430,7 +16749,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>43822</v>
       </c>
@@ -16439,7 +16758,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>43823</v>
       </c>
@@ -16448,7 +16767,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>43824</v>
       </c>
@@ -16457,7 +16776,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>43825</v>
       </c>
@@ -16466,7 +16785,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>43826</v>
       </c>
@@ -16475,7 +16794,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>43827</v>
       </c>
@@ -16484,7 +16803,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>43828</v>
       </c>
@@ -16493,7 +16812,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>43829</v>
       </c>
@@ -16502,7 +16821,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>43830</v>
       </c>

</xml_diff>